<commit_message>
Actualizacion datos de tiempos
Actualizacion, modificacion y agregado de tiempos de algoritmo burbuja y burbuja opt 2
</commit_message>
<xml_diff>
--- a/practica-1/Recopilacion de datos/Tabla de tiempos de algoritmos.xlsx
+++ b/practica-1/Recopilacion de datos/Tabla de tiempos de algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Analisis-y-Disegno-de-Algoritmos\practica-1\Recopilacion de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C975EFD0-0817-4E74-BF3B-97A407544438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2405DF34-C8AD-4FE8-9287-9441F2654324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6D9A99E9-C192-43DF-AC6A-A482D0DE89DC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="27">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Optimized Bubble Sort 1</t>
+  </si>
+  <si>
+    <t>Optimized Bubble Sort 2</t>
   </si>
 </sst>
 </file>
@@ -251,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -270,9 +276,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -290,6 +293,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,10 +424,10 @@
                   <c:v>Bubble Sort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Optimized Bubble Sort 1 *</c:v>
+                  <c:v>Optimized Bubble Sort 1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Optimized Bubble Sort 2 *</c:v>
+                  <c:v>Optimized Bubble Sort 2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Insertion Sort</c:v>
@@ -453,13 +460,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>912.37877988820003</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>675.10587501529994</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>688.3177878857</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>144.7588801384</c:v>
@@ -524,10 +531,10 @@
                   <c:v>Bubble Sort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Optimized Bubble Sort 1 *</c:v>
+                  <c:v>Optimized Bubble Sort 1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Optimized Bubble Sort 2 *</c:v>
+                  <c:v>Optimized Bubble Sort 2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Insertion Sort</c:v>
@@ -560,13 +567,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>913.34052999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>675.10241799999994</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>688.46476900000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>144.747165</c:v>
@@ -631,10 +638,10 @@
                   <c:v>Bubble Sort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Optimized Bubble Sort 1 *</c:v>
+                  <c:v>Optimized Bubble Sort 1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Optimized Bubble Sort 2 *</c:v>
+                  <c:v>Optimized Bubble Sort 2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Insertion Sort</c:v>
@@ -667,13 +674,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>2.1246999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.8530000000000001E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.31E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.1691999999999999E-2</c:v>
@@ -1141,16 +1148,16 @@
                   <c:v>9.2890977900000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.1436157199999998E-2</c:v>
+                  <c:v>0.11007239532</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.12597107890000001</c:v>
+                  <c:v>0.1192560196</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1040768623</c:v>
+                  <c:v>0.1805579662</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.1454982800000001E-2</c:v>
+                  <c:v>0.18689107890000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.21202397349999999</c:v>
@@ -1325,16 +1332,16 @@
                   <c:v>9.2026999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.0890000000000004E-2</c:v>
+                  <c:v>0.11007239532</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.129939</c:v>
+                  <c:v>0.116401</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.102663</c:v>
+                  <c:v>0.178812</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.143457</c:v>
+                  <c:v>0.18689107890000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.215008</c:v>
@@ -1515,7 +1522,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.418E-3</c:v>
+                  <c:v>1.3860000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.0269999999999999E-3</c:v>
@@ -2688,43 +2695,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.6160011E-3</c:v>
+                  <c:v>5.3410530000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4470767999999998E-3</c:v>
+                  <c:v>2.0967960399999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.47697926E-2</c:v>
+                  <c:v>3.8478851299999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7949094800000001E-2</c:v>
+                  <c:v>5.0436973599999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14117407800000001</c:v>
+                  <c:v>0.202974081</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.22094607350000001</c:v>
+                  <c:v>0.31697583200000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5079309939999996</c:v>
+                  <c:v>9.0544888973000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.752557992900002</c:v>
+                  <c:v>35.357850074799998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59.227169990500002</c:v>
+                  <c:v>78.645340919500001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>103.09226202959999</c:v>
+                  <c:v>141.74525403979999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>230.20986580850001</c:v>
+                  <c:v>405.49503517149998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>410.62090611460002</c:v>
+                  <c:v>578.68121910100001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>640.25535511969997</c:v>
+                  <c:v>912.37877988820003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2830,43 +2837,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.621E-3</c:v>
+                  <c:v>3.5400000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4450000000000002E-3</c:v>
+                  <c:v>2.0254000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4871000000000001E-2</c:v>
+                  <c:v>3.7157999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7952000000000001E-2</c:v>
+                  <c:v>4.87E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.141177</c:v>
+                  <c:v>0.195963</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.22095200000000001</c:v>
+                  <c:v>0.30601899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5078880000000003</c:v>
+                  <c:v>8.7281659999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.749362999999999</c:v>
+                  <c:v>35.217261000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59.227144000000003</c:v>
+                  <c:v>79.153655000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>103.092235</c:v>
+                  <c:v>141.09704400000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>230.207098</c:v>
+                  <c:v>405.50267200000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>410.57353000000001</c:v>
+                  <c:v>578.17917599999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>640.25501699999995</c:v>
+                  <c:v>913.34052999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2972,7 +2979,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.627E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2999,16 +3006,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>2.1440000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.5080000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.1770000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.0698000000000001E-2</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2.1246999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3400,10 +3407,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3442,37 +3449,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$41:$U$41</c:f>
+              <c:f>Hoja1!$B$41:$N$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.6160011E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4470767999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.47697926E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7949094800000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14117407800000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22094607350000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5079309939999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.752557992900002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.227169990500002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>103.09226202959999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>230.20986580850001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>494.42150998120002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>675.10587501529994</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3524,10 +3549,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3566,37 +3591,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$42:$U$42</c:f>
+              <c:f>Hoja1!$B$42:$N$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.621E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4450000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4871000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7952000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.141177</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22095200000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5078880000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.749362999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.227144000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>103.092235</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>230.207098</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>494.35421700000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>675.10241799999994</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3648,10 +3691,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3690,37 +3733,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$43:$U$43</c:f>
+              <c:f>Hoja1!$B$43:$N$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1770000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3744E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.8530000000000001E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4111,10 +4172,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4153,37 +4214,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$52:$U$52</c:f>
+              <c:f>Hoja1!$B$52:$N$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.8229485E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9580077999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6651153599999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0879020699999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14686989780000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25073909760000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7361590861999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.236689090700001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.848061084699999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>108.50353097919999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>366.31396508220001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>429.93227386469999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>688.3177878857</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4235,10 +4314,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4277,37 +4356,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$53:$U$53</c:f>
+              <c:f>Hoja1!$B$53:$N$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7650000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6177E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0009999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.135573</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24366199999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5335419999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.353097000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.916975000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>108.16159399999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>366.289851</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>430.24897600000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>688.46476900000005</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4359,10 +4456,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4401,37 +4498,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$54:$U$54</c:f>
+              <c:f>Hoja1!$B$54:$N$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.7780000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1549999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3189999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0630999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.4349999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.31E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8263,7 +8378,7 @@
                   <c:v>3.8465023000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.102408886</c:v>
+                  <c:v>9.0778112399999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>7.6631069199999999E-2</c:v>
@@ -8281,7 +8396,7 @@
                   <c:v>0.16359996800000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.29176807399999999</c:v>
+                  <c:v>0.22102785110000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.24379897119999999</c:v>
@@ -8447,7 +8562,7 @@
                   <c:v>3.8543000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.9287999999999997E-2</c:v>
+                  <c:v>9.0782000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>7.6680999999999999E-2</c:v>
@@ -8465,7 +8580,7 @@
                   <c:v>0.15345900000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28173199999999998</c:v>
+                  <c:v>0.22102785110000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.24270900000000001</c:v>
@@ -8631,7 +8746,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3192000000000001E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -15825,10 +15940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F19DE01-9E71-422D-A8E5-2FF9C6F5908D}">
-  <dimension ref="A1:U620"/>
+  <dimension ref="A1:AS620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="59" zoomScaleNormal="41" workbookViewId="0">
-      <selection activeCell="S66" sqref="S66"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="55" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="T98" sqref="T98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15842,13 +15957,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -15871,67 +15986,67 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9">
-        <v>675.10587501529994</v>
-      </c>
-      <c r="C3" s="9">
-        <v>675.10241799999994</v>
-      </c>
-      <c r="D3" s="9">
-        <v>2.8530000000000001E-3</v>
-      </c>
-      <c r="E3" s="9">
-        <v>99.999910530299999</v>
+      <c r="B3" s="8">
+        <v>912.37877988820003</v>
+      </c>
+      <c r="C3" s="8">
+        <v>913.34052999999994</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2.1246999999999999E-2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>100.1077400235</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="8">
+        <v>675.10587501529994</v>
+      </c>
+      <c r="C4" s="8">
+        <v>675.10241799999994</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2.8530000000000001E-3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>99.999910530299999</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="8">
+        <v>688.3177878857</v>
+      </c>
+      <c r="C5" s="8">
+        <v>688.46476900000005</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3.31E-3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>100.0218345533</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>144.7588801384</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>144.747165</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>1.1691999999999999E-2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>99.999984015899997</v>
       </c>
     </row>
@@ -15939,16 +16054,16 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>256.26689410210003</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>256.26093200000003</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>5.9420000000000002E-3</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>99.999992155800001</v>
       </c>
     </row>
@@ -15956,16 +16071,16 @@
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.53191399569999998</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>0.52315100000000003</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>8.7740000000000005E-3</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>100.0020688038</v>
       </c>
     </row>
@@ -15973,16 +16088,16 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>0</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>0</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>0</v>
       </c>
     </row>
@@ -15990,16 +16105,16 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>9.3252897299999998E-2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>9.3253000000000003E-2</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>6.4300000000000002E-4</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>100.0001101708</v>
       </c>
     </row>
@@ -16007,16 +16122,16 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>6.61728382E-2</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>6.4346E-2</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>1.823E-3</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>99.994199718199994</v>
       </c>
     </row>
@@ -16024,16 +16139,16 @@
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>0</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>0</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>0</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>0</v>
       </c>
     </row>
@@ -16041,29 +16156,29 @@
       <c r="R13" s="5"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
@@ -16134,55 +16249,55 @@
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="9">
-        <v>1.6160011E-3</v>
-      </c>
-      <c r="C23" s="9">
-        <v>6.4470767999999998E-3</v>
-      </c>
-      <c r="D23" s="9">
-        <v>1.47697926E-2</v>
-      </c>
-      <c r="E23" s="9">
-        <v>2.7949094800000001E-2</v>
-      </c>
-      <c r="F23" s="9">
-        <v>0.14117407800000001</v>
-      </c>
-      <c r="G23" s="9">
-        <v>0.22094607350000001</v>
-      </c>
-      <c r="H23" s="9">
-        <v>6.5079309939999996</v>
-      </c>
-      <c r="I23" s="9">
-        <v>26.752557992900002</v>
-      </c>
-      <c r="J23" s="9">
-        <v>59.227169990500002</v>
-      </c>
-      <c r="K23" s="9">
-        <v>103.09226202959999</v>
-      </c>
-      <c r="L23" s="9">
-        <v>230.20986580850001</v>
-      </c>
-      <c r="M23" s="9">
-        <v>410.62090611460002</v>
-      </c>
-      <c r="N23" s="9">
-        <v>640.25535511969997</v>
-      </c>
-      <c r="O23" s="9" t="s">
+      <c r="B23" s="8">
+        <v>5.3410530000000001E-3</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2.0967960399999999E-2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>3.8478851299999998E-2</v>
+      </c>
+      <c r="E23" s="8">
+        <v>5.0436973599999997E-2</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.202974081</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.31697583200000001</v>
+      </c>
+      <c r="H23" s="8">
+        <v>9.0544888973000006</v>
+      </c>
+      <c r="I23" s="8">
+        <v>35.357850074799998</v>
+      </c>
+      <c r="J23" s="8">
+        <v>78.645340919500001</v>
+      </c>
+      <c r="K23" s="8">
+        <v>141.74525403979999</v>
+      </c>
+      <c r="L23" s="8">
+        <v>405.49503517149998</v>
+      </c>
+      <c r="M23" s="8">
+        <v>578.68121910100001</v>
+      </c>
+      <c r="N23" s="8">
+        <v>912.37877988820003</v>
+      </c>
+      <c r="O23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="P23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q23" s="9" t="s">
+      <c r="Q23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="9" t="s">
+      <c r="R23" s="8" t="s">
         <v>24</v>
       </c>
       <c r="S23" s="6" t="s">
@@ -16199,55 +16314,55 @@
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="9">
-        <v>1.621E-3</v>
-      </c>
-      <c r="C24" s="9">
-        <v>6.4450000000000002E-3</v>
-      </c>
-      <c r="D24" s="9">
-        <v>1.4871000000000001E-2</v>
-      </c>
-      <c r="E24" s="9">
-        <v>2.7952000000000001E-2</v>
-      </c>
-      <c r="F24" s="9">
-        <v>0.141177</v>
-      </c>
-      <c r="G24" s="9">
-        <v>0.22095200000000001</v>
-      </c>
-      <c r="H24" s="9">
-        <v>6.5078880000000003</v>
-      </c>
-      <c r="I24" s="9">
-        <v>26.749362999999999</v>
-      </c>
-      <c r="J24" s="9">
-        <v>59.227144000000003</v>
-      </c>
-      <c r="K24" s="9">
-        <v>103.092235</v>
-      </c>
-      <c r="L24" s="9">
-        <v>230.207098</v>
-      </c>
-      <c r="M24" s="9">
-        <v>410.57353000000001</v>
-      </c>
-      <c r="N24" s="9">
-        <v>640.25501699999995</v>
-      </c>
-      <c r="O24" s="9" t="s">
+      <c r="B24" s="8">
+        <v>3.5400000000000002E-3</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2.0254000000000001E-2</v>
+      </c>
+      <c r="D24" s="8">
+        <v>3.7157999999999997E-2</v>
+      </c>
+      <c r="E24" s="8">
+        <v>4.87E-2</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.195963</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.30601899999999999</v>
+      </c>
+      <c r="H24" s="8">
+        <v>8.7281659999999999</v>
+      </c>
+      <c r="I24" s="8">
+        <v>35.217261000000001</v>
+      </c>
+      <c r="J24" s="8">
+        <v>79.153655000000001</v>
+      </c>
+      <c r="K24" s="8">
+        <v>141.09704400000001</v>
+      </c>
+      <c r="L24" s="8">
+        <v>405.50267200000002</v>
+      </c>
+      <c r="M24" s="8">
+        <v>578.17917599999998</v>
+      </c>
+      <c r="N24" s="8">
+        <v>913.34052999999994</v>
+      </c>
+      <c r="O24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P24" s="9" t="s">
+      <c r="P24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q24" s="9" t="s">
+      <c r="Q24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R24" s="9" t="s">
+      <c r="R24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="S24" s="6" t="s">
@@ -16264,55 +16379,55 @@
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="8">
+        <v>1.627E-3</v>
+      </c>
+      <c r="C25" s="8">
         <v>0</v>
       </c>
-      <c r="C25" s="9">
+      <c r="D25" s="8">
         <v>0</v>
       </c>
-      <c r="D25" s="9">
+      <c r="E25" s="8">
         <v>0</v>
       </c>
-      <c r="E25" s="9">
+      <c r="F25" s="8">
         <v>0</v>
       </c>
-      <c r="F25" s="9">
+      <c r="G25" s="8">
         <v>0</v>
       </c>
-      <c r="G25" s="9">
+      <c r="H25" s="8">
         <v>0</v>
       </c>
-      <c r="H25" s="9">
+      <c r="I25" s="8">
         <v>0</v>
       </c>
-      <c r="I25" s="9">
+      <c r="J25" s="8">
         <v>0</v>
       </c>
-      <c r="J25" s="9">
+      <c r="K25" s="8">
+        <v>2.1440000000000001E-3</v>
+      </c>
+      <c r="L25" s="8">
+        <v>9.5080000000000008E-3</v>
+      </c>
+      <c r="M25" s="8">
         <v>0</v>
       </c>
-      <c r="K25" s="9">
-        <v>0</v>
-      </c>
-      <c r="L25" s="9">
-        <v>2.1770000000000001E-3</v>
-      </c>
-      <c r="M25" s="9">
-        <v>2.0698000000000001E-2</v>
-      </c>
-      <c r="N25" s="9">
-        <v>0</v>
-      </c>
-      <c r="O25" s="9" t="s">
+      <c r="N25" s="8">
+        <v>2.1246999999999999E-2</v>
+      </c>
+      <c r="O25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P25" s="9" t="s">
+      <c r="P25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q25" s="9" t="s">
+      <c r="Q25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R25" s="9" t="s">
+      <c r="R25" s="8" t="s">
         <v>24</v>
       </c>
       <c r="S25" s="6" t="s">
@@ -16329,55 +16444,55 @@
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="9">
-        <v>100.30933585130001</v>
-      </c>
-      <c r="C26" s="9">
-        <v>99.967786990099995</v>
-      </c>
-      <c r="D26" s="9">
-        <v>100.6852326656</v>
-      </c>
-      <c r="E26" s="9">
-        <v>100.01039471110001</v>
-      </c>
-      <c r="F26" s="9">
-        <v>100.0020697938</v>
-      </c>
-      <c r="G26" s="9">
-        <v>100.0026823142</v>
-      </c>
-      <c r="H26" s="9">
-        <v>99.999339359399997</v>
-      </c>
-      <c r="I26" s="9">
-        <v>99.988057243200004</v>
-      </c>
-      <c r="J26" s="9">
-        <v>99.9999561172</v>
-      </c>
-      <c r="K26" s="9">
-        <v>99.999973781099996</v>
-      </c>
-      <c r="L26" s="9">
-        <v>99.999743360899998</v>
-      </c>
-      <c r="M26" s="9">
-        <v>99.993502981899994</v>
-      </c>
-      <c r="N26" s="9">
-        <v>99.999947189899999</v>
-      </c>
-      <c r="O26" s="9" t="s">
+      <c r="B26" s="8">
+        <v>96.741222962199998</v>
+      </c>
+      <c r="C26" s="8">
+        <v>96.594993764400002</v>
+      </c>
+      <c r="D26" s="8">
+        <v>96.567331733900005</v>
+      </c>
+      <c r="E26" s="8">
+        <v>96.556150282700003</v>
+      </c>
+      <c r="F26" s="8">
+        <v>96.545824469999999</v>
+      </c>
+      <c r="G26" s="8">
+        <v>96.543322588099997</v>
+      </c>
+      <c r="H26" s="8">
+        <v>96.396009746900006</v>
+      </c>
+      <c r="I26" s="8">
+        <v>99.602382287200001</v>
+      </c>
+      <c r="J26" s="8">
+        <v>100.6463371823</v>
+      </c>
+      <c r="K26" s="8">
+        <v>99.544206228199997</v>
+      </c>
+      <c r="L26" s="8">
+        <v>100.0042281229</v>
+      </c>
+      <c r="M26" s="8">
+        <v>99.913243581399996</v>
+      </c>
+      <c r="N26" s="8">
+        <v>100.1077400235</v>
+      </c>
+      <c r="O26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P26" s="9" t="s">
+      <c r="P26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q26" s="9" t="s">
+      <c r="Q26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R26" s="9" t="s">
+      <c r="R26" s="8" t="s">
         <v>24</v>
       </c>
       <c r="S26" s="6" t="s">
@@ -16393,32 +16508,32 @@
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="P27" s="5"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+    </row>
+    <row r="40" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
@@ -16482,24 +16597,64 @@
       <c r="U40" s="4">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="AF40" s="14"/>
+      <c r="AG40" s="14"/>
+      <c r="AH40" s="14"/>
+      <c r="AI40" s="14"/>
+      <c r="AJ40" s="14"/>
+      <c r="AK40" s="14"/>
+      <c r="AL40" s="14"/>
+      <c r="AM40" s="14"/>
+      <c r="AN40" s="14"/>
+      <c r="AO40" s="14"/>
+      <c r="AP40" s="14"/>
+      <c r="AQ40" s="14"/>
+      <c r="AR40" s="14"/>
+      <c r="AS40" s="14"/>
+    </row>
+    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
+      <c r="B41" s="8">
+        <v>1.6160011E-3</v>
+      </c>
+      <c r="C41" s="8">
+        <v>6.4470767999999998E-3</v>
+      </c>
+      <c r="D41" s="8">
+        <v>1.47697926E-2</v>
+      </c>
+      <c r="E41" s="8">
+        <v>2.7949094800000001E-2</v>
+      </c>
+      <c r="F41" s="8">
+        <v>0.14117407800000001</v>
+      </c>
+      <c r="G41" s="8">
+        <v>0.22094607350000001</v>
+      </c>
+      <c r="H41" s="8">
+        <v>6.5079309939999996</v>
+      </c>
+      <c r="I41" s="8">
+        <v>26.752557992900002</v>
+      </c>
+      <c r="J41" s="8">
+        <v>59.227169990500002</v>
+      </c>
+      <c r="K41" s="8">
+        <v>103.09226202959999</v>
+      </c>
+      <c r="L41" s="8">
+        <v>230.20986580850001</v>
+      </c>
+      <c r="M41" s="8">
+        <v>494.42150998120002</v>
+      </c>
+      <c r="N41" s="8">
+        <v>675.10587501529994</v>
+      </c>
       <c r="O41" s="1"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
@@ -16507,24 +16662,64 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="AF41" s="14"/>
+      <c r="AG41" s="15"/>
+      <c r="AH41" s="15"/>
+      <c r="AI41" s="15"/>
+      <c r="AJ41" s="15"/>
+      <c r="AK41" s="15"/>
+      <c r="AL41" s="15"/>
+      <c r="AM41" s="15"/>
+      <c r="AN41" s="15"/>
+      <c r="AO41" s="15"/>
+      <c r="AP41" s="15"/>
+      <c r="AQ41" s="15"/>
+      <c r="AR41" s="15"/>
+      <c r="AS41" s="15"/>
+    </row>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="B42" s="8">
+        <v>1.621E-3</v>
+      </c>
+      <c r="C42" s="8">
+        <v>6.4450000000000002E-3</v>
+      </c>
+      <c r="D42" s="8">
+        <v>1.4871000000000001E-2</v>
+      </c>
+      <c r="E42" s="8">
+        <v>2.7952000000000001E-2</v>
+      </c>
+      <c r="F42" s="8">
+        <v>0.141177</v>
+      </c>
+      <c r="G42" s="8">
+        <v>0.22095200000000001</v>
+      </c>
+      <c r="H42" s="8">
+        <v>6.5078880000000003</v>
+      </c>
+      <c r="I42" s="8">
+        <v>26.749362999999999</v>
+      </c>
+      <c r="J42" s="8">
+        <v>59.227144000000003</v>
+      </c>
+      <c r="K42" s="8">
+        <v>103.092235</v>
+      </c>
+      <c r="L42" s="8">
+        <v>230.207098</v>
+      </c>
+      <c r="M42" s="8">
+        <v>494.35421700000001</v>
+      </c>
+      <c r="N42" s="8">
+        <v>675.10241799999994</v>
+      </c>
       <c r="O42" s="1"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
@@ -16532,24 +16727,64 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="AF42" s="14"/>
+      <c r="AG42" s="15"/>
+      <c r="AH42" s="15"/>
+      <c r="AI42" s="15"/>
+      <c r="AJ42" s="15"/>
+      <c r="AK42" s="15"/>
+      <c r="AL42" s="15"/>
+      <c r="AM42" s="15"/>
+      <c r="AN42" s="15"/>
+      <c r="AO42" s="15"/>
+      <c r="AP42" s="15"/>
+      <c r="AQ42" s="15"/>
+      <c r="AR42" s="15"/>
+      <c r="AS42" s="15"/>
+    </row>
+    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
+      <c r="B43" s="8">
+        <v>0</v>
+      </c>
+      <c r="C43" s="8">
+        <v>0</v>
+      </c>
+      <c r="D43" s="8">
+        <v>0</v>
+      </c>
+      <c r="E43" s="8">
+        <v>0</v>
+      </c>
+      <c r="F43" s="8">
+        <v>0</v>
+      </c>
+      <c r="G43" s="8">
+        <v>0</v>
+      </c>
+      <c r="H43" s="8">
+        <v>0</v>
+      </c>
+      <c r="I43" s="8">
+        <v>0</v>
+      </c>
+      <c r="J43" s="8">
+        <v>0</v>
+      </c>
+      <c r="K43" s="8">
+        <v>0</v>
+      </c>
+      <c r="L43" s="8">
+        <v>2.1770000000000001E-3</v>
+      </c>
+      <c r="M43" s="8">
+        <v>5.3744E-2</v>
+      </c>
+      <c r="N43" s="8">
+        <v>2.8530000000000001E-3</v>
+      </c>
       <c r="O43" s="1"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
@@ -16557,24 +16792,64 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="AF43" s="14"/>
+      <c r="AG43" s="15"/>
+      <c r="AH43" s="15"/>
+      <c r="AI43" s="15"/>
+      <c r="AJ43" s="15"/>
+      <c r="AK43" s="15"/>
+      <c r="AL43" s="15"/>
+      <c r="AM43" s="15"/>
+      <c r="AN43" s="15"/>
+      <c r="AO43" s="15"/>
+      <c r="AP43" s="15"/>
+      <c r="AQ43" s="15"/>
+      <c r="AR43" s="15"/>
+      <c r="AS43" s="15"/>
+    </row>
+    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
+      <c r="B44" s="8">
+        <v>100.30933585130001</v>
+      </c>
+      <c r="C44" s="8">
+        <v>99.967786990099995</v>
+      </c>
+      <c r="D44" s="8">
+        <v>100.6852326656</v>
+      </c>
+      <c r="E44" s="8">
+        <v>100.01039471110001</v>
+      </c>
+      <c r="F44" s="8">
+        <v>100.0020697938</v>
+      </c>
+      <c r="G44" s="8">
+        <v>100.0026823142</v>
+      </c>
+      <c r="H44" s="8">
+        <v>99.999339359399997</v>
+      </c>
+      <c r="I44" s="8">
+        <v>99.988057243200004</v>
+      </c>
+      <c r="J44" s="8">
+        <v>99.9999561172</v>
+      </c>
+      <c r="K44" s="8">
+        <v>99.999973781099996</v>
+      </c>
+      <c r="L44" s="8">
+        <v>99.999743360899998</v>
+      </c>
+      <c r="M44" s="8">
+        <v>99.997259629499993</v>
+      </c>
+      <c r="N44" s="8">
+        <v>99.999910530299999</v>
+      </c>
       <c r="O44" s="1"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
@@ -16582,32 +16857,62 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
+      <c r="AF44" s="14"/>
+      <c r="AG44" s="14"/>
+      <c r="AH44" s="14"/>
+      <c r="AI44" s="14"/>
+      <c r="AJ44" s="14"/>
+      <c r="AK44" s="14"/>
+      <c r="AL44" s="14"/>
+      <c r="AM44" s="14"/>
+      <c r="AN44" s="14"/>
+      <c r="AO44" s="14"/>
+      <c r="AP44" s="14"/>
+      <c r="AQ44" s="14"/>
+      <c r="AR44" s="14"/>
+      <c r="AS44" s="14"/>
+    </row>
+    <row r="45" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="AF45" s="14"/>
+      <c r="AG45" s="14"/>
+      <c r="AH45" s="14"/>
+      <c r="AI45" s="14"/>
+      <c r="AJ45" s="14"/>
+      <c r="AK45" s="14"/>
+      <c r="AL45" s="14"/>
+      <c r="AM45" s="14"/>
+      <c r="AN45" s="14"/>
+      <c r="AO45" s="14"/>
+      <c r="AP45" s="14"/>
+      <c r="AQ45" s="14"/>
+      <c r="AR45" s="14"/>
+      <c r="AS45" s="14"/>
     </row>
     <row r="49" spans="1:21" ht="229.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
-      <c r="S50" s="8"/>
-      <c r="T50" s="8"/>
-      <c r="U50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
@@ -16678,19 +16983,45 @@
       <c r="A52" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+      <c r="B52" s="8">
+        <v>1.8229485E-3</v>
+      </c>
+      <c r="C52" s="8">
+        <v>6.9580077999999998E-3</v>
+      </c>
+      <c r="D52" s="8">
+        <v>1.6651153599999999E-2</v>
+      </c>
+      <c r="E52" s="8">
+        <v>3.0879020699999999E-2</v>
+      </c>
+      <c r="F52" s="8">
+        <v>0.14686989780000001</v>
+      </c>
+      <c r="G52" s="8">
+        <v>0.25073909760000002</v>
+      </c>
+      <c r="H52" s="8">
+        <v>6.7361590861999998</v>
+      </c>
+      <c r="I52" s="8">
+        <v>27.236689090700001</v>
+      </c>
+      <c r="J52" s="8">
+        <v>59.848061084699999</v>
+      </c>
+      <c r="K52" s="8">
+        <v>108.50353097919999</v>
+      </c>
+      <c r="L52" s="8">
+        <v>366.31396508220001</v>
+      </c>
+      <c r="M52" s="8">
+        <v>429.93227386469999</v>
+      </c>
+      <c r="N52" s="8">
+        <v>688.3177878857</v>
+      </c>
       <c r="O52" s="1"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="6"/>
@@ -16703,19 +17034,45 @@
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
+      <c r="B53" s="8">
+        <v>0</v>
+      </c>
+      <c r="C53" s="8">
+        <v>6.7650000000000002E-3</v>
+      </c>
+      <c r="D53" s="8">
+        <v>1.6177E-2</v>
+      </c>
+      <c r="E53" s="8">
+        <v>3.0009999999999998E-2</v>
+      </c>
+      <c r="F53" s="8">
+        <v>0.135573</v>
+      </c>
+      <c r="G53" s="8">
+        <v>0.24366199999999999</v>
+      </c>
+      <c r="H53" s="8">
+        <v>6.5335419999999997</v>
+      </c>
+      <c r="I53" s="8">
+        <v>27.353097000000002</v>
+      </c>
+      <c r="J53" s="8">
+        <v>59.916975000000001</v>
+      </c>
+      <c r="K53" s="8">
+        <v>108.16159399999999</v>
+      </c>
+      <c r="L53" s="8">
+        <v>366.289851</v>
+      </c>
+      <c r="M53" s="8">
+        <v>430.24897600000003</v>
+      </c>
+      <c r="N53" s="8">
+        <v>688.46476900000005</v>
+      </c>
       <c r="O53" s="1"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
@@ -16728,19 +17085,45 @@
       <c r="A54" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
+      <c r="B54" s="8">
+        <v>1.7780000000000001E-3</v>
+      </c>
+      <c r="C54" s="8">
+        <v>0</v>
+      </c>
+      <c r="D54" s="8">
+        <v>0</v>
+      </c>
+      <c r="E54" s="8">
+        <v>0</v>
+      </c>
+      <c r="F54" s="8">
+        <v>7.1549999999999999E-3</v>
+      </c>
+      <c r="G54" s="8">
+        <v>0</v>
+      </c>
+      <c r="H54" s="8">
+        <v>0</v>
+      </c>
+      <c r="I54" s="8">
+        <v>0</v>
+      </c>
+      <c r="J54" s="8">
+        <v>9.3189999999999992E-3</v>
+      </c>
+      <c r="K54" s="8">
+        <v>0</v>
+      </c>
+      <c r="L54" s="8">
+        <v>3.0630999999999999E-2</v>
+      </c>
+      <c r="M54" s="8">
+        <v>4.4349999999999997E-3</v>
+      </c>
+      <c r="N54" s="8">
+        <v>3.31E-3</v>
+      </c>
       <c r="O54" s="1"/>
       <c r="P54" s="6"/>
       <c r="Q54" s="6"/>
@@ -16753,19 +17136,45 @@
       <c r="A55" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
+      <c r="B55" s="8">
+        <v>97.534299136800001</v>
+      </c>
+      <c r="C55" s="8">
+        <v>97.226105263199997</v>
+      </c>
+      <c r="D55" s="8">
+        <v>97.152428132899999</v>
+      </c>
+      <c r="E55" s="8">
+        <v>97.185724574600002</v>
+      </c>
+      <c r="F55" s="8">
+        <v>97.179886482399993</v>
+      </c>
+      <c r="G55" s="8">
+        <v>97.177505357900003</v>
+      </c>
+      <c r="H55" s="8">
+        <v>96.992097668200003</v>
+      </c>
+      <c r="I55" s="8">
+        <v>100.42739375879999</v>
+      </c>
+      <c r="J55" s="8">
+        <v>100.1307192143</v>
+      </c>
+      <c r="K55" s="8">
+        <v>99.684860966200006</v>
+      </c>
+      <c r="L55" s="8">
+        <v>100.0017790525</v>
+      </c>
+      <c r="M55" s="8">
+        <v>100.07469481930001</v>
+      </c>
+      <c r="N55" s="8">
+        <v>100.0218345533</v>
+      </c>
       <c r="O55" s="1"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="6"/>
@@ -16776,29 +17185,29 @@
     </row>
     <row r="56" spans="1:21" ht="206" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="57" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
-      <c r="Q57" s="14"/>
-      <c r="R57" s="14"/>
-      <c r="S57" s="14"/>
-      <c r="T57" s="14"/>
-      <c r="U57" s="14"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="13"/>
+      <c r="U57" s="13"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
@@ -16869,61 +17278,61 @@
       <c r="A59" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B59" s="8">
         <v>5.7601929999999998E-4</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="8">
         <v>2.3689269999999998E-3</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="8">
         <v>4.9281120000000001E-3</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="8">
         <v>9.1629028000000008E-3</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F59" s="8">
         <v>3.5285949699999999E-2</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G59" s="8">
         <v>5.4972886999999998E-2</v>
       </c>
-      <c r="H59" s="9">
+      <c r="H59" s="8">
         <v>1.3339941501999999</v>
       </c>
-      <c r="I59" s="9">
+      <c r="I59" s="8">
         <v>5.2925069332000003</v>
       </c>
-      <c r="J59" s="9">
+      <c r="J59" s="8">
         <v>12.082659959800001</v>
       </c>
-      <c r="K59" s="9">
+      <c r="K59" s="8">
         <v>21.359937906300001</v>
       </c>
-      <c r="L59" s="9">
+      <c r="L59" s="8">
         <v>50.672094821899996</v>
       </c>
-      <c r="M59" s="9">
+      <c r="M59" s="8">
         <v>87.357614040399994</v>
       </c>
-      <c r="N59" s="9">
+      <c r="N59" s="8">
         <v>142.77942395209999</v>
       </c>
-      <c r="O59" s="9">
+      <c r="O59" s="8">
         <v>214.40739488599999</v>
       </c>
-      <c r="P59" s="9">
+      <c r="P59" s="8">
         <v>285.78975009919998</v>
       </c>
-      <c r="Q59" s="9">
+      <c r="Q59" s="8">
         <v>365.74295783039997</v>
       </c>
-      <c r="R59" s="9">
+      <c r="R59" s="8">
         <v>468.78817796710001</v>
       </c>
-      <c r="S59" s="9">
+      <c r="S59" s="8">
         <v>572.85432004929999</v>
       </c>
-      <c r="T59" s="9" t="s">
+      <c r="T59" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U59" s="6" t="s">
@@ -16934,61 +17343,61 @@
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B60" s="8">
         <v>5.8E-4</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="8">
         <v>2.3730000000000001E-3</v>
       </c>
-      <c r="D60" s="9">
+      <c r="D60" s="8">
         <v>4.9890000000000004E-3</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="8">
         <v>9.1660000000000005E-3</v>
       </c>
-      <c r="F60" s="9">
+      <c r="F60" s="8">
         <v>3.5290000000000002E-2</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G60" s="8">
         <v>5.4976999999999998E-2</v>
       </c>
-      <c r="H60" s="9">
+      <c r="H60" s="8">
         <v>1.333947</v>
       </c>
-      <c r="I60" s="9">
+      <c r="I60" s="8">
         <v>5.2924709999999999</v>
       </c>
-      <c r="J60" s="9">
+      <c r="J60" s="8">
         <v>12.082432000000001</v>
       </c>
-      <c r="K60" s="9">
+      <c r="K60" s="8">
         <v>21.359826999999999</v>
       </c>
-      <c r="L60" s="9">
+      <c r="L60" s="8">
         <v>50.672055999999998</v>
       </c>
-      <c r="M60" s="9">
+      <c r="M60" s="8">
         <v>87.356798999999995</v>
       </c>
-      <c r="N60" s="9">
+      <c r="N60" s="8">
         <v>142.77932799999999</v>
       </c>
-      <c r="O60" s="9">
+      <c r="O60" s="8">
         <v>214.39453800000001</v>
       </c>
-      <c r="P60" s="9">
+      <c r="P60" s="8">
         <v>285.78916199999998</v>
       </c>
-      <c r="Q60" s="9">
+      <c r="Q60" s="8">
         <v>365.728814</v>
       </c>
-      <c r="R60" s="9">
+      <c r="R60" s="8">
         <v>468.75717900000001</v>
       </c>
-      <c r="S60" s="9">
+      <c r="S60" s="8">
         <v>572.84291800000005</v>
       </c>
-      <c r="T60" s="9" t="s">
+      <c r="T60" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U60" s="6" t="s">
@@ -16999,61 +17408,61 @@
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B61" s="8">
         <v>0</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="8">
         <v>0</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="8">
         <v>0</v>
       </c>
-      <c r="E61" s="9">
+      <c r="E61" s="8">
         <v>0</v>
       </c>
-      <c r="F61" s="9">
+      <c r="F61" s="8">
         <v>0</v>
       </c>
-      <c r="G61" s="9">
+      <c r="G61" s="8">
         <v>0</v>
       </c>
-      <c r="H61" s="9">
+      <c r="H61" s="8">
         <v>0</v>
       </c>
-      <c r="I61" s="9">
+      <c r="I61" s="8">
         <v>0</v>
       </c>
-      <c r="J61" s="9">
+      <c r="J61" s="8">
         <v>0</v>
       </c>
-      <c r="K61" s="9">
+      <c r="K61" s="8">
         <v>0</v>
       </c>
-      <c r="L61" s="9">
+      <c r="L61" s="8">
         <v>0</v>
       </c>
-      <c r="M61" s="9">
+      <c r="M61" s="8">
         <v>7.5100000000000004E-4</v>
       </c>
-      <c r="N61" s="9">
+      <c r="N61" s="8">
         <v>0</v>
       </c>
-      <c r="O61" s="9">
+      <c r="O61" s="8">
         <v>1.7240000000000001E-3</v>
       </c>
-      <c r="P61" s="9">
+      <c r="P61" s="8">
         <v>0</v>
       </c>
-      <c r="Q61" s="9">
+      <c r="Q61" s="8">
         <v>1.4119E-2</v>
       </c>
-      <c r="R61" s="9">
+      <c r="R61" s="8">
         <v>3.0170000000000002E-3</v>
       </c>
-      <c r="S61" s="9">
+      <c r="S61" s="8">
         <v>1.1112E-2</v>
       </c>
-      <c r="T61" s="9" t="s">
+      <c r="T61" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U61" s="6" t="s">
@@ -17064,61 +17473,61 @@
       <c r="A62" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="8">
         <v>100.6910728477</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="8">
         <v>100.17193429949999</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="8">
         <v>101.23552325110001</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="8">
         <v>100.0338011657</v>
       </c>
-      <c r="F62" s="9">
+      <c r="F62" s="8">
         <v>100.0114784865</v>
       </c>
-      <c r="G62" s="9">
+      <c r="G62" s="8">
         <v>100.0074817988</v>
       </c>
-      <c r="H62" s="9">
+      <c r="H62" s="8">
         <v>99.996465489599998</v>
       </c>
-      <c r="I62" s="9">
+      <c r="I62" s="8">
         <v>99.999321054999996</v>
       </c>
-      <c r="J62" s="9">
+      <c r="J62" s="8">
         <v>99.998113331100001</v>
       </c>
-      <c r="K62" s="9">
+      <c r="K62" s="8">
         <v>99.999480774399998</v>
       </c>
-      <c r="L62" s="9">
+      <c r="L62" s="8">
         <v>99.999923386000006</v>
       </c>
-      <c r="M62" s="9">
+      <c r="M62" s="8">
         <v>99.999926691699997</v>
       </c>
-      <c r="N62" s="9">
+      <c r="N62" s="8">
         <v>99.999932797</v>
       </c>
-      <c r="O62" s="9">
+      <c r="O62" s="8">
         <v>99.994807601700003</v>
       </c>
-      <c r="P62" s="9">
+      <c r="P62" s="8">
         <v>99.999794219600005</v>
       </c>
-      <c r="Q62" s="9">
+      <c r="Q62" s="8">
         <v>99.999993211000003</v>
       </c>
-      <c r="R62" s="9">
+      <c r="R62" s="8">
         <v>99.994030999800003</v>
       </c>
-      <c r="S62" s="9">
+      <c r="S62" s="8">
         <v>99.999949367699998</v>
       </c>
-      <c r="T62" s="9" t="s">
+      <c r="T62" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U62" s="6" t="s">
@@ -17127,29 +17536,29 @@
     </row>
     <row r="63" spans="1:21" ht="221" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
-      <c r="P64" s="10"/>
-      <c r="Q64" s="10"/>
-      <c r="R64" s="10"/>
-      <c r="S64" s="10"/>
-      <c r="T64" s="10"/>
-      <c r="U64" s="10"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="P64" s="9"/>
+      <c r="Q64" s="9"/>
+      <c r="R64" s="9"/>
+      <c r="S64" s="9"/>
+      <c r="T64" s="9"/>
+      <c r="U64" s="9"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
@@ -17220,61 +17629,61 @@
       <c r="A66" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="8">
         <v>2.8278828000000002E-3</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="8">
         <v>8.5809231000000003E-3</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D66" s="8">
         <v>1.6232967399999999E-2</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E66" s="8">
         <v>3.3911228199999997E-2</v>
       </c>
-      <c r="F66" s="9">
+      <c r="F66" s="8">
         <v>7.7762126900000006E-2</v>
       </c>
-      <c r="G66" s="9">
+      <c r="G66" s="8">
         <v>0.1040349007</v>
       </c>
-      <c r="H66" s="9">
+      <c r="H66" s="8">
         <v>2.6799488068000001</v>
       </c>
-      <c r="I66" s="9">
+      <c r="I66" s="8">
         <v>11.709309101100001</v>
       </c>
-      <c r="J66" s="9">
+      <c r="J66" s="8">
         <v>26.516411066100002</v>
       </c>
-      <c r="K66" s="9">
+      <c r="K66" s="8">
         <v>47.511326074599999</v>
       </c>
-      <c r="L66" s="9">
+      <c r="L66" s="8">
         <v>110.3050270081</v>
       </c>
-      <c r="M66" s="9">
+      <c r="M66" s="8">
         <v>215.80932497980001</v>
       </c>
-      <c r="N66" s="9">
+      <c r="N66" s="8">
         <v>370.09260606769999</v>
       </c>
-      <c r="O66" s="9">
+      <c r="O66" s="8">
         <v>423.15952706339999</v>
       </c>
-      <c r="P66" s="9">
+      <c r="P66" s="8">
         <v>539.57744288440006</v>
       </c>
-      <c r="Q66" s="9">
+      <c r="Q66" s="8">
         <v>742.98159098630003</v>
       </c>
-      <c r="R66" s="9">
+      <c r="R66" s="8">
         <v>1081.3501529693999</v>
       </c>
-      <c r="S66" s="9">
+      <c r="S66" s="8">
         <v>1392.5612359047</v>
       </c>
-      <c r="T66" s="9" t="s">
+      <c r="T66" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U66" s="6" t="s">
@@ -17285,61 +17694,61 @@
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="8">
         <v>2.843E-3</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="8">
         <v>8.6009999999999993E-3</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D67" s="8">
         <v>1.6343E-2</v>
       </c>
-      <c r="E67" s="9">
+      <c r="E67" s="8">
         <v>3.3945999999999997E-2</v>
       </c>
-      <c r="F67" s="9">
+      <c r="F67" s="8">
         <v>7.7830999999999997E-2</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G67" s="8">
         <v>9.6765000000000004E-2</v>
       </c>
-      <c r="H67" s="9">
+      <c r="H67" s="8">
         <v>2.674061</v>
       </c>
-      <c r="I67" s="9">
+      <c r="I67" s="8">
         <v>11.629759</v>
       </c>
-      <c r="J67" s="9">
+      <c r="J67" s="8">
         <v>26.561571000000001</v>
       </c>
-      <c r="K67" s="9">
+      <c r="K67" s="8">
         <v>47.486843999999998</v>
       </c>
-      <c r="L67" s="9">
+      <c r="L67" s="8">
         <v>110.336692</v>
       </c>
-      <c r="M67" s="9">
+      <c r="M67" s="8">
         <v>215.82109399999999</v>
       </c>
-      <c r="N67" s="9">
+      <c r="N67" s="8">
         <v>370.01094000000001</v>
       </c>
-      <c r="O67" s="9">
+      <c r="O67" s="8">
         <v>423.06676299999998</v>
       </c>
-      <c r="P67" s="9">
+      <c r="P67" s="8">
         <v>539.63937899999996</v>
       </c>
-      <c r="Q67" s="9">
+      <c r="Q67" s="8">
         <v>742.91013499999997</v>
       </c>
-      <c r="R67" s="9">
+      <c r="R67" s="8">
         <v>1081.401175</v>
       </c>
-      <c r="S67" s="9">
+      <c r="S67" s="8">
         <v>1392.5149739999999</v>
       </c>
-      <c r="T67" s="9" t="s">
+      <c r="T67" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U67" s="6" t="s">
@@ -17350,61 +17759,61 @@
       <c r="A68" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B68" s="8">
         <v>0</v>
       </c>
-      <c r="C68" s="9">
+      <c r="C68" s="8">
         <v>0</v>
       </c>
-      <c r="D68" s="9">
+      <c r="D68" s="8">
         <v>0</v>
       </c>
-      <c r="E68" s="9">
+      <c r="E68" s="8">
         <v>0</v>
       </c>
-      <c r="F68" s="9">
+      <c r="F68" s="8">
         <v>0</v>
       </c>
-      <c r="G68" s="9">
+      <c r="G68" s="8">
         <v>7.2179999999999996E-3</v>
       </c>
-      <c r="H68" s="9">
+      <c r="H68" s="8">
         <v>0</v>
       </c>
-      <c r="I68" s="9">
+      <c r="I68" s="8">
         <v>0</v>
       </c>
-      <c r="J68" s="9">
+      <c r="J68" s="8">
         <v>0</v>
       </c>
-      <c r="K68" s="9">
+      <c r="K68" s="8">
         <v>0</v>
       </c>
-      <c r="L68" s="9">
+      <c r="L68" s="8">
         <v>4.744E-3</v>
       </c>
-      <c r="M68" s="9">
+      <c r="M68" s="8">
         <v>1.9910000000000001E-2</v>
       </c>
-      <c r="N68" s="9">
+      <c r="N68" s="8">
         <v>1.0709999999999999E-3</v>
       </c>
-      <c r="O68" s="9">
+      <c r="O68" s="8">
         <v>5.8708999999999997E-2</v>
       </c>
-      <c r="P68" s="9">
+      <c r="P68" s="8">
         <v>3.6080000000000001E-3</v>
       </c>
-      <c r="Q68" s="9">
+      <c r="Q68" s="8">
         <v>5.4938000000000001E-2</v>
       </c>
-      <c r="R68" s="9">
+      <c r="R68" s="8">
         <v>9.3329999999999993E-3</v>
       </c>
-      <c r="S68" s="9">
+      <c r="S68" s="8">
         <v>0</v>
       </c>
-      <c r="T68" s="9" t="s">
+      <c r="T68" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U68" s="6" t="s">
@@ -17415,61 +17824,61 @@
       <c r="A69" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="8">
         <v>100.53457779279999</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C69" s="8">
         <v>100.23397155959999</v>
       </c>
-      <c r="D69" s="9">
+      <c r="D69" s="8">
         <v>100.67783431540001</v>
       </c>
-      <c r="E69" s="9">
+      <c r="E69" s="8">
         <v>100.1025377786</v>
       </c>
-      <c r="F69" s="9">
+      <c r="F69" s="8">
         <v>100.0885689218</v>
       </c>
-      <c r="G69" s="9">
+      <c r="G69" s="8">
         <v>99.950112255600004</v>
       </c>
-      <c r="H69" s="9">
+      <c r="H69" s="8">
         <v>99.7803015211</v>
       </c>
-      <c r="I69" s="9">
+      <c r="I69" s="8">
         <v>99.320625150300003</v>
       </c>
-      <c r="J69" s="9">
+      <c r="J69" s="8">
         <v>100.1703093749</v>
       </c>
-      <c r="K69" s="9">
+      <c r="K69" s="8">
         <v>99.948471077099995</v>
       </c>
-      <c r="L69" s="9">
+      <c r="L69" s="8">
         <v>100.0330075545</v>
       </c>
-      <c r="M69" s="9">
+      <c r="M69" s="8">
         <v>100.0146791712</v>
       </c>
-      <c r="N69" s="9">
+      <c r="N69" s="8">
         <v>99.978222999799996</v>
       </c>
-      <c r="O69" s="9">
+      <c r="O69" s="8">
         <v>99.991952192699998</v>
       </c>
-      <c r="P69" s="9">
+      <c r="P69" s="8">
         <v>100.01214730460001</v>
       </c>
-      <c r="Q69" s="9">
+      <c r="Q69" s="8">
         <v>99.997776797399993</v>
       </c>
-      <c r="R69" s="9">
+      <c r="R69" s="8">
         <v>100.0055814512</v>
       </c>
-      <c r="S69" s="9">
+      <c r="S69" s="8">
         <v>99.996677926700002</v>
       </c>
-      <c r="T69" s="9" t="s">
+      <c r="T69" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U69" s="6" t="s">
@@ -17478,29 +17887,29 @@
     </row>
     <row r="70" spans="1:21" ht="204.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="71" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
-      <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10"/>
-      <c r="O71" s="10"/>
-      <c r="P71" s="10"/>
-      <c r="Q71" s="10"/>
-      <c r="R71" s="10"/>
-      <c r="S71" s="10"/>
-      <c r="T71" s="10"/>
-      <c r="U71" s="10"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+      <c r="O71" s="9"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="9"/>
+      <c r="R71" s="9"/>
+      <c r="S71" s="9"/>
+      <c r="T71" s="9"/>
+      <c r="U71" s="9"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
@@ -17571,64 +17980,64 @@
       <c r="A73" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" s="8">
         <v>2.2101400000000001E-4</v>
       </c>
-      <c r="C73" s="9">
+      <c r="C73" s="8">
         <v>5.6385989999999998E-4</v>
       </c>
-      <c r="D73" s="9">
+      <c r="D73" s="8">
         <v>7.7605250000000001E-4</v>
       </c>
-      <c r="E73" s="9">
+      <c r="E73" s="8">
         <v>1.3959408000000001E-3</v>
       </c>
-      <c r="F73" s="9">
+      <c r="F73" s="8">
         <v>1.20360851E-2</v>
       </c>
-      <c r="G73" s="9">
+      <c r="G73" s="8">
         <v>7.7548026999999997E-3</v>
       </c>
-      <c r="H73" s="9">
+      <c r="H73" s="8">
         <v>4.8887014399999998E-2</v>
       </c>
-      <c r="I73" s="9">
+      <c r="I73" s="8">
         <v>7.8410148599999993E-2</v>
       </c>
-      <c r="J73" s="9">
+      <c r="J73" s="8">
         <v>0.1100490093</v>
       </c>
-      <c r="K73" s="9">
+      <c r="K73" s="8">
         <v>0.19690799710000001</v>
       </c>
-      <c r="L73" s="9">
+      <c r="L73" s="8">
         <v>0.25797605509999999</v>
       </c>
-      <c r="M73" s="9">
+      <c r="M73" s="8">
         <v>0.44618296619999998</v>
       </c>
-      <c r="N73" s="9">
+      <c r="N73" s="8">
         <v>0.53032684330000002</v>
       </c>
-      <c r="O73" s="9">
+      <c r="O73" s="8">
         <v>0.66568994520000002</v>
       </c>
-      <c r="P73" s="9">
+      <c r="P73" s="8">
         <v>0.72402000430000002</v>
       </c>
-      <c r="Q73" s="9">
+      <c r="Q73" s="8">
         <v>1.0612299441999999</v>
       </c>
-      <c r="R73" s="9">
+      <c r="R73" s="8">
         <v>1.1045930386</v>
       </c>
-      <c r="S73" s="9">
+      <c r="S73" s="8">
         <v>1.2405769824999999</v>
       </c>
-      <c r="T73" s="9">
+      <c r="T73" s="8">
         <v>2.1346609592000001</v>
       </c>
-      <c r="U73" s="9">
+      <c r="U73" s="8">
         <v>3.3455178738</v>
       </c>
     </row>
@@ -17636,64 +18045,64 @@
       <c r="A74" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="9">
+      <c r="B74" s="8">
         <v>2.2499999999999999E-4</v>
       </c>
-      <c r="C74" s="9">
+      <c r="C74" s="8">
         <v>5.6599999999999999E-4</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="8">
         <v>7.85E-4</v>
       </c>
-      <c r="E74" s="9">
+      <c r="E74" s="8">
         <v>1.3910000000000001E-3</v>
       </c>
-      <c r="F74" s="9">
+      <c r="F74" s="8">
         <v>1.1957000000000001E-2</v>
       </c>
-      <c r="G74" s="9">
+      <c r="G74" s="8">
         <v>5.9369999999999996E-3</v>
       </c>
-      <c r="H74" s="9">
+      <c r="H74" s="8">
         <v>4.8524999999999999E-2</v>
       </c>
-      <c r="I74" s="9">
+      <c r="I74" s="8">
         <v>7.7803999999999998E-2</v>
       </c>
-      <c r="J74" s="9">
+      <c r="J74" s="8">
         <v>0.10614800000000001</v>
       </c>
-      <c r="K74" s="9">
+      <c r="K74" s="8">
         <v>0.19534899999999999</v>
       </c>
-      <c r="L74" s="9">
+      <c r="L74" s="8">
         <v>0.255888</v>
       </c>
-      <c r="M74" s="9">
+      <c r="M74" s="8">
         <v>0.43981100000000001</v>
       </c>
-      <c r="N74" s="9">
+      <c r="N74" s="8">
         <v>0.51870700000000003</v>
       </c>
-      <c r="O74" s="9">
+      <c r="O74" s="8">
         <v>0.65995000000000004</v>
       </c>
-      <c r="P74" s="9">
+      <c r="P74" s="8">
         <v>0.71764399999999995</v>
       </c>
-      <c r="Q74" s="9">
+      <c r="Q74" s="8">
         <v>1.0397400000000001</v>
       </c>
-      <c r="R74" s="9">
+      <c r="R74" s="8">
         <v>1.0990470000000001</v>
       </c>
-      <c r="S74" s="9">
+      <c r="S74" s="8">
         <v>1.2740940000000001</v>
       </c>
-      <c r="T74" s="9">
+      <c r="T74" s="8">
         <v>2.1465109999999998</v>
       </c>
-      <c r="U74" s="9">
+      <c r="U74" s="8">
         <v>3.338778</v>
       </c>
     </row>
@@ -17701,64 +18110,64 @@
       <c r="A75" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B75" s="8">
         <v>6.1300000000000005E-4</v>
       </c>
-      <c r="C75" s="9">
+      <c r="C75" s="8">
         <v>0</v>
       </c>
-      <c r="D75" s="9">
+      <c r="D75" s="8">
         <v>0</v>
       </c>
-      <c r="E75" s="9">
+      <c r="E75" s="8">
         <v>0</v>
       </c>
-      <c r="F75" s="9">
+      <c r="F75" s="8">
         <v>0</v>
       </c>
-      <c r="G75" s="9">
+      <c r="G75" s="8">
         <v>1.7669999999999999E-3</v>
       </c>
-      <c r="H75" s="9">
+      <c r="H75" s="8">
         <v>0</v>
       </c>
-      <c r="I75" s="9">
+      <c r="I75" s="8">
         <v>0</v>
       </c>
-      <c r="J75" s="9">
+      <c r="J75" s="8">
         <v>3.026E-3</v>
       </c>
-      <c r="K75" s="9">
+      <c r="K75" s="8">
         <v>0</v>
       </c>
-      <c r="L75" s="9">
+      <c r="L75" s="8">
         <v>0</v>
       </c>
-      <c r="M75" s="9">
+      <c r="M75" s="8">
         <v>2.6749999999999999E-3</v>
       </c>
-      <c r="N75" s="9">
+      <c r="N75" s="8">
         <v>7.1630000000000001E-3</v>
       </c>
-      <c r="O75" s="9">
+      <c r="O75" s="8">
         <v>0</v>
       </c>
-      <c r="P75" s="9">
+      <c r="P75" s="8">
         <v>0</v>
       </c>
-      <c r="Q75" s="9">
+      <c r="Q75" s="8">
         <v>1.1790999999999999E-2</v>
       </c>
-      <c r="R75" s="9">
+      <c r="R75" s="8">
         <v>0</v>
       </c>
-      <c r="S75" s="9">
+      <c r="S75" s="8">
         <v>1.3339999999999999E-3</v>
       </c>
-      <c r="T75" s="9">
+      <c r="T75" s="8">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="U75" s="9">
+      <c r="U75" s="8">
         <v>1.7364999999999998E-2</v>
       </c>
     </row>
@@ -17766,92 +18175,92 @@
       <c r="A76" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="9">
+      <c r="B76" s="8">
         <v>101.8034951456</v>
       </c>
-      <c r="C76" s="9">
+      <c r="C76" s="8">
         <v>100.3795375899</v>
       </c>
-      <c r="D76" s="9">
+      <c r="D76" s="8">
         <v>101.15295360979999</v>
       </c>
-      <c r="E76" s="9">
+      <c r="E76" s="8">
         <v>99.646060871100005</v>
       </c>
-      <c r="F76" s="9">
+      <c r="F76" s="8">
         <v>99.342933122000005</v>
       </c>
-      <c r="G76" s="9">
+      <c r="G76" s="8">
         <v>99.344887216399997</v>
       </c>
-      <c r="H76" s="9">
+      <c r="H76" s="8">
         <v>99.259487629700004</v>
       </c>
-      <c r="I76" s="9">
+      <c r="I76" s="8">
         <v>99.226951317800001</v>
       </c>
-      <c r="J76" s="9">
+      <c r="J76" s="8">
         <v>99.204891231199994</v>
       </c>
-      <c r="K76" s="9">
+      <c r="K76" s="8">
         <v>99.208261140199994</v>
       </c>
-      <c r="L76" s="9">
+      <c r="L76" s="8">
         <v>99.190601180399995</v>
       </c>
-      <c r="M76" s="9">
+      <c r="M76" s="8">
         <v>99.171423718100002</v>
       </c>
-      <c r="N76" s="9">
+      <c r="N76" s="8">
         <v>99.159604436699993</v>
       </c>
-      <c r="O76" s="9">
+      <c r="O76" s="8">
         <v>99.137744942300003</v>
       </c>
-      <c r="P76" s="9">
+      <c r="P76" s="8">
         <v>99.119360758699997</v>
       </c>
-      <c r="Q76" s="9">
+      <c r="Q76" s="8">
         <v>99.086065722000001</v>
       </c>
-      <c r="R76" s="9">
+      <c r="R76" s="8">
         <v>99.497911143300001</v>
       </c>
-      <c r="S76" s="9">
+      <c r="S76" s="8">
         <v>102.8092587557</v>
       </c>
-      <c r="T76" s="9">
+      <c r="T76" s="8">
         <v>101.1781749531</v>
       </c>
-      <c r="U76" s="9">
+      <c r="U76" s="8">
         <v>100.3175928701</v>
       </c>
     </row>
     <row r="77" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="78" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
-      <c r="H78" s="10"/>
-      <c r="I78" s="10"/>
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="10"/>
-      <c r="N78" s="10"/>
-      <c r="O78" s="10"/>
-      <c r="P78" s="10"/>
-      <c r="Q78" s="10"/>
-      <c r="R78" s="10"/>
-      <c r="S78" s="10"/>
-      <c r="T78" s="10"/>
-      <c r="U78" s="10"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+      <c r="O78" s="9"/>
+      <c r="P78" s="9"/>
+      <c r="Q78" s="9"/>
+      <c r="R78" s="9"/>
+      <c r="S78" s="9"/>
+      <c r="T78" s="9"/>
+      <c r="U78" s="9"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
@@ -18020,29 +18429,29 @@
     </row>
     <row r="84" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="85" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
-      <c r="I85" s="10"/>
-      <c r="J85" s="10"/>
-      <c r="K85" s="10"/>
-      <c r="L85" s="10"/>
-      <c r="M85" s="10"/>
-      <c r="N85" s="10"/>
-      <c r="O85" s="10"/>
-      <c r="P85" s="10"/>
-      <c r="Q85" s="10"/>
-      <c r="R85" s="10"/>
-      <c r="S85" s="10"/>
-      <c r="T85" s="10"/>
-      <c r="U85" s="10"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
+      <c r="O85" s="9"/>
+      <c r="P85" s="9"/>
+      <c r="Q85" s="9"/>
+      <c r="R85" s="9"/>
+      <c r="S85" s="9"/>
+      <c r="T85" s="9"/>
+      <c r="U85" s="9"/>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
@@ -18113,64 +18522,64 @@
       <c r="A87" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87" s="8">
         <v>1.158714E-4</v>
       </c>
-      <c r="C87" s="9">
+      <c r="C87" s="8">
         <v>2.6392940000000001E-4</v>
       </c>
-      <c r="D87" s="9">
+      <c r="D87" s="8">
         <v>3.7097930000000001E-4</v>
       </c>
-      <c r="E87" s="9">
+      <c r="E87" s="8">
         <v>5.2189830000000002E-4</v>
       </c>
-      <c r="F87" s="9">
+      <c r="F87" s="8">
         <v>1.1429787E-3</v>
       </c>
-      <c r="G87" s="9">
+      <c r="G87" s="8">
         <v>1.445055E-3</v>
       </c>
-      <c r="H87" s="9">
+      <c r="H87" s="8">
         <v>1.8814086899999999E-2</v>
       </c>
-      <c r="I87" s="9">
+      <c r="I87" s="8">
         <v>1.9310951199999999E-2</v>
       </c>
-      <c r="J87" s="9">
+      <c r="J87" s="8">
         <v>3.8014173499999998E-2</v>
       </c>
-      <c r="K87" s="9">
+      <c r="K87" s="8">
         <v>3.8465023000000001E-2</v>
       </c>
-      <c r="L87" s="9">
-        <v>0.102408886</v>
-      </c>
-      <c r="M87" s="9">
+      <c r="L87" s="8">
+        <v>9.0778112399999999E-2</v>
+      </c>
+      <c r="M87" s="8">
         <v>7.6631069199999999E-2</v>
       </c>
-      <c r="N87" s="9">
+      <c r="N87" s="8">
         <v>9.5789909399999998E-2</v>
       </c>
-      <c r="O87" s="9">
+      <c r="O87" s="8">
         <v>0.14233803749999999</v>
       </c>
-      <c r="P87" s="9">
+      <c r="P87" s="8">
         <v>0.16123008729999999</v>
       </c>
-      <c r="Q87" s="9">
+      <c r="Q87" s="8">
         <v>0.16359996800000001</v>
       </c>
-      <c r="R87" s="9">
-        <v>0.29176807399999999</v>
-      </c>
-      <c r="S87" s="9">
+      <c r="R87" s="8">
+        <v>0.22102785110000001</v>
+      </c>
+      <c r="S87" s="8">
         <v>0.24379897119999999</v>
       </c>
-      <c r="T87" s="9">
+      <c r="T87" s="8">
         <v>0.31916880609999998</v>
       </c>
-      <c r="U87" s="9">
+      <c r="U87" s="8">
         <v>0.48191308980000003</v>
       </c>
     </row>
@@ -18178,64 +18587,64 @@
       <c r="A88" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="9">
+      <c r="B88" s="8">
         <v>1.21E-4</v>
       </c>
-      <c r="C88" s="9">
+      <c r="C88" s="8">
         <v>2.7E-4</v>
       </c>
-      <c r="D88" s="9">
+      <c r="D88" s="8">
         <v>3.77E-4</v>
       </c>
-      <c r="E88" s="9">
+      <c r="E88" s="8">
         <v>5.2800000000000004E-4</v>
       </c>
-      <c r="F88" s="9">
+      <c r="F88" s="8">
         <v>1.1479999999999999E-3</v>
       </c>
-      <c r="G88" s="9">
+      <c r="G88" s="8">
         <v>1.4530000000000001E-3</v>
       </c>
-      <c r="H88" s="9">
+      <c r="H88" s="8">
         <v>1.8869E-2</v>
       </c>
-      <c r="I88" s="9">
+      <c r="I88" s="8">
         <v>1.8360999999999999E-2</v>
       </c>
-      <c r="J88" s="9">
+      <c r="J88" s="8">
         <v>2.9499999999999998E-2</v>
       </c>
-      <c r="K88" s="9">
+      <c r="K88" s="8">
         <v>3.8543000000000001E-2</v>
       </c>
-      <c r="L88" s="9">
-        <v>7.9287999999999997E-2</v>
-      </c>
-      <c r="M88" s="9">
+      <c r="L88" s="8">
+        <v>9.0782000000000002E-2</v>
+      </c>
+      <c r="M88" s="8">
         <v>7.6680999999999999E-2</v>
       </c>
-      <c r="N88" s="9">
+      <c r="N88" s="8">
         <v>9.4359999999999999E-2</v>
       </c>
-      <c r="O88" s="9">
+      <c r="O88" s="8">
         <v>0.1421</v>
       </c>
-      <c r="P88" s="9">
+      <c r="P88" s="8">
         <v>0.15512500000000001</v>
       </c>
-      <c r="Q88" s="9">
+      <c r="Q88" s="8">
         <v>0.15345900000000001</v>
       </c>
-      <c r="R88" s="9">
-        <v>0.28173199999999998</v>
-      </c>
-      <c r="S88" s="9">
+      <c r="R88" s="8">
+        <v>0.22102785110000001</v>
+      </c>
+      <c r="S88" s="8">
         <v>0.24270900000000001</v>
       </c>
-      <c r="T88" s="9">
+      <c r="T88" s="8">
         <v>0.306338</v>
       </c>
-      <c r="U88" s="9">
+      <c r="U88" s="8">
         <v>0.43904399999999999</v>
       </c>
     </row>
@@ -18243,64 +18652,64 @@
       <c r="A89" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B89" s="8">
         <v>0</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C89" s="8">
         <v>0</v>
       </c>
-      <c r="D89" s="9">
+      <c r="D89" s="8">
         <v>0</v>
       </c>
-      <c r="E89" s="9">
+      <c r="E89" s="8">
         <v>0</v>
       </c>
-      <c r="F89" s="9">
+      <c r="F89" s="8">
         <v>0</v>
       </c>
-      <c r="G89" s="9">
+      <c r="G89" s="8">
         <v>0</v>
       </c>
-      <c r="H89" s="9">
+      <c r="H89" s="8">
         <v>0</v>
       </c>
-      <c r="I89" s="9">
+      <c r="I89" s="8">
         <v>9.990000000000001E-4</v>
       </c>
-      <c r="J89" s="9">
+      <c r="J89" s="8">
         <v>8.6060000000000008E-3</v>
       </c>
-      <c r="K89" s="9">
+      <c r="K89" s="8">
         <v>0</v>
       </c>
-      <c r="L89" s="9">
-        <v>2.3192000000000001E-2</v>
-      </c>
-      <c r="M89" s="9">
+      <c r="L89" s="8">
         <v>0</v>
       </c>
-      <c r="N89" s="9">
+      <c r="M89" s="8">
+        <v>0</v>
+      </c>
+      <c r="N89" s="8">
         <v>1.4779999999999999E-3</v>
       </c>
-      <c r="O89" s="9">
+      <c r="O89" s="8">
         <v>0</v>
       </c>
-      <c r="P89" s="9">
+      <c r="P89" s="8">
         <v>5.633E-3</v>
       </c>
-      <c r="Q89" s="9">
+      <c r="Q89" s="8">
         <v>9.6740000000000003E-3</v>
       </c>
-      <c r="R89" s="9">
+      <c r="R89" s="8">
         <v>8.9200000000000008E-3</v>
       </c>
-      <c r="S89" s="9">
+      <c r="S89" s="8">
         <v>0</v>
       </c>
-      <c r="T89" s="9">
+      <c r="T89" s="8">
         <v>1.076E-2</v>
       </c>
-      <c r="U89" s="9">
+      <c r="U89" s="8">
         <v>3.9167E-2</v>
       </c>
     </row>
@@ -18308,92 +18717,92 @@
       <c r="A90" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="9">
+      <c r="B90" s="8">
         <v>104.42608724279999</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C90" s="8">
         <v>102.300097561</v>
       </c>
-      <c r="D90" s="9">
+      <c r="D90" s="8">
         <v>101.6229182519</v>
       </c>
-      <c r="E90" s="9">
+      <c r="E90" s="8">
         <v>101.16914170850001</v>
       </c>
-      <c r="F90" s="9">
+      <c r="F90" s="8">
         <v>100.4393198164</v>
       </c>
-      <c r="G90" s="9">
+      <c r="G90" s="8">
         <v>100.5498055106</v>
       </c>
-      <c r="H90" s="9">
+      <c r="H90" s="8">
         <v>100.2918721817</v>
       </c>
-      <c r="I90" s="9">
+      <c r="I90" s="8">
         <v>100.2539945676</v>
       </c>
-      <c r="J90" s="9">
+      <c r="J90" s="8">
         <v>100.24155856580001</v>
       </c>
-      <c r="K90" s="9">
+      <c r="K90" s="8">
         <v>100.20272172759999</v>
       </c>
-      <c r="L90" s="9">
+      <c r="L90" s="8">
         <v>100.0694412829</v>
       </c>
-      <c r="M90" s="9">
+      <c r="M90" s="8">
         <v>100.06515740570001</v>
       </c>
-      <c r="N90" s="9">
+      <c r="N90" s="8">
         <v>100.050204283</v>
       </c>
-      <c r="O90" s="9">
+      <c r="O90" s="8">
         <v>99.832766072200002</v>
       </c>
-      <c r="P90" s="9">
+      <c r="P90" s="8">
         <v>99.707196536200001</v>
       </c>
-      <c r="Q90" s="9">
+      <c r="Q90" s="8">
         <v>99.714567207800002</v>
       </c>
-      <c r="R90" s="9">
+      <c r="R90" s="8">
         <v>99.617479040700005</v>
       </c>
-      <c r="S90" s="9">
+      <c r="S90" s="8">
         <v>99.552922159199994</v>
       </c>
-      <c r="T90" s="9">
+      <c r="T90" s="8">
         <v>99.351187823900005</v>
       </c>
-      <c r="U90" s="9">
+      <c r="U90" s="8">
         <v>99.231793069999995</v>
       </c>
     </row>
     <row r="91" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
-      <c r="H92" s="10"/>
-      <c r="I92" s="10"/>
-      <c r="J92" s="10"/>
-      <c r="K92" s="10"/>
-      <c r="L92" s="10"/>
-      <c r="M92" s="10"/>
-      <c r="N92" s="10"/>
-      <c r="O92" s="10"/>
-      <c r="P92" s="10"/>
-      <c r="Q92" s="10"/>
-      <c r="R92" s="10"/>
-      <c r="S92" s="10"/>
-      <c r="T92" s="10"/>
-      <c r="U92" s="10"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
+      <c r="K92" s="9"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
+      <c r="O92" s="9"/>
+      <c r="P92" s="9"/>
+      <c r="Q92" s="9"/>
+      <c r="R92" s="9"/>
+      <c r="S92" s="9"/>
+      <c r="T92" s="9"/>
+      <c r="U92" s="9"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
@@ -18464,64 +18873,64 @@
       <c r="A94" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="8">
         <v>4.6396259999999999E-4</v>
       </c>
-      <c r="D94" s="9">
+      <c r="D94" s="8">
         <v>2.5916099999999999E-4</v>
       </c>
-      <c r="E94" s="9">
+      <c r="E94" s="8">
         <v>9.529591E-4</v>
       </c>
-      <c r="F94" s="9">
+      <c r="F94" s="8">
         <v>2.0458697999999999E-3</v>
       </c>
-      <c r="G94" s="9">
+      <c r="G94" s="8">
         <v>2.7518272000000002E-3</v>
       </c>
-      <c r="H94" s="9">
+      <c r="H94" s="8">
         <v>1.1997938200000001E-2</v>
       </c>
-      <c r="I94" s="9">
+      <c r="I94" s="8">
         <v>2.5484085100000001E-2</v>
       </c>
-      <c r="J94" s="9">
+      <c r="J94" s="8">
         <v>1.9181013100000002E-2</v>
       </c>
-      <c r="K94" s="9">
+      <c r="K94" s="8">
         <v>2.5506019599999999E-2</v>
       </c>
-      <c r="L94" s="9">
+      <c r="L94" s="8">
         <v>4.0510177600000002E-2</v>
       </c>
-      <c r="M94" s="9">
+      <c r="M94" s="8">
         <v>7.1151971800000005E-2</v>
       </c>
-      <c r="N94" s="9">
+      <c r="N94" s="8">
         <v>9.2890977900000005E-2</v>
       </c>
-      <c r="O94" s="9">
-        <v>8.1436157199999998E-2</v>
-      </c>
-      <c r="P94" s="9">
-        <v>0.12597107890000001</v>
-      </c>
-      <c r="Q94" s="9">
-        <v>0.1040768623</v>
-      </c>
-      <c r="R94" s="9">
-        <v>9.1454982800000001E-2</v>
-      </c>
-      <c r="S94" s="9">
+      <c r="O94" s="8">
+        <v>0.11007239532</v>
+      </c>
+      <c r="P94" s="8">
+        <v>0.1192560196</v>
+      </c>
+      <c r="Q94" s="8">
+        <v>0.1805579662</v>
+      </c>
+      <c r="R94" s="8">
+        <v>0.18689107890000001</v>
+      </c>
+      <c r="S94" s="8">
         <v>0.21202397349999999</v>
       </c>
-      <c r="T94" s="9">
+      <c r="T94" s="8">
         <v>0.21988415720000001</v>
       </c>
-      <c r="U94" s="9">
+      <c r="U94" s="8">
         <v>0.31857085229999998</v>
       </c>
     </row>
@@ -18529,64 +18938,64 @@
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B95" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C95" s="8">
         <v>4.73E-4</v>
       </c>
-      <c r="D95" s="9">
+      <c r="D95" s="8">
         <v>2.6600000000000001E-4</v>
       </c>
-      <c r="E95" s="9">
+      <c r="E95" s="8">
         <v>9.5799999999999998E-4</v>
       </c>
-      <c r="F95" s="9">
+      <c r="F95" s="8">
         <v>2.039E-3</v>
       </c>
-      <c r="G95" s="9">
+      <c r="G95" s="8">
         <v>2.7360000000000002E-3</v>
       </c>
-      <c r="H95" s="9">
+      <c r="H95" s="8">
         <v>1.0503999999999999E-2</v>
       </c>
-      <c r="I95" s="9">
+      <c r="I95" s="8">
         <v>2.5267000000000001E-2</v>
       </c>
-      <c r="J95" s="9">
+      <c r="J95" s="8">
         <v>1.7767000000000002E-2</v>
       </c>
-      <c r="K95" s="9">
+      <c r="K95" s="8">
         <v>2.3609000000000002E-2</v>
       </c>
-      <c r="L95" s="9">
+      <c r="L95" s="8">
         <v>4.0133000000000002E-2</v>
       </c>
-      <c r="M95" s="9">
+      <c r="M95" s="8">
         <v>6.9967000000000001E-2</v>
       </c>
-      <c r="N95" s="9">
+      <c r="N95" s="8">
         <v>9.2026999999999998E-2</v>
       </c>
-      <c r="O95" s="9">
-        <v>8.0890000000000004E-2</v>
-      </c>
-      <c r="P95" s="9">
-        <v>0.129939</v>
-      </c>
-      <c r="Q95" s="9">
-        <v>0.102663</v>
-      </c>
-      <c r="R95" s="9">
-        <v>0.143457</v>
-      </c>
-      <c r="S95" s="9">
+      <c r="O95" s="8">
+        <v>0.11007239532</v>
+      </c>
+      <c r="P95" s="8">
+        <v>0.116401</v>
+      </c>
+      <c r="Q95" s="8">
+        <v>0.178812</v>
+      </c>
+      <c r="R95" s="8">
+        <v>0.18689107890000001</v>
+      </c>
+      <c r="S95" s="8">
         <v>0.215008</v>
       </c>
-      <c r="T95" s="9">
+      <c r="T95" s="8">
         <v>0.22231000000000001</v>
       </c>
-      <c r="U95" s="9">
+      <c r="U95" s="8">
         <v>0.31664199999999998</v>
       </c>
     </row>
@@ -18594,64 +19003,64 @@
       <c r="A96" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C96" s="8">
         <v>0</v>
       </c>
-      <c r="D96" s="9">
+      <c r="D96" s="8">
         <v>0</v>
       </c>
-      <c r="E96" s="9">
+      <c r="E96" s="8">
         <v>0</v>
       </c>
-      <c r="F96" s="9">
+      <c r="F96" s="8">
         <v>0</v>
       </c>
-      <c r="G96" s="9">
+      <c r="G96" s="8">
         <v>0</v>
       </c>
-      <c r="H96" s="9">
+      <c r="H96" s="8">
         <v>1.3940000000000001E-3</v>
       </c>
-      <c r="I96" s="9">
+      <c r="I96" s="8">
         <v>0</v>
       </c>
-      <c r="J96" s="9">
+      <c r="J96" s="8">
         <v>1.243E-3</v>
       </c>
-      <c r="K96" s="9">
+      <c r="K96" s="8">
         <v>1.6639999999999999E-3</v>
       </c>
-      <c r="L96" s="9">
+      <c r="L96" s="8">
         <v>0</v>
       </c>
-      <c r="M96" s="9">
+      <c r="M96" s="8">
         <v>5.3700000000000004E-4</v>
       </c>
-      <c r="N96" s="9">
+      <c r="N96" s="8">
         <v>0</v>
       </c>
-      <c r="O96" s="9">
+      <c r="O96" s="8">
         <v>0</v>
       </c>
-      <c r="P96" s="9">
+      <c r="P96" s="8">
         <v>0</v>
       </c>
-      <c r="Q96" s="9">
-        <v>1.418E-3</v>
-      </c>
-      <c r="R96" s="9">
+      <c r="Q96" s="8">
+        <v>1.3860000000000001E-3</v>
+      </c>
+      <c r="R96" s="8">
         <v>1.0269999999999999E-3</v>
       </c>
-      <c r="S96" s="9">
+      <c r="S96" s="8">
         <v>0</v>
       </c>
-      <c r="T96" s="9">
+      <c r="T96" s="8">
         <v>0</v>
       </c>
-      <c r="U96" s="9">
+      <c r="U96" s="8">
         <v>2.96E-3</v>
       </c>
     </row>
@@ -18659,92 +19068,92 @@
       <c r="A97" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B97" s="9">
+      <c r="B97" s="8">
         <v>240.01000492719999</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C97" s="8">
         <v>101.9478824255</v>
       </c>
-      <c r="D97" s="9">
+      <c r="D97" s="8">
         <v>102.63890193189999</v>
       </c>
-      <c r="E97" s="9">
+      <c r="E97" s="8">
         <v>100.5289775331</v>
       </c>
-      <c r="F97" s="9">
+      <c r="F97" s="8">
         <v>99.664209952199997</v>
       </c>
-      <c r="G97" s="9">
+      <c r="G97" s="8">
         <v>99.424846161800005</v>
       </c>
-      <c r="H97" s="9">
+      <c r="H97" s="8">
         <v>99.167038912600006</v>
       </c>
-      <c r="I97" s="9">
+      <c r="I97" s="8">
         <v>99.148154299799998</v>
       </c>
-      <c r="J97" s="9">
+      <c r="J97" s="8">
         <v>99.108425053800005</v>
       </c>
-      <c r="K97" s="9">
+      <c r="K97" s="8">
         <v>99.086413340799993</v>
       </c>
-      <c r="L97" s="9">
+      <c r="L97" s="8">
         <v>99.068931230299995</v>
       </c>
-      <c r="M97" s="9">
+      <c r="M97" s="8">
         <v>99.089312916500006</v>
       </c>
-      <c r="N97" s="9">
+      <c r="N97" s="8">
         <v>99.0699012117</v>
       </c>
-      <c r="O97" s="9">
+      <c r="O97" s="8">
         <v>99.329343076599997</v>
       </c>
-      <c r="P97" s="9">
+      <c r="P97" s="8">
         <v>103.1498667494</v>
       </c>
-      <c r="Q97" s="9">
+      <c r="Q97" s="8">
         <v>102.306260337</v>
       </c>
-      <c r="R97" s="9">
+      <c r="R97" s="8">
         <v>101.77803328660001</v>
       </c>
-      <c r="S97" s="9">
+      <c r="S97" s="8">
         <v>101.40740053410001</v>
       </c>
-      <c r="T97" s="9">
+      <c r="T97" s="8">
         <v>101.10323674529999</v>
       </c>
-      <c r="U97" s="9">
+      <c r="U97" s="8">
         <v>100.3236792421</v>
       </c>
     </row>
     <row r="98" spans="1:21" ht="190.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="99" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B99" s="10"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="10"/>
-      <c r="H99" s="10"/>
-      <c r="I99" s="10"/>
-      <c r="J99" s="10"/>
-      <c r="K99" s="10"/>
-      <c r="L99" s="10"/>
-      <c r="M99" s="10"/>
-      <c r="N99" s="10"/>
-      <c r="O99" s="10"/>
-      <c r="P99" s="10"/>
-      <c r="Q99" s="10"/>
-      <c r="R99" s="10"/>
-      <c r="S99" s="10"/>
-      <c r="T99" s="10"/>
-      <c r="U99" s="10"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="9"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="9"/>
+      <c r="L99" s="9"/>
+      <c r="M99" s="9"/>
+      <c r="N99" s="9"/>
+      <c r="O99" s="9"/>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="9"/>
+      <c r="R99" s="9"/>
+      <c r="S99" s="9"/>
+      <c r="T99" s="9"/>
+      <c r="U99" s="9"/>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
@@ -19579,7 +19988,7 @@
       <c r="A620" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A92:U92"/>
     <mergeCell ref="A99:U99"/>
     <mergeCell ref="A85:U85"/>
@@ -19590,6 +19999,7 @@
     <mergeCell ref="A64:U64"/>
     <mergeCell ref="A57:U57"/>
     <mergeCell ref="A39:U39"/>
+    <mergeCell ref="A50:U50"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizacion y llenado de datos de algorimto burbuja (#2)
* Actualizacion datos de tiempos

Actualizacion, modificacion y agregado de tiempos de algoritmo burbuja y burbuja opt 2

* AHORA SI?

. -.
</commit_message>
<xml_diff>
--- a/practica-1/Recopilacion de datos/Tabla de tiempos de algoritmos.xlsx
+++ b/practica-1/Recopilacion de datos/Tabla de tiempos de algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Analisis-y-Disegno-de-Algoritmos\practica-1\Recopilacion de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C975EFD0-0817-4E74-BF3B-97A407544438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639A49D2-053F-4500-99D9-67C5D6BE15ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6D9A99E9-C192-43DF-AC6A-A482D0DE89DC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="27">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Optimized Bubble Sort 1</t>
+  </si>
+  <si>
+    <t>Optimized Bubble Sort 2</t>
   </si>
 </sst>
 </file>
@@ -251,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -270,10 +276,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -289,6 +295,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -417,10 +426,10 @@
                   <c:v>Bubble Sort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Optimized Bubble Sort 1 *</c:v>
+                  <c:v>Optimized Bubble Sort 1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Optimized Bubble Sort 2 *</c:v>
+                  <c:v>Optimized Bubble Sort 2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Insertion Sort</c:v>
@@ -453,13 +462,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>912.37877988820003</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>675.10587501529994</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>688.3177878857</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>144.7588801384</c:v>
@@ -524,10 +533,10 @@
                   <c:v>Bubble Sort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Optimized Bubble Sort 1 *</c:v>
+                  <c:v>Optimized Bubble Sort 1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Optimized Bubble Sort 2 *</c:v>
+                  <c:v>Optimized Bubble Sort 2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Insertion Sort</c:v>
@@ -560,13 +569,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>913.34052999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>675.10241799999994</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>688.46476900000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>144.747165</c:v>
@@ -631,10 +640,10 @@
                   <c:v>Bubble Sort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Optimized Bubble Sort 1 *</c:v>
+                  <c:v>Optimized Bubble Sort 1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Optimized Bubble Sort 2 *</c:v>
+                  <c:v>Optimized Bubble Sort 2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Insertion Sort</c:v>
@@ -667,13 +676,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>2.1246999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.8530000000000001E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.31E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.1691999999999999E-2</c:v>
@@ -1141,16 +1150,16 @@
                   <c:v>9.2890977900000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.1436157199999998E-2</c:v>
+                  <c:v>0.11007239532</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.12597107890000001</c:v>
+                  <c:v>0.1192560196</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1040768623</c:v>
+                  <c:v>0.1805579662</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.1454982800000001E-2</c:v>
+                  <c:v>0.18689107890000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.21202397349999999</c:v>
@@ -1325,16 +1334,16 @@
                   <c:v>9.2026999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.0890000000000004E-2</c:v>
+                  <c:v>0.11007239532</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.129939</c:v>
+                  <c:v>0.116401</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.102663</c:v>
+                  <c:v>0.178812</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.143457</c:v>
+                  <c:v>0.18689107890000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.215008</c:v>
@@ -1515,7 +1524,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.418E-3</c:v>
+                  <c:v>1.3860000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.0269999999999999E-3</c:v>
@@ -2688,43 +2697,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.6160011E-3</c:v>
+                  <c:v>5.3410530000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4470767999999998E-3</c:v>
+                  <c:v>2.0967960399999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.47697926E-2</c:v>
+                  <c:v>3.8478851299999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7949094800000001E-2</c:v>
+                  <c:v>5.0436973599999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14117407800000001</c:v>
+                  <c:v>0.202974081</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.22094607350000001</c:v>
+                  <c:v>0.31697583200000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5079309939999996</c:v>
+                  <c:v>9.0544888973000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.752557992900002</c:v>
+                  <c:v>35.357850074799998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59.227169990500002</c:v>
+                  <c:v>78.645340919500001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>103.09226202959999</c:v>
+                  <c:v>141.74525403979999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>230.20986580850001</c:v>
+                  <c:v>405.49503517149998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>410.62090611460002</c:v>
+                  <c:v>578.68121910100001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>640.25535511969997</c:v>
+                  <c:v>912.37877988820003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2830,43 +2839,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.621E-3</c:v>
+                  <c:v>3.5400000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4450000000000002E-3</c:v>
+                  <c:v>2.0254000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4871000000000001E-2</c:v>
+                  <c:v>3.7157999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7952000000000001E-2</c:v>
+                  <c:v>4.87E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.141177</c:v>
+                  <c:v>0.195963</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.22095200000000001</c:v>
+                  <c:v>0.30601899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5078880000000003</c:v>
+                  <c:v>8.7281659999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.749362999999999</c:v>
+                  <c:v>35.217261000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59.227144000000003</c:v>
+                  <c:v>79.153655000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>103.092235</c:v>
+                  <c:v>141.09704400000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>230.207098</c:v>
+                  <c:v>405.50267200000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>410.57353000000001</c:v>
+                  <c:v>578.17917599999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>640.25501699999995</c:v>
+                  <c:v>913.34052999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2972,7 +2981,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.627E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2999,16 +3008,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>2.1440000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.5080000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.1770000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.0698000000000001E-2</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2.1246999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3400,10 +3409,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3442,37 +3451,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$41:$U$41</c:f>
+              <c:f>Hoja1!$B$41:$N$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.6160011E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4470767999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.47697926E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7949094800000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14117407800000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22094607350000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5079309939999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.752557992900002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.227169990500002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>103.09226202959999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>230.20986580850001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>494.42150998120002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>675.10587501529994</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3524,10 +3551,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3566,37 +3593,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$42:$U$42</c:f>
+              <c:f>Hoja1!$B$42:$N$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.621E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4450000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4871000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7952000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.141177</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22095200000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5078880000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.749362999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.227144000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>103.092235</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>230.207098</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>494.35421700000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>675.10241799999994</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3648,10 +3693,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3690,37 +3735,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$43:$U$43</c:f>
+              <c:f>Hoja1!$B$43:$N$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1770000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3744E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.8530000000000001E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4111,10 +4174,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4153,37 +4216,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$52:$U$52</c:f>
+              <c:f>Hoja1!$B$52:$N$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.8229485E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9580077999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6651153599999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0879020699999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14686989780000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25073909760000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7361590861999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.236689090700001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.848061084699999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>108.50353097919999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>366.31396508220001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>429.93227386469999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>688.3177878857</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4235,10 +4316,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4277,37 +4358,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$53:$U$53</c:f>
+              <c:f>Hoja1!$B$53:$N$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7650000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6177E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0009999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.135573</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24366199999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5335419999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.353097000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.916975000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>108.16159399999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>366.289851</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>430.24897600000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>688.46476900000005</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4359,10 +4458,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$22:$U$22</c:f>
+              <c:f>Hoja1!$B$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4401,37 +4500,55 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>600000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>700000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>900000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1500000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$54:$U$54</c:f>
+              <c:f>Hoja1!$B$54:$N$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.7780000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1549999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3189999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0630999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.4349999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.31E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8263,7 +8380,7 @@
                   <c:v>3.8465023000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.102408886</c:v>
+                  <c:v>9.0778112399999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>7.6631069199999999E-2</c:v>
@@ -8281,7 +8398,7 @@
                   <c:v>0.16359996800000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.29176807399999999</c:v>
+                  <c:v>0.22102785110000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.24379897119999999</c:v>
@@ -8447,7 +8564,7 @@
                   <c:v>3.8543000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.9287999999999997E-2</c:v>
+                  <c:v>9.0782000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>7.6680999999999999E-2</c:v>
@@ -8465,7 +8582,7 @@
                   <c:v>0.15345900000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28173199999999998</c:v>
+                  <c:v>0.22102785110000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.24270900000000001</c:v>
@@ -8631,7 +8748,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3192000000000001E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -15825,10 +15942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F19DE01-9E71-422D-A8E5-2FF9C6F5908D}">
-  <dimension ref="A1:U620"/>
+  <dimension ref="A1:AS620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="59" zoomScaleNormal="41" workbookViewId="0">
-      <selection activeCell="S66" sqref="S66"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="55" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15871,67 +15988,67 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9">
-        <v>675.10587501529994</v>
-      </c>
-      <c r="C3" s="9">
-        <v>675.10241799999994</v>
-      </c>
-      <c r="D3" s="9">
-        <v>2.8530000000000001E-3</v>
-      </c>
-      <c r="E3" s="9">
-        <v>99.999910530299999</v>
+      <c r="B3" s="8">
+        <v>912.37877988820003</v>
+      </c>
+      <c r="C3" s="8">
+        <v>913.34052999999994</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2.1246999999999999E-2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>100.1077400235</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="8">
+        <v>675.10587501529994</v>
+      </c>
+      <c r="C4" s="8">
+        <v>675.10241799999994</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2.8530000000000001E-3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>99.999910530299999</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="8">
+        <v>688.3177878857</v>
+      </c>
+      <c r="C5" s="8">
+        <v>688.46476900000005</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3.31E-3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>100.0218345533</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>144.7588801384</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>144.747165</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>1.1691999999999999E-2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>99.999984015899997</v>
       </c>
     </row>
@@ -15939,16 +16056,16 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>256.26689410210003</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>256.26093200000003</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>5.9420000000000002E-3</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>99.999992155800001</v>
       </c>
     </row>
@@ -15956,16 +16073,16 @@
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.53191399569999998</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>0.52315100000000003</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>8.7740000000000005E-3</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>100.0020688038</v>
       </c>
     </row>
@@ -15973,16 +16090,16 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>0</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>0</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>0</v>
       </c>
     </row>
@@ -15990,16 +16107,16 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>9.3252897299999998E-2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>9.3253000000000003E-2</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>6.4300000000000002E-4</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>100.0001101708</v>
       </c>
     </row>
@@ -16007,16 +16124,16 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>6.61728382E-2</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>6.4346E-2</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>1.823E-3</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>99.994199718199994</v>
       </c>
     </row>
@@ -16024,16 +16141,16 @@
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>0</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>0</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>0</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>0</v>
       </c>
     </row>
@@ -16134,55 +16251,55 @@
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="9">
-        <v>1.6160011E-3</v>
-      </c>
-      <c r="C23" s="9">
-        <v>6.4470767999999998E-3</v>
-      </c>
-      <c r="D23" s="9">
-        <v>1.47697926E-2</v>
-      </c>
-      <c r="E23" s="9">
-        <v>2.7949094800000001E-2</v>
-      </c>
-      <c r="F23" s="9">
-        <v>0.14117407800000001</v>
-      </c>
-      <c r="G23" s="9">
-        <v>0.22094607350000001</v>
-      </c>
-      <c r="H23" s="9">
-        <v>6.5079309939999996</v>
-      </c>
-      <c r="I23" s="9">
-        <v>26.752557992900002</v>
-      </c>
-      <c r="J23" s="9">
-        <v>59.227169990500002</v>
-      </c>
-      <c r="K23" s="9">
-        <v>103.09226202959999</v>
-      </c>
-      <c r="L23" s="9">
-        <v>230.20986580850001</v>
-      </c>
-      <c r="M23" s="9">
-        <v>410.62090611460002</v>
-      </c>
-      <c r="N23" s="9">
-        <v>640.25535511969997</v>
-      </c>
-      <c r="O23" s="9" t="s">
+      <c r="B23" s="8">
+        <v>5.3410530000000001E-3</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2.0967960399999999E-2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>3.8478851299999998E-2</v>
+      </c>
+      <c r="E23" s="8">
+        <v>5.0436973599999997E-2</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.202974081</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.31697583200000001</v>
+      </c>
+      <c r="H23" s="8">
+        <v>9.0544888973000006</v>
+      </c>
+      <c r="I23" s="8">
+        <v>35.357850074799998</v>
+      </c>
+      <c r="J23" s="8">
+        <v>78.645340919500001</v>
+      </c>
+      <c r="K23" s="8">
+        <v>141.74525403979999</v>
+      </c>
+      <c r="L23" s="8">
+        <v>405.49503517149998</v>
+      </c>
+      <c r="M23" s="8">
+        <v>578.68121910100001</v>
+      </c>
+      <c r="N23" s="8">
+        <v>912.37877988820003</v>
+      </c>
+      <c r="O23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="P23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Q23" s="9" t="s">
+      <c r="Q23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="9" t="s">
+      <c r="R23" s="15" t="s">
         <v>24</v>
       </c>
       <c r="S23" s="6" t="s">
@@ -16199,55 +16316,55 @@
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="9">
-        <v>1.621E-3</v>
-      </c>
-      <c r="C24" s="9">
-        <v>6.4450000000000002E-3</v>
-      </c>
-      <c r="D24" s="9">
-        <v>1.4871000000000001E-2</v>
-      </c>
-      <c r="E24" s="9">
-        <v>2.7952000000000001E-2</v>
-      </c>
-      <c r="F24" s="9">
-        <v>0.141177</v>
-      </c>
-      <c r="G24" s="9">
-        <v>0.22095200000000001</v>
-      </c>
-      <c r="H24" s="9">
-        <v>6.5078880000000003</v>
-      </c>
-      <c r="I24" s="9">
-        <v>26.749362999999999</v>
-      </c>
-      <c r="J24" s="9">
-        <v>59.227144000000003</v>
-      </c>
-      <c r="K24" s="9">
-        <v>103.092235</v>
-      </c>
-      <c r="L24" s="9">
-        <v>230.207098</v>
-      </c>
-      <c r="M24" s="9">
-        <v>410.57353000000001</v>
-      </c>
-      <c r="N24" s="9">
-        <v>640.25501699999995</v>
-      </c>
-      <c r="O24" s="9" t="s">
+      <c r="B24" s="8">
+        <v>3.5400000000000002E-3</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2.0254000000000001E-2</v>
+      </c>
+      <c r="D24" s="8">
+        <v>3.7157999999999997E-2</v>
+      </c>
+      <c r="E24" s="8">
+        <v>4.87E-2</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.195963</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.30601899999999999</v>
+      </c>
+      <c r="H24" s="8">
+        <v>8.7281659999999999</v>
+      </c>
+      <c r="I24" s="8">
+        <v>35.217261000000001</v>
+      </c>
+      <c r="J24" s="8">
+        <v>79.153655000000001</v>
+      </c>
+      <c r="K24" s="8">
+        <v>141.09704400000001</v>
+      </c>
+      <c r="L24" s="8">
+        <v>405.50267200000002</v>
+      </c>
+      <c r="M24" s="8">
+        <v>578.17917599999998</v>
+      </c>
+      <c r="N24" s="8">
+        <v>913.34052999999994</v>
+      </c>
+      <c r="O24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="P24" s="9" t="s">
+      <c r="P24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Q24" s="9" t="s">
+      <c r="Q24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="R24" s="9" t="s">
+      <c r="R24" s="15" t="s">
         <v>24</v>
       </c>
       <c r="S24" s="6" t="s">
@@ -16264,55 +16381,55 @@
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="8">
+        <v>1.627E-3</v>
+      </c>
+      <c r="C25" s="8">
         <v>0</v>
       </c>
-      <c r="C25" s="9">
+      <c r="D25" s="8">
         <v>0</v>
       </c>
-      <c r="D25" s="9">
+      <c r="E25" s="8">
         <v>0</v>
       </c>
-      <c r="E25" s="9">
+      <c r="F25" s="8">
         <v>0</v>
       </c>
-      <c r="F25" s="9">
+      <c r="G25" s="8">
         <v>0</v>
       </c>
-      <c r="G25" s="9">
+      <c r="H25" s="8">
         <v>0</v>
       </c>
-      <c r="H25" s="9">
+      <c r="I25" s="8">
         <v>0</v>
       </c>
-      <c r="I25" s="9">
+      <c r="J25" s="8">
         <v>0</v>
       </c>
-      <c r="J25" s="9">
+      <c r="K25" s="8">
+        <v>2.1440000000000001E-3</v>
+      </c>
+      <c r="L25" s="8">
+        <v>9.5080000000000008E-3</v>
+      </c>
+      <c r="M25" s="8">
         <v>0</v>
       </c>
-      <c r="K25" s="9">
-        <v>0</v>
-      </c>
-      <c r="L25" s="9">
-        <v>2.1770000000000001E-3</v>
-      </c>
-      <c r="M25" s="9">
-        <v>2.0698000000000001E-2</v>
-      </c>
-      <c r="N25" s="9">
-        <v>0</v>
-      </c>
-      <c r="O25" s="9" t="s">
+      <c r="N25" s="8">
+        <v>2.1246999999999999E-2</v>
+      </c>
+      <c r="O25" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="P25" s="9" t="s">
+      <c r="P25" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Q25" s="9" t="s">
+      <c r="Q25" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="R25" s="9" t="s">
+      <c r="R25" s="15" t="s">
         <v>24</v>
       </c>
       <c r="S25" s="6" t="s">
@@ -16329,55 +16446,55 @@
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="9">
-        <v>100.30933585130001</v>
-      </c>
-      <c r="C26" s="9">
-        <v>99.967786990099995</v>
-      </c>
-      <c r="D26" s="9">
-        <v>100.6852326656</v>
-      </c>
-      <c r="E26" s="9">
-        <v>100.01039471110001</v>
-      </c>
-      <c r="F26" s="9">
-        <v>100.0020697938</v>
-      </c>
-      <c r="G26" s="9">
-        <v>100.0026823142</v>
-      </c>
-      <c r="H26" s="9">
-        <v>99.999339359399997</v>
-      </c>
-      <c r="I26" s="9">
-        <v>99.988057243200004</v>
-      </c>
-      <c r="J26" s="9">
-        <v>99.9999561172</v>
-      </c>
-      <c r="K26" s="9">
-        <v>99.999973781099996</v>
-      </c>
-      <c r="L26" s="9">
-        <v>99.999743360899998</v>
-      </c>
-      <c r="M26" s="9">
-        <v>99.993502981899994</v>
-      </c>
-      <c r="N26" s="9">
-        <v>99.999947189899999</v>
-      </c>
-      <c r="O26" s="9" t="s">
+      <c r="B26" s="8">
+        <v>96.741222962199998</v>
+      </c>
+      <c r="C26" s="8">
+        <v>96.594993764400002</v>
+      </c>
+      <c r="D26" s="8">
+        <v>96.567331733900005</v>
+      </c>
+      <c r="E26" s="8">
+        <v>96.556150282700003</v>
+      </c>
+      <c r="F26" s="8">
+        <v>96.545824469999999</v>
+      </c>
+      <c r="G26" s="8">
+        <v>96.543322588099997</v>
+      </c>
+      <c r="H26" s="8">
+        <v>96.396009746900006</v>
+      </c>
+      <c r="I26" s="8">
+        <v>99.602382287200001</v>
+      </c>
+      <c r="J26" s="8">
+        <v>100.6463371823</v>
+      </c>
+      <c r="K26" s="8">
+        <v>99.544206228199997</v>
+      </c>
+      <c r="L26" s="8">
+        <v>100.0042281229</v>
+      </c>
+      <c r="M26" s="8">
+        <v>99.913243581399996</v>
+      </c>
+      <c r="N26" s="8">
+        <v>100.1077400235</v>
+      </c>
+      <c r="O26" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="P26" s="9" t="s">
+      <c r="P26" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Q26" s="9" t="s">
+      <c r="Q26" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="R26" s="9" t="s">
+      <c r="R26" s="15" t="s">
         <v>24</v>
       </c>
       <c r="S26" s="6" t="s">
@@ -16393,7 +16510,7 @@
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="P27" s="5"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>14</v>
       </c>
@@ -16418,7 +16535,7 @@
       <c r="T39" s="10"/>
       <c r="U39" s="10"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
@@ -16483,23 +16600,49 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
+      <c r="B41" s="8">
+        <v>1.6160011E-3</v>
+      </c>
+      <c r="C41" s="8">
+        <v>6.4470767999999998E-3</v>
+      </c>
+      <c r="D41" s="8">
+        <v>1.47697926E-2</v>
+      </c>
+      <c r="E41" s="8">
+        <v>2.7949094800000001E-2</v>
+      </c>
+      <c r="F41" s="8">
+        <v>0.14117407800000001</v>
+      </c>
+      <c r="G41" s="8">
+        <v>0.22094607350000001</v>
+      </c>
+      <c r="H41" s="8">
+        <v>6.5079309939999996</v>
+      </c>
+      <c r="I41" s="8">
+        <v>26.752557992900002</v>
+      </c>
+      <c r="J41" s="8">
+        <v>59.227169990500002</v>
+      </c>
+      <c r="K41" s="8">
+        <v>103.09226202959999</v>
+      </c>
+      <c r="L41" s="8">
+        <v>230.20986580850001</v>
+      </c>
+      <c r="M41" s="8">
+        <v>494.42150998120002</v>
+      </c>
+      <c r="N41" s="8">
+        <v>675.10587501529994</v>
+      </c>
       <c r="O41" s="1"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
@@ -16507,24 +16650,63 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="AG41" s="9"/>
+      <c r="AH41" s="9"/>
+      <c r="AI41" s="9"/>
+      <c r="AJ41" s="9"/>
+      <c r="AK41" s="9"/>
+      <c r="AL41" s="9"/>
+      <c r="AM41" s="9"/>
+      <c r="AN41" s="9"/>
+      <c r="AO41" s="9"/>
+      <c r="AP41" s="9"/>
+      <c r="AQ41" s="9"/>
+      <c r="AR41" s="9"/>
+      <c r="AS41" s="9"/>
+    </row>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="B42" s="8">
+        <v>1.621E-3</v>
+      </c>
+      <c r="C42" s="8">
+        <v>6.4450000000000002E-3</v>
+      </c>
+      <c r="D42" s="8">
+        <v>1.4871000000000001E-2</v>
+      </c>
+      <c r="E42" s="8">
+        <v>2.7952000000000001E-2</v>
+      </c>
+      <c r="F42" s="8">
+        <v>0.141177</v>
+      </c>
+      <c r="G42" s="8">
+        <v>0.22095200000000001</v>
+      </c>
+      <c r="H42" s="8">
+        <v>6.5078880000000003</v>
+      </c>
+      <c r="I42" s="8">
+        <v>26.749362999999999</v>
+      </c>
+      <c r="J42" s="8">
+        <v>59.227144000000003</v>
+      </c>
+      <c r="K42" s="8">
+        <v>103.092235</v>
+      </c>
+      <c r="L42" s="8">
+        <v>230.207098</v>
+      </c>
+      <c r="M42" s="8">
+        <v>494.35421700000001</v>
+      </c>
+      <c r="N42" s="8">
+        <v>675.10241799999994</v>
+      </c>
       <c r="O42" s="1"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
@@ -16532,24 +16714,63 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="AG42" s="9"/>
+      <c r="AH42" s="9"/>
+      <c r="AI42" s="9"/>
+      <c r="AJ42" s="9"/>
+      <c r="AK42" s="9"/>
+      <c r="AL42" s="9"/>
+      <c r="AM42" s="9"/>
+      <c r="AN42" s="9"/>
+      <c r="AO42" s="9"/>
+      <c r="AP42" s="9"/>
+      <c r="AQ42" s="9"/>
+      <c r="AR42" s="9"/>
+      <c r="AS42" s="9"/>
+    </row>
+    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
+      <c r="B43" s="8">
+        <v>0</v>
+      </c>
+      <c r="C43" s="8">
+        <v>0</v>
+      </c>
+      <c r="D43" s="8">
+        <v>0</v>
+      </c>
+      <c r="E43" s="8">
+        <v>0</v>
+      </c>
+      <c r="F43" s="8">
+        <v>0</v>
+      </c>
+      <c r="G43" s="8">
+        <v>0</v>
+      </c>
+      <c r="H43" s="8">
+        <v>0</v>
+      </c>
+      <c r="I43" s="8">
+        <v>0</v>
+      </c>
+      <c r="J43" s="8">
+        <v>0</v>
+      </c>
+      <c r="K43" s="8">
+        <v>0</v>
+      </c>
+      <c r="L43" s="8">
+        <v>2.1770000000000001E-3</v>
+      </c>
+      <c r="M43" s="8">
+        <v>5.3744E-2</v>
+      </c>
+      <c r="N43" s="8">
+        <v>2.8530000000000001E-3</v>
+      </c>
       <c r="O43" s="1"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
@@ -16557,24 +16778,63 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="AG43" s="9"/>
+      <c r="AH43" s="9"/>
+      <c r="AI43" s="9"/>
+      <c r="AJ43" s="9"/>
+      <c r="AK43" s="9"/>
+      <c r="AL43" s="9"/>
+      <c r="AM43" s="9"/>
+      <c r="AN43" s="9"/>
+      <c r="AO43" s="9"/>
+      <c r="AP43" s="9"/>
+      <c r="AQ43" s="9"/>
+      <c r="AR43" s="9"/>
+      <c r="AS43" s="9"/>
+    </row>
+    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
+      <c r="B44" s="8">
+        <v>100.30933585130001</v>
+      </c>
+      <c r="C44" s="8">
+        <v>99.967786990099995</v>
+      </c>
+      <c r="D44" s="8">
+        <v>100.6852326656</v>
+      </c>
+      <c r="E44" s="8">
+        <v>100.01039471110001</v>
+      </c>
+      <c r="F44" s="8">
+        <v>100.0020697938</v>
+      </c>
+      <c r="G44" s="8">
+        <v>100.0026823142</v>
+      </c>
+      <c r="H44" s="8">
+        <v>99.999339359399997</v>
+      </c>
+      <c r="I44" s="8">
+        <v>99.988057243200004</v>
+      </c>
+      <c r="J44" s="8">
+        <v>99.9999561172</v>
+      </c>
+      <c r="K44" s="8">
+        <v>99.999973781099996</v>
+      </c>
+      <c r="L44" s="8">
+        <v>99.999743360899998</v>
+      </c>
+      <c r="M44" s="8">
+        <v>99.997259629499993</v>
+      </c>
+      <c r="N44" s="8">
+        <v>99.999910530299999</v>
+      </c>
       <c r="O44" s="1"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
@@ -16585,29 +16845,29 @@
     </row>
     <row r="49" spans="1:21" ht="229.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
-      <c r="S50" s="8"/>
-      <c r="T50" s="8"/>
-      <c r="U50" s="8"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
+      <c r="T50" s="10"/>
+      <c r="U50" s="10"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
@@ -16678,19 +16938,45 @@
       <c r="A52" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+      <c r="B52" s="8">
+        <v>1.8229485E-3</v>
+      </c>
+      <c r="C52" s="8">
+        <v>6.9580077999999998E-3</v>
+      </c>
+      <c r="D52" s="8">
+        <v>1.6651153599999999E-2</v>
+      </c>
+      <c r="E52" s="8">
+        <v>3.0879020699999999E-2</v>
+      </c>
+      <c r="F52" s="8">
+        <v>0.14686989780000001</v>
+      </c>
+      <c r="G52" s="8">
+        <v>0.25073909760000002</v>
+      </c>
+      <c r="H52" s="8">
+        <v>6.7361590861999998</v>
+      </c>
+      <c r="I52" s="8">
+        <v>27.236689090700001</v>
+      </c>
+      <c r="J52" s="8">
+        <v>59.848061084699999</v>
+      </c>
+      <c r="K52" s="8">
+        <v>108.50353097919999</v>
+      </c>
+      <c r="L52" s="8">
+        <v>366.31396508220001</v>
+      </c>
+      <c r="M52" s="8">
+        <v>429.93227386469999</v>
+      </c>
+      <c r="N52" s="8">
+        <v>688.3177878857</v>
+      </c>
       <c r="O52" s="1"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="6"/>
@@ -16703,19 +16989,45 @@
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
+      <c r="B53" s="8">
+        <v>0</v>
+      </c>
+      <c r="C53" s="8">
+        <v>6.7650000000000002E-3</v>
+      </c>
+      <c r="D53" s="8">
+        <v>1.6177E-2</v>
+      </c>
+      <c r="E53" s="8">
+        <v>3.0009999999999998E-2</v>
+      </c>
+      <c r="F53" s="8">
+        <v>0.135573</v>
+      </c>
+      <c r="G53" s="8">
+        <v>0.24366199999999999</v>
+      </c>
+      <c r="H53" s="8">
+        <v>6.5335419999999997</v>
+      </c>
+      <c r="I53" s="8">
+        <v>27.353097000000002</v>
+      </c>
+      <c r="J53" s="8">
+        <v>59.916975000000001</v>
+      </c>
+      <c r="K53" s="8">
+        <v>108.16159399999999</v>
+      </c>
+      <c r="L53" s="8">
+        <v>366.289851</v>
+      </c>
+      <c r="M53" s="8">
+        <v>430.24897600000003</v>
+      </c>
+      <c r="N53" s="8">
+        <v>688.46476900000005</v>
+      </c>
       <c r="O53" s="1"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
@@ -16728,19 +17040,45 @@
       <c r="A54" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
+      <c r="B54" s="8">
+        <v>1.7780000000000001E-3</v>
+      </c>
+      <c r="C54" s="8">
+        <v>0</v>
+      </c>
+      <c r="D54" s="8">
+        <v>0</v>
+      </c>
+      <c r="E54" s="8">
+        <v>0</v>
+      </c>
+      <c r="F54" s="8">
+        <v>7.1549999999999999E-3</v>
+      </c>
+      <c r="G54" s="8">
+        <v>0</v>
+      </c>
+      <c r="H54" s="8">
+        <v>0</v>
+      </c>
+      <c r="I54" s="8">
+        <v>0</v>
+      </c>
+      <c r="J54" s="8">
+        <v>9.3189999999999992E-3</v>
+      </c>
+      <c r="K54" s="8">
+        <v>0</v>
+      </c>
+      <c r="L54" s="8">
+        <v>3.0630999999999999E-2</v>
+      </c>
+      <c r="M54" s="8">
+        <v>4.4349999999999997E-3</v>
+      </c>
+      <c r="N54" s="8">
+        <v>3.31E-3</v>
+      </c>
       <c r="O54" s="1"/>
       <c r="P54" s="6"/>
       <c r="Q54" s="6"/>
@@ -16753,19 +17091,45 @@
       <c r="A55" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
+      <c r="B55" s="8">
+        <v>97.534299136800001</v>
+      </c>
+      <c r="C55" s="8">
+        <v>97.226105263199997</v>
+      </c>
+      <c r="D55" s="8">
+        <v>97.152428132899999</v>
+      </c>
+      <c r="E55" s="8">
+        <v>97.185724574600002</v>
+      </c>
+      <c r="F55" s="8">
+        <v>97.179886482399993</v>
+      </c>
+      <c r="G55" s="8">
+        <v>97.177505357900003</v>
+      </c>
+      <c r="H55" s="8">
+        <v>96.992097668200003</v>
+      </c>
+      <c r="I55" s="8">
+        <v>100.42739375879999</v>
+      </c>
+      <c r="J55" s="8">
+        <v>100.1307192143</v>
+      </c>
+      <c r="K55" s="8">
+        <v>99.684860966200006</v>
+      </c>
+      <c r="L55" s="8">
+        <v>100.0017790525</v>
+      </c>
+      <c r="M55" s="8">
+        <v>100.07469481930001</v>
+      </c>
+      <c r="N55" s="8">
+        <v>100.0218345533</v>
+      </c>
       <c r="O55" s="1"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="6"/>
@@ -16869,61 +17233,61 @@
       <c r="A59" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B59" s="8">
         <v>5.7601929999999998E-4</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="8">
         <v>2.3689269999999998E-3</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="8">
         <v>4.9281120000000001E-3</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="8">
         <v>9.1629028000000008E-3</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F59" s="8">
         <v>3.5285949699999999E-2</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G59" s="8">
         <v>5.4972886999999998E-2</v>
       </c>
-      <c r="H59" s="9">
+      <c r="H59" s="8">
         <v>1.3339941501999999</v>
       </c>
-      <c r="I59" s="9">
+      <c r="I59" s="8">
         <v>5.2925069332000003</v>
       </c>
-      <c r="J59" s="9">
+      <c r="J59" s="8">
         <v>12.082659959800001</v>
       </c>
-      <c r="K59" s="9">
+      <c r="K59" s="8">
         <v>21.359937906300001</v>
       </c>
-      <c r="L59" s="9">
+      <c r="L59" s="8">
         <v>50.672094821899996</v>
       </c>
-      <c r="M59" s="9">
+      <c r="M59" s="8">
         <v>87.357614040399994</v>
       </c>
-      <c r="N59" s="9">
+      <c r="N59" s="8">
         <v>142.77942395209999</v>
       </c>
-      <c r="O59" s="9">
+      <c r="O59" s="8">
         <v>214.40739488599999</v>
       </c>
-      <c r="P59" s="9">
+      <c r="P59" s="8">
         <v>285.78975009919998</v>
       </c>
-      <c r="Q59" s="9">
+      <c r="Q59" s="8">
         <v>365.74295783039997</v>
       </c>
-      <c r="R59" s="9">
+      <c r="R59" s="8">
         <v>468.78817796710001</v>
       </c>
-      <c r="S59" s="9">
+      <c r="S59" s="8">
         <v>572.85432004929999</v>
       </c>
-      <c r="T59" s="9" t="s">
+      <c r="T59" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U59" s="6" t="s">
@@ -16934,61 +17298,61 @@
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B60" s="8">
         <v>5.8E-4</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="8">
         <v>2.3730000000000001E-3</v>
       </c>
-      <c r="D60" s="9">
+      <c r="D60" s="8">
         <v>4.9890000000000004E-3</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="8">
         <v>9.1660000000000005E-3</v>
       </c>
-      <c r="F60" s="9">
+      <c r="F60" s="8">
         <v>3.5290000000000002E-2</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G60" s="8">
         <v>5.4976999999999998E-2</v>
       </c>
-      <c r="H60" s="9">
+      <c r="H60" s="8">
         <v>1.333947</v>
       </c>
-      <c r="I60" s="9">
+      <c r="I60" s="8">
         <v>5.2924709999999999</v>
       </c>
-      <c r="J60" s="9">
+      <c r="J60" s="8">
         <v>12.082432000000001</v>
       </c>
-      <c r="K60" s="9">
+      <c r="K60" s="8">
         <v>21.359826999999999</v>
       </c>
-      <c r="L60" s="9">
+      <c r="L60" s="8">
         <v>50.672055999999998</v>
       </c>
-      <c r="M60" s="9">
+      <c r="M60" s="8">
         <v>87.356798999999995</v>
       </c>
-      <c r="N60" s="9">
+      <c r="N60" s="8">
         <v>142.77932799999999</v>
       </c>
-      <c r="O60" s="9">
+      <c r="O60" s="8">
         <v>214.39453800000001</v>
       </c>
-      <c r="P60" s="9">
+      <c r="P60" s="8">
         <v>285.78916199999998</v>
       </c>
-      <c r="Q60" s="9">
+      <c r="Q60" s="8">
         <v>365.728814</v>
       </c>
-      <c r="R60" s="9">
+      <c r="R60" s="8">
         <v>468.75717900000001</v>
       </c>
-      <c r="S60" s="9">
+      <c r="S60" s="8">
         <v>572.84291800000005</v>
       </c>
-      <c r="T60" s="9" t="s">
+      <c r="T60" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U60" s="6" t="s">
@@ -16999,61 +17363,61 @@
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B61" s="8">
         <v>0</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="8">
         <v>0</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="8">
         <v>0</v>
       </c>
-      <c r="E61" s="9">
+      <c r="E61" s="8">
         <v>0</v>
       </c>
-      <c r="F61" s="9">
+      <c r="F61" s="8">
         <v>0</v>
       </c>
-      <c r="G61" s="9">
+      <c r="G61" s="8">
         <v>0</v>
       </c>
-      <c r="H61" s="9">
+      <c r="H61" s="8">
         <v>0</v>
       </c>
-      <c r="I61" s="9">
+      <c r="I61" s="8">
         <v>0</v>
       </c>
-      <c r="J61" s="9">
+      <c r="J61" s="8">
         <v>0</v>
       </c>
-      <c r="K61" s="9">
+      <c r="K61" s="8">
         <v>0</v>
       </c>
-      <c r="L61" s="9">
+      <c r="L61" s="8">
         <v>0</v>
       </c>
-      <c r="M61" s="9">
+      <c r="M61" s="8">
         <v>7.5100000000000004E-4</v>
       </c>
-      <c r="N61" s="9">
+      <c r="N61" s="8">
         <v>0</v>
       </c>
-      <c r="O61" s="9">
+      <c r="O61" s="8">
         <v>1.7240000000000001E-3</v>
       </c>
-      <c r="P61" s="9">
+      <c r="P61" s="8">
         <v>0</v>
       </c>
-      <c r="Q61" s="9">
+      <c r="Q61" s="8">
         <v>1.4119E-2</v>
       </c>
-      <c r="R61" s="9">
+      <c r="R61" s="8">
         <v>3.0170000000000002E-3</v>
       </c>
-      <c r="S61" s="9">
+      <c r="S61" s="8">
         <v>1.1112E-2</v>
       </c>
-      <c r="T61" s="9" t="s">
+      <c r="T61" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U61" s="6" t="s">
@@ -17064,61 +17428,61 @@
       <c r="A62" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="8">
         <v>100.6910728477</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="8">
         <v>100.17193429949999</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="8">
         <v>101.23552325110001</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="8">
         <v>100.0338011657</v>
       </c>
-      <c r="F62" s="9">
+      <c r="F62" s="8">
         <v>100.0114784865</v>
       </c>
-      <c r="G62" s="9">
+      <c r="G62" s="8">
         <v>100.0074817988</v>
       </c>
-      <c r="H62" s="9">
+      <c r="H62" s="8">
         <v>99.996465489599998</v>
       </c>
-      <c r="I62" s="9">
+      <c r="I62" s="8">
         <v>99.999321054999996</v>
       </c>
-      <c r="J62" s="9">
+      <c r="J62" s="8">
         <v>99.998113331100001</v>
       </c>
-      <c r="K62" s="9">
+      <c r="K62" s="8">
         <v>99.999480774399998</v>
       </c>
-      <c r="L62" s="9">
+      <c r="L62" s="8">
         <v>99.999923386000006</v>
       </c>
-      <c r="M62" s="9">
+      <c r="M62" s="8">
         <v>99.999926691699997</v>
       </c>
-      <c r="N62" s="9">
+      <c r="N62" s="8">
         <v>99.999932797</v>
       </c>
-      <c r="O62" s="9">
+      <c r="O62" s="8">
         <v>99.994807601700003</v>
       </c>
-      <c r="P62" s="9">
+      <c r="P62" s="8">
         <v>99.999794219600005</v>
       </c>
-      <c r="Q62" s="9">
+      <c r="Q62" s="8">
         <v>99.999993211000003</v>
       </c>
-      <c r="R62" s="9">
+      <c r="R62" s="8">
         <v>99.994030999800003</v>
       </c>
-      <c r="S62" s="9">
+      <c r="S62" s="8">
         <v>99.999949367699998</v>
       </c>
-      <c r="T62" s="9" t="s">
+      <c r="T62" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U62" s="6" t="s">
@@ -17220,61 +17584,61 @@
       <c r="A66" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="8">
         <v>2.8278828000000002E-3</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="8">
         <v>8.5809231000000003E-3</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D66" s="8">
         <v>1.6232967399999999E-2</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E66" s="8">
         <v>3.3911228199999997E-2</v>
       </c>
-      <c r="F66" s="9">
+      <c r="F66" s="8">
         <v>7.7762126900000006E-2</v>
       </c>
-      <c r="G66" s="9">
+      <c r="G66" s="8">
         <v>0.1040349007</v>
       </c>
-      <c r="H66" s="9">
+      <c r="H66" s="8">
         <v>2.6799488068000001</v>
       </c>
-      <c r="I66" s="9">
+      <c r="I66" s="8">
         <v>11.709309101100001</v>
       </c>
-      <c r="J66" s="9">
+      <c r="J66" s="8">
         <v>26.516411066100002</v>
       </c>
-      <c r="K66" s="9">
+      <c r="K66" s="8">
         <v>47.511326074599999</v>
       </c>
-      <c r="L66" s="9">
+      <c r="L66" s="8">
         <v>110.3050270081</v>
       </c>
-      <c r="M66" s="9">
+      <c r="M66" s="8">
         <v>215.80932497980001</v>
       </c>
-      <c r="N66" s="9">
+      <c r="N66" s="8">
         <v>370.09260606769999</v>
       </c>
-      <c r="O66" s="9">
+      <c r="O66" s="8">
         <v>423.15952706339999</v>
       </c>
-      <c r="P66" s="9">
+      <c r="P66" s="8">
         <v>539.57744288440006</v>
       </c>
-      <c r="Q66" s="9">
+      <c r="Q66" s="8">
         <v>742.98159098630003</v>
       </c>
-      <c r="R66" s="9">
+      <c r="R66" s="8">
         <v>1081.3501529693999</v>
       </c>
-      <c r="S66" s="9">
+      <c r="S66" s="8">
         <v>1392.5612359047</v>
       </c>
-      <c r="T66" s="9" t="s">
+      <c r="T66" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U66" s="6" t="s">
@@ -17285,61 +17649,61 @@
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="8">
         <v>2.843E-3</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="8">
         <v>8.6009999999999993E-3</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D67" s="8">
         <v>1.6343E-2</v>
       </c>
-      <c r="E67" s="9">
+      <c r="E67" s="8">
         <v>3.3945999999999997E-2</v>
       </c>
-      <c r="F67" s="9">
+      <c r="F67" s="8">
         <v>7.7830999999999997E-2</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G67" s="8">
         <v>9.6765000000000004E-2</v>
       </c>
-      <c r="H67" s="9">
+      <c r="H67" s="8">
         <v>2.674061</v>
       </c>
-      <c r="I67" s="9">
+      <c r="I67" s="8">
         <v>11.629759</v>
       </c>
-      <c r="J67" s="9">
+      <c r="J67" s="8">
         <v>26.561571000000001</v>
       </c>
-      <c r="K67" s="9">
+      <c r="K67" s="8">
         <v>47.486843999999998</v>
       </c>
-      <c r="L67" s="9">
+      <c r="L67" s="8">
         <v>110.336692</v>
       </c>
-      <c r="M67" s="9">
+      <c r="M67" s="8">
         <v>215.82109399999999</v>
       </c>
-      <c r="N67" s="9">
+      <c r="N67" s="8">
         <v>370.01094000000001</v>
       </c>
-      <c r="O67" s="9">
+      <c r="O67" s="8">
         <v>423.06676299999998</v>
       </c>
-      <c r="P67" s="9">
+      <c r="P67" s="8">
         <v>539.63937899999996</v>
       </c>
-      <c r="Q67" s="9">
+      <c r="Q67" s="8">
         <v>742.91013499999997</v>
       </c>
-      <c r="R67" s="9">
+      <c r="R67" s="8">
         <v>1081.401175</v>
       </c>
-      <c r="S67" s="9">
+      <c r="S67" s="8">
         <v>1392.5149739999999</v>
       </c>
-      <c r="T67" s="9" t="s">
+      <c r="T67" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U67" s="6" t="s">
@@ -17350,61 +17714,61 @@
       <c r="A68" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B68" s="8">
         <v>0</v>
       </c>
-      <c r="C68" s="9">
+      <c r="C68" s="8">
         <v>0</v>
       </c>
-      <c r="D68" s="9">
+      <c r="D68" s="8">
         <v>0</v>
       </c>
-      <c r="E68" s="9">
+      <c r="E68" s="8">
         <v>0</v>
       </c>
-      <c r="F68" s="9">
+      <c r="F68" s="8">
         <v>0</v>
       </c>
-      <c r="G68" s="9">
+      <c r="G68" s="8">
         <v>7.2179999999999996E-3</v>
       </c>
-      <c r="H68" s="9">
+      <c r="H68" s="8">
         <v>0</v>
       </c>
-      <c r="I68" s="9">
+      <c r="I68" s="8">
         <v>0</v>
       </c>
-      <c r="J68" s="9">
+      <c r="J68" s="8">
         <v>0</v>
       </c>
-      <c r="K68" s="9">
+      <c r="K68" s="8">
         <v>0</v>
       </c>
-      <c r="L68" s="9">
+      <c r="L68" s="8">
         <v>4.744E-3</v>
       </c>
-      <c r="M68" s="9">
+      <c r="M68" s="8">
         <v>1.9910000000000001E-2</v>
       </c>
-      <c r="N68" s="9">
+      <c r="N68" s="8">
         <v>1.0709999999999999E-3</v>
       </c>
-      <c r="O68" s="9">
+      <c r="O68" s="8">
         <v>5.8708999999999997E-2</v>
       </c>
-      <c r="P68" s="9">
+      <c r="P68" s="8">
         <v>3.6080000000000001E-3</v>
       </c>
-      <c r="Q68" s="9">
+      <c r="Q68" s="8">
         <v>5.4938000000000001E-2</v>
       </c>
-      <c r="R68" s="9">
+      <c r="R68" s="8">
         <v>9.3329999999999993E-3</v>
       </c>
-      <c r="S68" s="9">
+      <c r="S68" s="8">
         <v>0</v>
       </c>
-      <c r="T68" s="9" t="s">
+      <c r="T68" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U68" s="6" t="s">
@@ -17415,61 +17779,61 @@
       <c r="A69" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="8">
         <v>100.53457779279999</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C69" s="8">
         <v>100.23397155959999</v>
       </c>
-      <c r="D69" s="9">
+      <c r="D69" s="8">
         <v>100.67783431540001</v>
       </c>
-      <c r="E69" s="9">
+      <c r="E69" s="8">
         <v>100.1025377786</v>
       </c>
-      <c r="F69" s="9">
+      <c r="F69" s="8">
         <v>100.0885689218</v>
       </c>
-      <c r="G69" s="9">
+      <c r="G69" s="8">
         <v>99.950112255600004</v>
       </c>
-      <c r="H69" s="9">
+      <c r="H69" s="8">
         <v>99.7803015211</v>
       </c>
-      <c r="I69" s="9">
+      <c r="I69" s="8">
         <v>99.320625150300003</v>
       </c>
-      <c r="J69" s="9">
+      <c r="J69" s="8">
         <v>100.1703093749</v>
       </c>
-      <c r="K69" s="9">
+      <c r="K69" s="8">
         <v>99.948471077099995</v>
       </c>
-      <c r="L69" s="9">
+      <c r="L69" s="8">
         <v>100.0330075545</v>
       </c>
-      <c r="M69" s="9">
+      <c r="M69" s="8">
         <v>100.0146791712</v>
       </c>
-      <c r="N69" s="9">
+      <c r="N69" s="8">
         <v>99.978222999799996</v>
       </c>
-      <c r="O69" s="9">
+      <c r="O69" s="8">
         <v>99.991952192699998</v>
       </c>
-      <c r="P69" s="9">
+      <c r="P69" s="8">
         <v>100.01214730460001</v>
       </c>
-      <c r="Q69" s="9">
+      <c r="Q69" s="8">
         <v>99.997776797399993</v>
       </c>
-      <c r="R69" s="9">
+      <c r="R69" s="8">
         <v>100.0055814512</v>
       </c>
-      <c r="S69" s="9">
+      <c r="S69" s="8">
         <v>99.996677926700002</v>
       </c>
-      <c r="T69" s="9" t="s">
+      <c r="T69" s="8" t="s">
         <v>24</v>
       </c>
       <c r="U69" s="6" t="s">
@@ -17571,64 +17935,64 @@
       <c r="A73" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" s="8">
         <v>2.2101400000000001E-4</v>
       </c>
-      <c r="C73" s="9">
+      <c r="C73" s="8">
         <v>5.6385989999999998E-4</v>
       </c>
-      <c r="D73" s="9">
+      <c r="D73" s="8">
         <v>7.7605250000000001E-4</v>
       </c>
-      <c r="E73" s="9">
+      <c r="E73" s="8">
         <v>1.3959408000000001E-3</v>
       </c>
-      <c r="F73" s="9">
+      <c r="F73" s="8">
         <v>1.20360851E-2</v>
       </c>
-      <c r="G73" s="9">
+      <c r="G73" s="8">
         <v>7.7548026999999997E-3</v>
       </c>
-      <c r="H73" s="9">
+      <c r="H73" s="8">
         <v>4.8887014399999998E-2</v>
       </c>
-      <c r="I73" s="9">
+      <c r="I73" s="8">
         <v>7.8410148599999993E-2</v>
       </c>
-      <c r="J73" s="9">
+      <c r="J73" s="8">
         <v>0.1100490093</v>
       </c>
-      <c r="K73" s="9">
+      <c r="K73" s="8">
         <v>0.19690799710000001</v>
       </c>
-      <c r="L73" s="9">
+      <c r="L73" s="8">
         <v>0.25797605509999999</v>
       </c>
-      <c r="M73" s="9">
+      <c r="M73" s="8">
         <v>0.44618296619999998</v>
       </c>
-      <c r="N73" s="9">
+      <c r="N73" s="8">
         <v>0.53032684330000002</v>
       </c>
-      <c r="O73" s="9">
+      <c r="O73" s="8">
         <v>0.66568994520000002</v>
       </c>
-      <c r="P73" s="9">
+      <c r="P73" s="8">
         <v>0.72402000430000002</v>
       </c>
-      <c r="Q73" s="9">
+      <c r="Q73" s="8">
         <v>1.0612299441999999</v>
       </c>
-      <c r="R73" s="9">
+      <c r="R73" s="8">
         <v>1.1045930386</v>
       </c>
-      <c r="S73" s="9">
+      <c r="S73" s="8">
         <v>1.2405769824999999</v>
       </c>
-      <c r="T73" s="9">
+      <c r="T73" s="8">
         <v>2.1346609592000001</v>
       </c>
-      <c r="U73" s="9">
+      <c r="U73" s="8">
         <v>3.3455178738</v>
       </c>
     </row>
@@ -17636,64 +18000,64 @@
       <c r="A74" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="9">
+      <c r="B74" s="8">
         <v>2.2499999999999999E-4</v>
       </c>
-      <c r="C74" s="9">
+      <c r="C74" s="8">
         <v>5.6599999999999999E-4</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="8">
         <v>7.85E-4</v>
       </c>
-      <c r="E74" s="9">
+      <c r="E74" s="8">
         <v>1.3910000000000001E-3</v>
       </c>
-      <c r="F74" s="9">
+      <c r="F74" s="8">
         <v>1.1957000000000001E-2</v>
       </c>
-      <c r="G74" s="9">
+      <c r="G74" s="8">
         <v>5.9369999999999996E-3</v>
       </c>
-      <c r="H74" s="9">
+      <c r="H74" s="8">
         <v>4.8524999999999999E-2</v>
       </c>
-      <c r="I74" s="9">
+      <c r="I74" s="8">
         <v>7.7803999999999998E-2</v>
       </c>
-      <c r="J74" s="9">
+      <c r="J74" s="8">
         <v>0.10614800000000001</v>
       </c>
-      <c r="K74" s="9">
+      <c r="K74" s="8">
         <v>0.19534899999999999</v>
       </c>
-      <c r="L74" s="9">
+      <c r="L74" s="8">
         <v>0.255888</v>
       </c>
-      <c r="M74" s="9">
+      <c r="M74" s="8">
         <v>0.43981100000000001</v>
       </c>
-      <c r="N74" s="9">
+      <c r="N74" s="8">
         <v>0.51870700000000003</v>
       </c>
-      <c r="O74" s="9">
+      <c r="O74" s="8">
         <v>0.65995000000000004</v>
       </c>
-      <c r="P74" s="9">
+      <c r="P74" s="8">
         <v>0.71764399999999995</v>
       </c>
-      <c r="Q74" s="9">
+      <c r="Q74" s="8">
         <v>1.0397400000000001</v>
       </c>
-      <c r="R74" s="9">
+      <c r="R74" s="8">
         <v>1.0990470000000001</v>
       </c>
-      <c r="S74" s="9">
+      <c r="S74" s="8">
         <v>1.2740940000000001</v>
       </c>
-      <c r="T74" s="9">
+      <c r="T74" s="8">
         <v>2.1465109999999998</v>
       </c>
-      <c r="U74" s="9">
+      <c r="U74" s="8">
         <v>3.338778</v>
       </c>
     </row>
@@ -17701,64 +18065,64 @@
       <c r="A75" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B75" s="8">
         <v>6.1300000000000005E-4</v>
       </c>
-      <c r="C75" s="9">
+      <c r="C75" s="8">
         <v>0</v>
       </c>
-      <c r="D75" s="9">
+      <c r="D75" s="8">
         <v>0</v>
       </c>
-      <c r="E75" s="9">
+      <c r="E75" s="8">
         <v>0</v>
       </c>
-      <c r="F75" s="9">
+      <c r="F75" s="8">
         <v>0</v>
       </c>
-      <c r="G75" s="9">
+      <c r="G75" s="8">
         <v>1.7669999999999999E-3</v>
       </c>
-      <c r="H75" s="9">
+      <c r="H75" s="8">
         <v>0</v>
       </c>
-      <c r="I75" s="9">
+      <c r="I75" s="8">
         <v>0</v>
       </c>
-      <c r="J75" s="9">
+      <c r="J75" s="8">
         <v>3.026E-3</v>
       </c>
-      <c r="K75" s="9">
+      <c r="K75" s="8">
         <v>0</v>
       </c>
-      <c r="L75" s="9">
+      <c r="L75" s="8">
         <v>0</v>
       </c>
-      <c r="M75" s="9">
+      <c r="M75" s="8">
         <v>2.6749999999999999E-3</v>
       </c>
-      <c r="N75" s="9">
+      <c r="N75" s="8">
         <v>7.1630000000000001E-3</v>
       </c>
-      <c r="O75" s="9">
+      <c r="O75" s="8">
         <v>0</v>
       </c>
-      <c r="P75" s="9">
+      <c r="P75" s="8">
         <v>0</v>
       </c>
-      <c r="Q75" s="9">
+      <c r="Q75" s="8">
         <v>1.1790999999999999E-2</v>
       </c>
-      <c r="R75" s="9">
+      <c r="R75" s="8">
         <v>0</v>
       </c>
-      <c r="S75" s="9">
+      <c r="S75" s="8">
         <v>1.3339999999999999E-3</v>
       </c>
-      <c r="T75" s="9">
+      <c r="T75" s="8">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="U75" s="9">
+      <c r="U75" s="8">
         <v>1.7364999999999998E-2</v>
       </c>
     </row>
@@ -17766,64 +18130,64 @@
       <c r="A76" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="9">
+      <c r="B76" s="8">
         <v>101.8034951456</v>
       </c>
-      <c r="C76" s="9">
+      <c r="C76" s="8">
         <v>100.3795375899</v>
       </c>
-      <c r="D76" s="9">
+      <c r="D76" s="8">
         <v>101.15295360979999</v>
       </c>
-      <c r="E76" s="9">
+      <c r="E76" s="8">
         <v>99.646060871100005</v>
       </c>
-      <c r="F76" s="9">
+      <c r="F76" s="8">
         <v>99.342933122000005</v>
       </c>
-      <c r="G76" s="9">
+      <c r="G76" s="8">
         <v>99.344887216399997</v>
       </c>
-      <c r="H76" s="9">
+      <c r="H76" s="8">
         <v>99.259487629700004</v>
       </c>
-      <c r="I76" s="9">
+      <c r="I76" s="8">
         <v>99.226951317800001</v>
       </c>
-      <c r="J76" s="9">
+      <c r="J76" s="8">
         <v>99.204891231199994</v>
       </c>
-      <c r="K76" s="9">
+      <c r="K76" s="8">
         <v>99.208261140199994</v>
       </c>
-      <c r="L76" s="9">
+      <c r="L76" s="8">
         <v>99.190601180399995</v>
       </c>
-      <c r="M76" s="9">
+      <c r="M76" s="8">
         <v>99.171423718100002</v>
       </c>
-      <c r="N76" s="9">
+      <c r="N76" s="8">
         <v>99.159604436699993</v>
       </c>
-      <c r="O76" s="9">
+      <c r="O76" s="8">
         <v>99.137744942300003</v>
       </c>
-      <c r="P76" s="9">
+      <c r="P76" s="8">
         <v>99.119360758699997</v>
       </c>
-      <c r="Q76" s="9">
+      <c r="Q76" s="8">
         <v>99.086065722000001</v>
       </c>
-      <c r="R76" s="9">
+      <c r="R76" s="8">
         <v>99.497911143300001</v>
       </c>
-      <c r="S76" s="9">
+      <c r="S76" s="8">
         <v>102.8092587557</v>
       </c>
-      <c r="T76" s="9">
+      <c r="T76" s="8">
         <v>101.1781749531</v>
       </c>
-      <c r="U76" s="9">
+      <c r="U76" s="8">
         <v>100.3175928701</v>
       </c>
     </row>
@@ -18113,64 +18477,64 @@
       <c r="A87" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87" s="8">
         <v>1.158714E-4</v>
       </c>
-      <c r="C87" s="9">
+      <c r="C87" s="8">
         <v>2.6392940000000001E-4</v>
       </c>
-      <c r="D87" s="9">
+      <c r="D87" s="8">
         <v>3.7097930000000001E-4</v>
       </c>
-      <c r="E87" s="9">
+      <c r="E87" s="8">
         <v>5.2189830000000002E-4</v>
       </c>
-      <c r="F87" s="9">
+      <c r="F87" s="8">
         <v>1.1429787E-3</v>
       </c>
-      <c r="G87" s="9">
+      <c r="G87" s="8">
         <v>1.445055E-3</v>
       </c>
-      <c r="H87" s="9">
+      <c r="H87" s="8">
         <v>1.8814086899999999E-2</v>
       </c>
-      <c r="I87" s="9">
+      <c r="I87" s="8">
         <v>1.9310951199999999E-2</v>
       </c>
-      <c r="J87" s="9">
+      <c r="J87" s="8">
         <v>3.8014173499999998E-2</v>
       </c>
-      <c r="K87" s="9">
+      <c r="K87" s="8">
         <v>3.8465023000000001E-2</v>
       </c>
-      <c r="L87" s="9">
-        <v>0.102408886</v>
-      </c>
-      <c r="M87" s="9">
+      <c r="L87" s="8">
+        <v>9.0778112399999999E-2</v>
+      </c>
+      <c r="M87" s="8">
         <v>7.6631069199999999E-2</v>
       </c>
-      <c r="N87" s="9">
+      <c r="N87" s="8">
         <v>9.5789909399999998E-2</v>
       </c>
-      <c r="O87" s="9">
+      <c r="O87" s="8">
         <v>0.14233803749999999</v>
       </c>
-      <c r="P87" s="9">
+      <c r="P87" s="8">
         <v>0.16123008729999999</v>
       </c>
-      <c r="Q87" s="9">
+      <c r="Q87" s="8">
         <v>0.16359996800000001</v>
       </c>
-      <c r="R87" s="9">
-        <v>0.29176807399999999</v>
-      </c>
-      <c r="S87" s="9">
+      <c r="R87" s="8">
+        <v>0.22102785110000001</v>
+      </c>
+      <c r="S87" s="8">
         <v>0.24379897119999999</v>
       </c>
-      <c r="T87" s="9">
+      <c r="T87" s="8">
         <v>0.31916880609999998</v>
       </c>
-      <c r="U87" s="9">
+      <c r="U87" s="8">
         <v>0.48191308980000003</v>
       </c>
     </row>
@@ -18178,64 +18542,64 @@
       <c r="A88" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="9">
+      <c r="B88" s="8">
         <v>1.21E-4</v>
       </c>
-      <c r="C88" s="9">
+      <c r="C88" s="8">
         <v>2.7E-4</v>
       </c>
-      <c r="D88" s="9">
+      <c r="D88" s="8">
         <v>3.77E-4</v>
       </c>
-      <c r="E88" s="9">
+      <c r="E88" s="8">
         <v>5.2800000000000004E-4</v>
       </c>
-      <c r="F88" s="9">
+      <c r="F88" s="8">
         <v>1.1479999999999999E-3</v>
       </c>
-      <c r="G88" s="9">
+      <c r="G88" s="8">
         <v>1.4530000000000001E-3</v>
       </c>
-      <c r="H88" s="9">
+      <c r="H88" s="8">
         <v>1.8869E-2</v>
       </c>
-      <c r="I88" s="9">
+      <c r="I88" s="8">
         <v>1.8360999999999999E-2</v>
       </c>
-      <c r="J88" s="9">
+      <c r="J88" s="8">
         <v>2.9499999999999998E-2</v>
       </c>
-      <c r="K88" s="9">
+      <c r="K88" s="8">
         <v>3.8543000000000001E-2</v>
       </c>
-      <c r="L88" s="9">
-        <v>7.9287999999999997E-2</v>
-      </c>
-      <c r="M88" s="9">
+      <c r="L88" s="8">
+        <v>9.0782000000000002E-2</v>
+      </c>
+      <c r="M88" s="8">
         <v>7.6680999999999999E-2</v>
       </c>
-      <c r="N88" s="9">
+      <c r="N88" s="8">
         <v>9.4359999999999999E-2</v>
       </c>
-      <c r="O88" s="9">
+      <c r="O88" s="8">
         <v>0.1421</v>
       </c>
-      <c r="P88" s="9">
+      <c r="P88" s="8">
         <v>0.15512500000000001</v>
       </c>
-      <c r="Q88" s="9">
+      <c r="Q88" s="8">
         <v>0.15345900000000001</v>
       </c>
-      <c r="R88" s="9">
-        <v>0.28173199999999998</v>
-      </c>
-      <c r="S88" s="9">
+      <c r="R88" s="8">
+        <v>0.22102785110000001</v>
+      </c>
+      <c r="S88" s="8">
         <v>0.24270900000000001</v>
       </c>
-      <c r="T88" s="9">
+      <c r="T88" s="8">
         <v>0.306338</v>
       </c>
-      <c r="U88" s="9">
+      <c r="U88" s="8">
         <v>0.43904399999999999</v>
       </c>
     </row>
@@ -18243,64 +18607,64 @@
       <c r="A89" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B89" s="8">
         <v>0</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C89" s="8">
         <v>0</v>
       </c>
-      <c r="D89" s="9">
+      <c r="D89" s="8">
         <v>0</v>
       </c>
-      <c r="E89" s="9">
+      <c r="E89" s="8">
         <v>0</v>
       </c>
-      <c r="F89" s="9">
+      <c r="F89" s="8">
         <v>0</v>
       </c>
-      <c r="G89" s="9">
+      <c r="G89" s="8">
         <v>0</v>
       </c>
-      <c r="H89" s="9">
+      <c r="H89" s="8">
         <v>0</v>
       </c>
-      <c r="I89" s="9">
+      <c r="I89" s="8">
         <v>9.990000000000001E-4</v>
       </c>
-      <c r="J89" s="9">
+      <c r="J89" s="8">
         <v>8.6060000000000008E-3</v>
       </c>
-      <c r="K89" s="9">
+      <c r="K89" s="8">
         <v>0</v>
       </c>
-      <c r="L89" s="9">
-        <v>2.3192000000000001E-2</v>
-      </c>
-      <c r="M89" s="9">
+      <c r="L89" s="8">
         <v>0</v>
       </c>
-      <c r="N89" s="9">
+      <c r="M89" s="8">
+        <v>0</v>
+      </c>
+      <c r="N89" s="8">
         <v>1.4779999999999999E-3</v>
       </c>
-      <c r="O89" s="9">
+      <c r="O89" s="8">
         <v>0</v>
       </c>
-      <c r="P89" s="9">
+      <c r="P89" s="8">
         <v>5.633E-3</v>
       </c>
-      <c r="Q89" s="9">
+      <c r="Q89" s="8">
         <v>9.6740000000000003E-3</v>
       </c>
-      <c r="R89" s="9">
+      <c r="R89" s="8">
         <v>8.9200000000000008E-3</v>
       </c>
-      <c r="S89" s="9">
+      <c r="S89" s="8">
         <v>0</v>
       </c>
-      <c r="T89" s="9">
+      <c r="T89" s="8">
         <v>1.076E-2</v>
       </c>
-      <c r="U89" s="9">
+      <c r="U89" s="8">
         <v>3.9167E-2</v>
       </c>
     </row>
@@ -18308,64 +18672,64 @@
       <c r="A90" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="9">
+      <c r="B90" s="8">
         <v>104.42608724279999</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C90" s="8">
         <v>102.300097561</v>
       </c>
-      <c r="D90" s="9">
+      <c r="D90" s="8">
         <v>101.6229182519</v>
       </c>
-      <c r="E90" s="9">
+      <c r="E90" s="8">
         <v>101.16914170850001</v>
       </c>
-      <c r="F90" s="9">
+      <c r="F90" s="8">
         <v>100.4393198164</v>
       </c>
-      <c r="G90" s="9">
+      <c r="G90" s="8">
         <v>100.5498055106</v>
       </c>
-      <c r="H90" s="9">
+      <c r="H90" s="8">
         <v>100.2918721817</v>
       </c>
-      <c r="I90" s="9">
+      <c r="I90" s="8">
         <v>100.2539945676</v>
       </c>
-      <c r="J90" s="9">
+      <c r="J90" s="8">
         <v>100.24155856580001</v>
       </c>
-      <c r="K90" s="9">
+      <c r="K90" s="8">
         <v>100.20272172759999</v>
       </c>
-      <c r="L90" s="9">
+      <c r="L90" s="8">
         <v>100.0694412829</v>
       </c>
-      <c r="M90" s="9">
+      <c r="M90" s="8">
         <v>100.06515740570001</v>
       </c>
-      <c r="N90" s="9">
+      <c r="N90" s="8">
         <v>100.050204283</v>
       </c>
-      <c r="O90" s="9">
+      <c r="O90" s="8">
         <v>99.832766072200002</v>
       </c>
-      <c r="P90" s="9">
+      <c r="P90" s="8">
         <v>99.707196536200001</v>
       </c>
-      <c r="Q90" s="9">
+      <c r="Q90" s="8">
         <v>99.714567207800002</v>
       </c>
-      <c r="R90" s="9">
+      <c r="R90" s="8">
         <v>99.617479040700005</v>
       </c>
-      <c r="S90" s="9">
+      <c r="S90" s="8">
         <v>99.552922159199994</v>
       </c>
-      <c r="T90" s="9">
+      <c r="T90" s="8">
         <v>99.351187823900005</v>
       </c>
-      <c r="U90" s="9">
+      <c r="U90" s="8">
         <v>99.231793069999995</v>
       </c>
     </row>
@@ -18464,64 +18828,64 @@
       <c r="A94" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="8">
         <v>4.6396259999999999E-4</v>
       </c>
-      <c r="D94" s="9">
+      <c r="D94" s="8">
         <v>2.5916099999999999E-4</v>
       </c>
-      <c r="E94" s="9">
+      <c r="E94" s="8">
         <v>9.529591E-4</v>
       </c>
-      <c r="F94" s="9">
+      <c r="F94" s="8">
         <v>2.0458697999999999E-3</v>
       </c>
-      <c r="G94" s="9">
+      <c r="G94" s="8">
         <v>2.7518272000000002E-3</v>
       </c>
-      <c r="H94" s="9">
+      <c r="H94" s="8">
         <v>1.1997938200000001E-2</v>
       </c>
-      <c r="I94" s="9">
+      <c r="I94" s="8">
         <v>2.5484085100000001E-2</v>
       </c>
-      <c r="J94" s="9">
+      <c r="J94" s="8">
         <v>1.9181013100000002E-2</v>
       </c>
-      <c r="K94" s="9">
+      <c r="K94" s="8">
         <v>2.5506019599999999E-2</v>
       </c>
-      <c r="L94" s="9">
+      <c r="L94" s="8">
         <v>4.0510177600000002E-2</v>
       </c>
-      <c r="M94" s="9">
+      <c r="M94" s="8">
         <v>7.1151971800000005E-2</v>
       </c>
-      <c r="N94" s="9">
+      <c r="N94" s="8">
         <v>9.2890977900000005E-2</v>
       </c>
-      <c r="O94" s="9">
-        <v>8.1436157199999998E-2</v>
-      </c>
-      <c r="P94" s="9">
-        <v>0.12597107890000001</v>
-      </c>
-      <c r="Q94" s="9">
-        <v>0.1040768623</v>
-      </c>
-      <c r="R94" s="9">
-        <v>9.1454982800000001E-2</v>
-      </c>
-      <c r="S94" s="9">
+      <c r="O94" s="8">
+        <v>0.11007239532</v>
+      </c>
+      <c r="P94" s="8">
+        <v>0.1192560196</v>
+      </c>
+      <c r="Q94" s="8">
+        <v>0.1805579662</v>
+      </c>
+      <c r="R94" s="8">
+        <v>0.18689107890000001</v>
+      </c>
+      <c r="S94" s="8">
         <v>0.21202397349999999</v>
       </c>
-      <c r="T94" s="9">
+      <c r="T94" s="8">
         <v>0.21988415720000001</v>
       </c>
-      <c r="U94" s="9">
+      <c r="U94" s="8">
         <v>0.31857085229999998</v>
       </c>
     </row>
@@ -18529,64 +18893,64 @@
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B95" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C95" s="8">
         <v>4.73E-4</v>
       </c>
-      <c r="D95" s="9">
+      <c r="D95" s="8">
         <v>2.6600000000000001E-4</v>
       </c>
-      <c r="E95" s="9">
+      <c r="E95" s="8">
         <v>9.5799999999999998E-4</v>
       </c>
-      <c r="F95" s="9">
+      <c r="F95" s="8">
         <v>2.039E-3</v>
       </c>
-      <c r="G95" s="9">
+      <c r="G95" s="8">
         <v>2.7360000000000002E-3</v>
       </c>
-      <c r="H95" s="9">
+      <c r="H95" s="8">
         <v>1.0503999999999999E-2</v>
       </c>
-      <c r="I95" s="9">
+      <c r="I95" s="8">
         <v>2.5267000000000001E-2</v>
       </c>
-      <c r="J95" s="9">
+      <c r="J95" s="8">
         <v>1.7767000000000002E-2</v>
       </c>
-      <c r="K95" s="9">
+      <c r="K95" s="8">
         <v>2.3609000000000002E-2</v>
       </c>
-      <c r="L95" s="9">
+      <c r="L95" s="8">
         <v>4.0133000000000002E-2</v>
       </c>
-      <c r="M95" s="9">
+      <c r="M95" s="8">
         <v>6.9967000000000001E-2</v>
       </c>
-      <c r="N95" s="9">
+      <c r="N95" s="8">
         <v>9.2026999999999998E-2</v>
       </c>
-      <c r="O95" s="9">
-        <v>8.0890000000000004E-2</v>
-      </c>
-      <c r="P95" s="9">
-        <v>0.129939</v>
-      </c>
-      <c r="Q95" s="9">
-        <v>0.102663</v>
-      </c>
-      <c r="R95" s="9">
-        <v>0.143457</v>
-      </c>
-      <c r="S95" s="9">
+      <c r="O95" s="8">
+        <v>0.11007239532</v>
+      </c>
+      <c r="P95" s="8">
+        <v>0.116401</v>
+      </c>
+      <c r="Q95" s="8">
+        <v>0.178812</v>
+      </c>
+      <c r="R95" s="8">
+        <v>0.18689107890000001</v>
+      </c>
+      <c r="S95" s="8">
         <v>0.215008</v>
       </c>
-      <c r="T95" s="9">
+      <c r="T95" s="8">
         <v>0.22231000000000001</v>
       </c>
-      <c r="U95" s="9">
+      <c r="U95" s="8">
         <v>0.31664199999999998</v>
       </c>
     </row>
@@ -18594,64 +18958,64 @@
       <c r="A96" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C96" s="8">
         <v>0</v>
       </c>
-      <c r="D96" s="9">
+      <c r="D96" s="8">
         <v>0</v>
       </c>
-      <c r="E96" s="9">
+      <c r="E96" s="8">
         <v>0</v>
       </c>
-      <c r="F96" s="9">
+      <c r="F96" s="8">
         <v>0</v>
       </c>
-      <c r="G96" s="9">
+      <c r="G96" s="8">
         <v>0</v>
       </c>
-      <c r="H96" s="9">
+      <c r="H96" s="8">
         <v>1.3940000000000001E-3</v>
       </c>
-      <c r="I96" s="9">
+      <c r="I96" s="8">
         <v>0</v>
       </c>
-      <c r="J96" s="9">
+      <c r="J96" s="8">
         <v>1.243E-3</v>
       </c>
-      <c r="K96" s="9">
+      <c r="K96" s="8">
         <v>1.6639999999999999E-3</v>
       </c>
-      <c r="L96" s="9">
+      <c r="L96" s="8">
         <v>0</v>
       </c>
-      <c r="M96" s="9">
+      <c r="M96" s="8">
         <v>5.3700000000000004E-4</v>
       </c>
-      <c r="N96" s="9">
+      <c r="N96" s="8">
         <v>0</v>
       </c>
-      <c r="O96" s="9">
+      <c r="O96" s="8">
         <v>0</v>
       </c>
-      <c r="P96" s="9">
+      <c r="P96" s="8">
         <v>0</v>
       </c>
-      <c r="Q96" s="9">
-        <v>1.418E-3</v>
-      </c>
-      <c r="R96" s="9">
+      <c r="Q96" s="8">
+        <v>1.3860000000000001E-3</v>
+      </c>
+      <c r="R96" s="8">
         <v>1.0269999999999999E-3</v>
       </c>
-      <c r="S96" s="9">
+      <c r="S96" s="8">
         <v>0</v>
       </c>
-      <c r="T96" s="9">
+      <c r="T96" s="8">
         <v>0</v>
       </c>
-      <c r="U96" s="9">
+      <c r="U96" s="8">
         <v>2.96E-3</v>
       </c>
     </row>
@@ -18659,64 +19023,64 @@
       <c r="A97" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B97" s="9">
+      <c r="B97" s="8">
         <v>240.01000492719999</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C97" s="8">
         <v>101.9478824255</v>
       </c>
-      <c r="D97" s="9">
+      <c r="D97" s="8">
         <v>102.63890193189999</v>
       </c>
-      <c r="E97" s="9">
+      <c r="E97" s="8">
         <v>100.5289775331</v>
       </c>
-      <c r="F97" s="9">
+      <c r="F97" s="8">
         <v>99.664209952199997</v>
       </c>
-      <c r="G97" s="9">
+      <c r="G97" s="8">
         <v>99.424846161800005</v>
       </c>
-      <c r="H97" s="9">
+      <c r="H97" s="8">
         <v>99.167038912600006</v>
       </c>
-      <c r="I97" s="9">
+      <c r="I97" s="8">
         <v>99.148154299799998</v>
       </c>
-      <c r="J97" s="9">
+      <c r="J97" s="8">
         <v>99.108425053800005</v>
       </c>
-      <c r="K97" s="9">
+      <c r="K97" s="8">
         <v>99.086413340799993</v>
       </c>
-      <c r="L97" s="9">
+      <c r="L97" s="8">
         <v>99.068931230299995</v>
       </c>
-      <c r="M97" s="9">
+      <c r="M97" s="8">
         <v>99.089312916500006</v>
       </c>
-      <c r="N97" s="9">
+      <c r="N97" s="8">
         <v>99.0699012117</v>
       </c>
-      <c r="O97" s="9">
+      <c r="O97" s="8">
         <v>99.329343076599997</v>
       </c>
-      <c r="P97" s="9">
+      <c r="P97" s="8">
         <v>103.1498667494</v>
       </c>
-      <c r="Q97" s="9">
+      <c r="Q97" s="8">
         <v>102.306260337</v>
       </c>
-      <c r="R97" s="9">
+      <c r="R97" s="8">
         <v>101.77803328660001</v>
       </c>
-      <c r="S97" s="9">
+      <c r="S97" s="8">
         <v>101.40740053410001</v>
       </c>
-      <c r="T97" s="9">
+      <c r="T97" s="8">
         <v>101.10323674529999</v>
       </c>
-      <c r="U97" s="9">
+      <c r="U97" s="8">
         <v>100.3236792421</v>
       </c>
     </row>
@@ -19579,7 +19943,7 @@
       <c r="A620" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A92:U92"/>
     <mergeCell ref="A99:U99"/>
     <mergeCell ref="A85:U85"/>
@@ -19590,6 +19954,7 @@
     <mergeCell ref="A64:U64"/>
     <mergeCell ref="A57:U57"/>
     <mergeCell ref="A39:U39"/>
+    <mergeCell ref="A50:U50"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tabla de datos completada
Agregado de tiempos de algoritmos restantes (heap y tree)
</commit_message>
<xml_diff>
--- a/practica-1/Recopilacion de datos/Tabla de tiempos de algoritmos.xlsx
+++ b/practica-1/Recopilacion de datos/Tabla de tiempos de algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Analisis-y-Disegno-de-Algoritmos\practica-1\Recopilacion de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639A49D2-053F-4500-99D9-67C5D6BE15ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380C6F14-4924-4809-B056-4AC3A6006D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6D9A99E9-C192-43DF-AC6A-A482D0DE89DC}"/>
   </bookViews>
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -253,11 +253,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -282,6 +295,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,8 +313,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,7 +499,7 @@
                   <c:v>0.53191399569999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.25702595709999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.3252897299999998E-2</c:v>
@@ -489,7 +508,7 @@
                   <c:v>6.61728382E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.1379179955</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -587,7 +606,7 @@
                   <c:v>0.52315100000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.24998000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.3253000000000003E-2</c:v>
@@ -596,7 +615,7 @@
                   <c:v>6.4346E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.13289400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,7 +722,7 @@
                   <c:v>1.823E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.2470000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2006,6 +2025,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.3399120000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.920628E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.880428E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8211560000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4481544E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0570755E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0325908700000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2229909900000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5598993299999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4061174400000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.7569961500000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1030540466</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1396610737</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17623305319999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.20921897889999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.24036788940000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.28201198579999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.32031297679999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.47633600230000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.63604521749999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2130,6 +2209,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.3799999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8200000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.69E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4170000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0052E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1631000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4598999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.2590999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5456999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.100207</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.135856</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17141999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.20350799999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.23380699999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.27412500000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.31157899999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.46196599999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.61857200000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2254,6 +2393,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0079999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7200000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.3849999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.5799999999999995E-4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7633,6 +7832,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.5187259999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0302999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3191179999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7605250000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.734972E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3238658999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.29802227E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9631853100000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2245855299999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.7632913599999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.126075983</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1911890507</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26713109019999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.34028887749999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.42636799809999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58567595480000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.61323094369999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70510792730000005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2633860110999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8008699417</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7757,6 +8016,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.5699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2400000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6199999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2650000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4689999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6924E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0789000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5757000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.122611</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.17460100000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25854199999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.32839699999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41468899999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.56961799999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.58808700000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.667022</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2138519999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7301839999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7881,6 +8200,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.01E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1619999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.895E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0022E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1348E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2669999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5699999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.3210000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8761E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5075E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1578E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -15944,8 +16323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F19DE01-9E71-422D-A8E5-2FF9C6F5908D}">
   <dimension ref="A1:AS620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="55" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="R97" zoomScale="94" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="T110" sqref="T110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15959,13 +16338,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -16091,16 +16470,16 @@
         <v>16</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>0.25702595709999998</v>
       </c>
       <c r="C9" s="8">
-        <v>0</v>
+        <v>0.24998000000000001</v>
       </c>
       <c r="D9" s="8">
         <v>0</v>
       </c>
-      <c r="E9" s="8">
-        <v>0</v>
+      <c r="E9" s="16">
+        <v>97.258659324999996</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -16142,45 +16521,48 @@
         <v>17</v>
       </c>
       <c r="B12" s="8">
-        <v>0</v>
+        <v>0.1379179955</v>
       </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>0.13289400000000001</v>
       </c>
       <c r="D12" s="8">
-        <v>0</v>
+        <v>1.2470000000000001E-3</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>97.261419410499997</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R13" s="5"/>
     </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D17" s="17"/>
+    </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
@@ -16290,16 +16672,16 @@
       <c r="N23" s="8">
         <v>912.37877988820003</v>
       </c>
-      <c r="O23" s="15" t="s">
+      <c r="O23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P23" s="15" t="s">
+      <c r="P23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q23" s="15" t="s">
+      <c r="Q23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="15" t="s">
+      <c r="R23" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S23" s="6" t="s">
@@ -16355,16 +16737,16 @@
       <c r="N24" s="8">
         <v>913.34052999999994</v>
       </c>
-      <c r="O24" s="15" t="s">
+      <c r="O24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P24" s="15" t="s">
+      <c r="P24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q24" s="15" t="s">
+      <c r="Q24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R24" s="15" t="s">
+      <c r="R24" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S24" s="6" t="s">
@@ -16420,16 +16802,16 @@
       <c r="N25" s="8">
         <v>2.1246999999999999E-2</v>
       </c>
-      <c r="O25" s="15" t="s">
+      <c r="O25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P25" s="15" t="s">
+      <c r="P25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q25" s="15" t="s">
+      <c r="Q25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R25" s="15" t="s">
+      <c r="R25" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S25" s="6" t="s">
@@ -16485,16 +16867,16 @@
       <c r="N26" s="8">
         <v>100.1077400235</v>
       </c>
-      <c r="O26" s="15" t="s">
+      <c r="O26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P26" s="15" t="s">
+      <c r="P26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q26" s="15" t="s">
+      <c r="Q26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R26" s="15" t="s">
+      <c r="R26" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S26" s="6" t="s">
@@ -16511,29 +16893,29 @@
       <c r="P27" s="5"/>
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
@@ -16845,29 +17227,29 @@
     </row>
     <row r="49" spans="1:21" ht="229.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="10"/>
-      <c r="T50" s="10"/>
-      <c r="U50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
@@ -17140,29 +17522,29 @@
     </row>
     <row r="56" spans="1:21" ht="206" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="57" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
-      <c r="Q57" s="14"/>
-      <c r="R57" s="14"/>
-      <c r="S57" s="14"/>
-      <c r="T57" s="14"/>
-      <c r="U57" s="14"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="15"/>
+      <c r="R57" s="15"/>
+      <c r="S57" s="15"/>
+      <c r="T57" s="15"/>
+      <c r="U57" s="15"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
@@ -17491,29 +17873,29 @@
     </row>
     <row r="63" spans="1:21" ht="221" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
-      <c r="P64" s="10"/>
-      <c r="Q64" s="10"/>
-      <c r="R64" s="10"/>
-      <c r="S64" s="10"/>
-      <c r="T64" s="10"/>
-      <c r="U64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
@@ -17842,29 +18224,29 @@
     </row>
     <row r="70" spans="1:21" ht="204.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="71" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
-      <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10"/>
-      <c r="O71" s="10"/>
-      <c r="P71" s="10"/>
-      <c r="Q71" s="10"/>
-      <c r="R71" s="10"/>
-      <c r="S71" s="10"/>
-      <c r="T71" s="10"/>
-      <c r="U71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="11"/>
+      <c r="T71" s="11"/>
+      <c r="U71" s="11"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
@@ -18193,29 +18575,29 @@
     </row>
     <row r="77" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="78" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
-      <c r="H78" s="10"/>
-      <c r="I78" s="10"/>
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="10"/>
-      <c r="N78" s="10"/>
-      <c r="O78" s="10"/>
-      <c r="P78" s="10"/>
-      <c r="Q78" s="10"/>
-      <c r="R78" s="10"/>
-      <c r="S78" s="10"/>
-      <c r="T78" s="10"/>
-      <c r="U78" s="10"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="11"/>
+      <c r="L78" s="11"/>
+      <c r="M78" s="11"/>
+      <c r="N78" s="11"/>
+      <c r="O78" s="11"/>
+      <c r="P78" s="11"/>
+      <c r="Q78" s="11"/>
+      <c r="R78" s="11"/>
+      <c r="S78" s="11"/>
+      <c r="T78" s="11"/>
+      <c r="U78" s="11"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
@@ -18286,127 +18668,287 @@
       <c r="A80" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="6"/>
-      <c r="Q80" s="6"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="1"/>
-      <c r="T80" s="1"/>
-      <c r="U80" s="1"/>
+      <c r="B80" s="8">
+        <v>1.5187259999999999E-4</v>
+      </c>
+      <c r="C80" s="8">
+        <v>3.0302999999999998E-4</v>
+      </c>
+      <c r="D80" s="8">
+        <v>5.3191179999999998E-4</v>
+      </c>
+      <c r="E80" s="8">
+        <v>7.7605250000000001E-4</v>
+      </c>
+      <c r="F80" s="8">
+        <v>1.734972E-3</v>
+      </c>
+      <c r="G80" s="8">
+        <v>2.3238658999999999E-3</v>
+      </c>
+      <c r="H80" s="8">
+        <v>1.29802227E-2</v>
+      </c>
+      <c r="I80" s="8">
+        <v>2.9631853100000001E-2</v>
+      </c>
+      <c r="J80" s="8">
+        <v>5.2245855299999998E-2</v>
+      </c>
+      <c r="K80" s="8">
+        <v>6.7632913599999997E-2</v>
+      </c>
+      <c r="L80" s="8">
+        <v>0.126075983</v>
+      </c>
+      <c r="M80" s="8">
+        <v>0.1911890507</v>
+      </c>
+      <c r="N80" s="8">
+        <v>0.26713109019999998</v>
+      </c>
+      <c r="O80" s="8">
+        <v>0.34028887749999998</v>
+      </c>
+      <c r="P80" s="8">
+        <v>0.42636799809999998</v>
+      </c>
+      <c r="Q80" s="8">
+        <v>0.58567595480000001</v>
+      </c>
+      <c r="R80" s="8">
+        <v>0.61323094369999998</v>
+      </c>
+      <c r="S80" s="8">
+        <v>0.70510792730000005</v>
+      </c>
+      <c r="T80" s="8">
+        <v>1.2633860110999999</v>
+      </c>
+      <c r="U80" s="8">
+        <v>1.8008699417</v>
+      </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
-      <c r="O81" s="1"/>
-      <c r="P81" s="6"/>
-      <c r="Q81" s="6"/>
-      <c r="R81" s="1"/>
-      <c r="S81" s="1"/>
-      <c r="T81" s="1"/>
-      <c r="U81" s="1"/>
+      <c r="B81" s="8">
+        <v>1.5699999999999999E-4</v>
+      </c>
+      <c r="C81" s="8">
+        <v>0</v>
+      </c>
+      <c r="D81" s="8">
+        <v>5.2400000000000005E-4</v>
+      </c>
+      <c r="E81" s="8">
+        <v>7.6199999999999998E-4</v>
+      </c>
+      <c r="F81" s="8">
+        <v>0</v>
+      </c>
+      <c r="G81" s="8">
+        <v>2.2650000000000001E-3</v>
+      </c>
+      <c r="H81" s="8">
+        <v>6.4689999999999999E-3</v>
+      </c>
+      <c r="I81" s="8">
+        <v>2.6924E-2</v>
+      </c>
+      <c r="J81" s="8">
+        <v>5.0789000000000001E-2</v>
+      </c>
+      <c r="K81" s="8">
+        <v>5.5757000000000001E-2</v>
+      </c>
+      <c r="L81" s="8">
+        <v>0.122611</v>
+      </c>
+      <c r="M81" s="8">
+        <v>0.17460100000000001</v>
+      </c>
+      <c r="N81" s="8">
+        <v>0.25854199999999999</v>
+      </c>
+      <c r="O81" s="8">
+        <v>0.32839699999999999</v>
+      </c>
+      <c r="P81" s="8">
+        <v>0.41468899999999997</v>
+      </c>
+      <c r="Q81" s="8">
+        <v>0.56961799999999996</v>
+      </c>
+      <c r="R81" s="8">
+        <v>0.58808700000000003</v>
+      </c>
+      <c r="S81" s="8">
+        <v>0.667022</v>
+      </c>
+      <c r="T81" s="8">
+        <v>1.2138519999999999</v>
+      </c>
+      <c r="U81" s="8">
+        <v>1.7301839999999999</v>
+      </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
-      <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
-      <c r="N82" s="1"/>
-      <c r="O82" s="1"/>
-      <c r="P82" s="6"/>
-      <c r="Q82" s="6"/>
-      <c r="R82" s="1"/>
-      <c r="S82" s="1"/>
-      <c r="T82" s="1"/>
-      <c r="U82" s="1"/>
+      <c r="B82" s="8">
+        <v>0</v>
+      </c>
+      <c r="C82" s="8">
+        <v>3.01E-4</v>
+      </c>
+      <c r="D82" s="8">
+        <v>0</v>
+      </c>
+      <c r="E82" s="8">
+        <v>0</v>
+      </c>
+      <c r="F82" s="8">
+        <v>1.6900000000000001E-3</v>
+      </c>
+      <c r="G82" s="8">
+        <v>0</v>
+      </c>
+      <c r="H82" s="8">
+        <v>6.1619999999999999E-3</v>
+      </c>
+      <c r="I82" s="8">
+        <v>1.895E-3</v>
+      </c>
+      <c r="J82" s="8">
+        <v>0</v>
+      </c>
+      <c r="K82" s="8">
+        <v>1.0022E-2</v>
+      </c>
+      <c r="L82" s="8">
+        <v>0</v>
+      </c>
+      <c r="M82" s="8">
+        <v>1.1348E-2</v>
+      </c>
+      <c r="N82" s="8">
+        <v>1.2669999999999999E-3</v>
+      </c>
+      <c r="O82" s="8">
+        <v>2.5699999999999998E-3</v>
+      </c>
+      <c r="P82" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="8">
+        <v>0</v>
+      </c>
+      <c r="R82" s="8">
+        <v>8.3210000000000003E-3</v>
+      </c>
+      <c r="S82" s="8">
+        <v>1.8761E-2</v>
+      </c>
+      <c r="T82" s="8">
+        <v>1.5075E-2</v>
+      </c>
+      <c r="U82" s="8">
+        <v>2.1578E-2</v>
+      </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
-      <c r="O83" s="1"/>
-      <c r="P83" s="6"/>
-      <c r="Q83" s="6"/>
-      <c r="R83" s="1"/>
-      <c r="S83" s="1"/>
-      <c r="T83" s="1"/>
-      <c r="U83" s="1"/>
+      <c r="B83" s="8">
+        <v>103.3760954474</v>
+      </c>
+      <c r="C83" s="8">
+        <v>99.330094728600002</v>
+      </c>
+      <c r="D83" s="8">
+        <v>98.512563693399997</v>
+      </c>
+      <c r="E83" s="8">
+        <v>98.189236497699994</v>
+      </c>
+      <c r="F83" s="8">
+        <v>97.407912051699995</v>
+      </c>
+      <c r="G83" s="8">
+        <v>97.466898122499998</v>
+      </c>
+      <c r="H83" s="8">
+        <v>97.309578502299999</v>
+      </c>
+      <c r="I83" s="8">
+        <v>97.256826629100004</v>
+      </c>
+      <c r="J83" s="8">
+        <v>97.211538939899995</v>
+      </c>
+      <c r="K83" s="8">
+        <v>97.258858903000004</v>
+      </c>
+      <c r="L83" s="8">
+        <v>97.251670806999996</v>
+      </c>
+      <c r="M83" s="8">
+        <v>97.259230768699993</v>
+      </c>
+      <c r="N83" s="8">
+        <v>97.258989898999999</v>
+      </c>
+      <c r="O83" s="8">
+        <v>97.260598831199999</v>
+      </c>
+      <c r="P83" s="8">
+        <v>97.260817375000002</v>
+      </c>
+      <c r="Q83" s="8">
+        <v>97.258218527400004</v>
+      </c>
+      <c r="R83" s="8">
+        <v>97.256670777400004</v>
+      </c>
+      <c r="S83" s="8">
+        <v>97.259295127200005</v>
+      </c>
+      <c r="T83" s="8">
+        <v>97.272487519999999</v>
+      </c>
+      <c r="U83" s="8">
+        <v>97.273098929900002</v>
+      </c>
     </row>
     <row r="84" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="85" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
-      <c r="I85" s="10"/>
-      <c r="J85" s="10"/>
-      <c r="K85" s="10"/>
-      <c r="L85" s="10"/>
-      <c r="M85" s="10"/>
-      <c r="N85" s="10"/>
-      <c r="O85" s="10"/>
-      <c r="P85" s="10"/>
-      <c r="Q85" s="10"/>
-      <c r="R85" s="10"/>
-      <c r="S85" s="10"/>
-      <c r="T85" s="10"/>
-      <c r="U85" s="10"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="11"/>
+      <c r="L85" s="11"/>
+      <c r="M85" s="11"/>
+      <c r="N85" s="11"/>
+      <c r="O85" s="11"/>
+      <c r="P85" s="11"/>
+      <c r="Q85" s="11"/>
+      <c r="R85" s="11"/>
+      <c r="S85" s="11"/>
+      <c r="T85" s="11"/>
+      <c r="U85" s="11"/>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
@@ -18735,29 +19277,29 @@
     </row>
     <row r="91" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
-      <c r="H92" s="10"/>
-      <c r="I92" s="10"/>
-      <c r="J92" s="10"/>
-      <c r="K92" s="10"/>
-      <c r="L92" s="10"/>
-      <c r="M92" s="10"/>
-      <c r="N92" s="10"/>
-      <c r="O92" s="10"/>
-      <c r="P92" s="10"/>
-      <c r="Q92" s="10"/>
-      <c r="R92" s="10"/>
-      <c r="S92" s="10"/>
-      <c r="T92" s="10"/>
-      <c r="U92" s="10"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="11"/>
+      <c r="L92" s="11"/>
+      <c r="M92" s="11"/>
+      <c r="N92" s="11"/>
+      <c r="O92" s="11"/>
+      <c r="P92" s="11"/>
+      <c r="Q92" s="11"/>
+      <c r="R92" s="11"/>
+      <c r="S92" s="11"/>
+      <c r="T92" s="11"/>
+      <c r="U92" s="11"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
@@ -19086,29 +19628,29 @@
     </row>
     <row r="98" spans="1:21" ht="190.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="99" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B99" s="10"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="10"/>
-      <c r="H99" s="10"/>
-      <c r="I99" s="10"/>
-      <c r="J99" s="10"/>
-      <c r="K99" s="10"/>
-      <c r="L99" s="10"/>
-      <c r="M99" s="10"/>
-      <c r="N99" s="10"/>
-      <c r="O99" s="10"/>
-      <c r="P99" s="10"/>
-      <c r="Q99" s="10"/>
-      <c r="R99" s="10"/>
-      <c r="S99" s="10"/>
-      <c r="T99" s="10"/>
-      <c r="U99" s="10"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="11"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="11"/>
+      <c r="K99" s="11"/>
+      <c r="L99" s="11"/>
+      <c r="M99" s="11"/>
+      <c r="N99" s="11"/>
+      <c r="O99" s="11"/>
+      <c r="P99" s="11"/>
+      <c r="Q99" s="11"/>
+      <c r="R99" s="11"/>
+      <c r="S99" s="11"/>
+      <c r="T99" s="11"/>
+      <c r="U99" s="11"/>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
@@ -19179,101 +19721,261 @@
       <c r="A101" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
-      <c r="P101" s="6"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="1"/>
-      <c r="S101" s="1"/>
-      <c r="T101" s="1"/>
-      <c r="U101" s="1"/>
+      <c r="B101" s="8">
+        <v>1.3399120000000001E-4</v>
+      </c>
+      <c r="C101" s="8">
+        <v>2.920628E-4</v>
+      </c>
+      <c r="D101" s="8">
+        <v>4.880428E-4</v>
+      </c>
+      <c r="E101" s="8">
+        <v>6.8211560000000005E-4</v>
+      </c>
+      <c r="F101" s="8">
+        <v>1.4481544E-3</v>
+      </c>
+      <c r="G101" s="8">
+        <v>2.0570755E-3</v>
+      </c>
+      <c r="H101" s="8">
+        <v>1.0325908700000001E-2</v>
+      </c>
+      <c r="I101" s="8">
+        <v>2.2229909900000001E-2</v>
+      </c>
+      <c r="J101" s="8">
+        <v>3.5598993299999999E-2</v>
+      </c>
+      <c r="K101" s="8">
+        <v>5.4061174400000002E-2</v>
+      </c>
+      <c r="L101" s="8">
+        <v>7.7569961500000006E-2</v>
+      </c>
+      <c r="M101" s="8">
+        <v>0.1030540466</v>
+      </c>
+      <c r="N101" s="8">
+        <v>0.1396610737</v>
+      </c>
+      <c r="O101" s="8">
+        <v>0.17623305319999999</v>
+      </c>
+      <c r="P101" s="8">
+        <v>0.20921897889999999</v>
+      </c>
+      <c r="Q101" s="8">
+        <v>0.24036788940000001</v>
+      </c>
+      <c r="R101" s="8">
+        <v>0.28201198579999998</v>
+      </c>
+      <c r="S101" s="8">
+        <v>0.32031297679999998</v>
+      </c>
+      <c r="T101" s="8">
+        <v>0.47633600230000001</v>
+      </c>
+      <c r="U101" s="8">
+        <v>0.63604521749999998</v>
+      </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="1"/>
-      <c r="P102" s="6"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="1"/>
-      <c r="S102" s="1"/>
-      <c r="T102" s="1"/>
-      <c r="U102" s="1"/>
+      <c r="B102" s="8">
+        <v>1.3799999999999999E-4</v>
+      </c>
+      <c r="C102" s="8">
+        <v>2.9E-4</v>
+      </c>
+      <c r="D102" s="8">
+        <v>4.8200000000000001E-4</v>
+      </c>
+      <c r="E102" s="8">
+        <v>6.69E-4</v>
+      </c>
+      <c r="F102" s="8">
+        <v>1.4170000000000001E-3</v>
+      </c>
+      <c r="G102" s="8">
+        <v>0</v>
+      </c>
+      <c r="H102" s="8">
+        <v>1.0052E-2</v>
+      </c>
+      <c r="I102" s="8">
+        <v>2.1631000000000001E-2</v>
+      </c>
+      <c r="J102" s="8">
+        <v>3.4598999999999998E-2</v>
+      </c>
+      <c r="K102" s="8">
+        <v>5.2590999999999999E-2</v>
+      </c>
+      <c r="L102" s="8">
+        <v>7.5456999999999996E-2</v>
+      </c>
+      <c r="M102" s="8">
+        <v>0.100207</v>
+      </c>
+      <c r="N102" s="8">
+        <v>0.135856</v>
+      </c>
+      <c r="O102" s="8">
+        <v>0.17141999999999999</v>
+      </c>
+      <c r="P102" s="8">
+        <v>0.20350799999999999</v>
+      </c>
+      <c r="Q102" s="8">
+        <v>0.23380699999999999</v>
+      </c>
+      <c r="R102" s="8">
+        <v>0.27412500000000001</v>
+      </c>
+      <c r="S102" s="8">
+        <v>0.31157899999999999</v>
+      </c>
+      <c r="T102" s="8">
+        <v>0.46196599999999999</v>
+      </c>
+      <c r="U102" s="8">
+        <v>0.61857200000000001</v>
+      </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
-      <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
-      <c r="O103" s="1"/>
-      <c r="P103" s="6"/>
-      <c r="Q103" s="6"/>
-      <c r="R103" s="1"/>
-      <c r="S103" s="1"/>
-      <c r="T103" s="1"/>
-      <c r="U103" s="1"/>
+      <c r="B103" s="8">
+        <v>0</v>
+      </c>
+      <c r="C103" s="8">
+        <v>0</v>
+      </c>
+      <c r="D103" s="8">
+        <v>0</v>
+      </c>
+      <c r="E103" s="8">
+        <v>0</v>
+      </c>
+      <c r="F103" s="8">
+        <v>0</v>
+      </c>
+      <c r="G103" s="8">
+        <v>2.0079999999999998E-3</v>
+      </c>
+      <c r="H103" s="8">
+        <v>0</v>
+      </c>
+      <c r="I103" s="8">
+        <v>0</v>
+      </c>
+      <c r="J103" s="8">
+        <v>0</v>
+      </c>
+      <c r="K103" s="8">
+        <v>0</v>
+      </c>
+      <c r="L103" s="8">
+        <v>0</v>
+      </c>
+      <c r="M103" s="8">
+        <v>0</v>
+      </c>
+      <c r="N103" s="8">
+        <v>0</v>
+      </c>
+      <c r="O103" s="8">
+        <v>0</v>
+      </c>
+      <c r="P103" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="8">
+        <v>0</v>
+      </c>
+      <c r="R103" s="8">
+        <v>1.7200000000000001E-4</v>
+      </c>
+      <c r="S103" s="8">
+        <v>0</v>
+      </c>
+      <c r="T103" s="8">
+        <v>1.3849999999999999E-3</v>
+      </c>
+      <c r="U103" s="8">
+        <v>6.5799999999999995E-4</v>
+      </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
-      <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
-      <c r="O104" s="1"/>
-      <c r="P104" s="6"/>
-      <c r="Q104" s="6"/>
-      <c r="R104" s="1"/>
-      <c r="S104" s="1"/>
-      <c r="T104" s="1"/>
-      <c r="U104" s="1"/>
+      <c r="B104" s="8">
+        <v>102.9918064057</v>
+      </c>
+      <c r="C104" s="8">
+        <v>99.293727346899999</v>
+      </c>
+      <c r="D104" s="8">
+        <v>98.761823546700001</v>
+      </c>
+      <c r="E104" s="8">
+        <v>98.077223907700002</v>
+      </c>
+      <c r="F104" s="8">
+        <v>97.848679091199998</v>
+      </c>
+      <c r="G104" s="8">
+        <v>97.614307278599995</v>
+      </c>
+      <c r="H104" s="8">
+        <v>97.347365061199994</v>
+      </c>
+      <c r="I104" s="8">
+        <v>97.305837497200002</v>
+      </c>
+      <c r="J104" s="8">
+        <v>97.190950617799999</v>
+      </c>
+      <c r="K104" s="8">
+        <v>97.280535598399993</v>
+      </c>
+      <c r="L104" s="8">
+        <v>97.276056986900002</v>
+      </c>
+      <c r="M104" s="8">
+        <v>97.237326699999997</v>
+      </c>
+      <c r="N104" s="8">
+        <v>97.275494463599998</v>
+      </c>
+      <c r="O104" s="8">
+        <v>97.2689270714</v>
+      </c>
+      <c r="P104" s="8">
+        <v>97.270334215199995</v>
+      </c>
+      <c r="Q104" s="8">
+        <v>97.270480087600006</v>
+      </c>
+      <c r="R104" s="8">
+        <v>97.264305714700001</v>
+      </c>
+      <c r="S104" s="8">
+        <v>97.273299095300004</v>
+      </c>
+      <c r="T104" s="8">
+        <v>97.273982590900005</v>
+      </c>
+      <c r="U104" s="8">
+        <v>97.356285834600001</v>
+      </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A415" s="5"/>

</xml_diff>

<commit_message>
Datos de excel completos (#6)
* Actualizacion datos de tiempos

Actualizacion, modificacion y agregado de tiempos de algoritmo burbuja y burbuja opt 2

* AHORA SI?

. -.

* Tabla de datos completada

Agregado de tiempos de algoritmos restantes (heap y tree)
</commit_message>
<xml_diff>
--- a/practica-1/Recopilacion de datos/Tabla de tiempos de algoritmos.xlsx
+++ b/practica-1/Recopilacion de datos/Tabla de tiempos de algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Analisis-y-Disegno-de-Algoritmos\practica-1\Recopilacion de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639A49D2-053F-4500-99D9-67C5D6BE15ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380C6F14-4924-4809-B056-4AC3A6006D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6D9A99E9-C192-43DF-AC6A-A482D0DE89DC}"/>
   </bookViews>
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -253,11 +253,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -282,6 +295,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,8 +313,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,7 +499,7 @@
                   <c:v>0.53191399569999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.25702595709999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.3252897299999998E-2</c:v>
@@ -489,7 +508,7 @@
                   <c:v>6.61728382E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.1379179955</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -587,7 +606,7 @@
                   <c:v>0.52315100000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.24998000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.3253000000000003E-2</c:v>
@@ -596,7 +615,7 @@
                   <c:v>6.4346E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.13289400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,7 +722,7 @@
                   <c:v>1.823E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.2470000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2006,6 +2025,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.3399120000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.920628E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.880428E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8211560000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4481544E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0570755E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0325908700000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2229909900000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5598993299999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4061174400000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.7569961500000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1030540466</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1396610737</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17623305319999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.20921897889999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.24036788940000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.28201198579999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.32031297679999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.47633600230000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.63604521749999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2130,6 +2209,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.3799999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8200000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.69E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4170000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0052E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1631000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4598999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.2590999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5456999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.100207</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.135856</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17141999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.20350799999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.23380699999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.27412500000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.31157899999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.46196599999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.61857200000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2254,6 +2393,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0079999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7200000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.3849999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.5799999999999995E-4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7633,6 +7832,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.5187259999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0302999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3191179999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7605250000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.734972E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3238658999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.29802227E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9631853100000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2245855299999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.7632913599999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.126075983</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1911890507</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26713109019999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.34028887749999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.42636799809999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58567595480000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.61323094369999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70510792730000005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2633860110999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8008699417</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7757,6 +8016,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.5699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2400000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6199999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2650000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4689999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6924E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0789000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5757000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.122611</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.17460100000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25854199999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.32839699999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41468899999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.56961799999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.58808700000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.667022</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2138519999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7301839999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7881,6 +8200,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.01E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1619999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.895E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0022E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1348E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2669999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5699999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.3210000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8761E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5075E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1578E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -15944,8 +16323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F19DE01-9E71-422D-A8E5-2FF9C6F5908D}">
   <dimension ref="A1:AS620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="55" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="R97" zoomScale="94" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="T110" sqref="T110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15959,13 +16338,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -16091,16 +16470,16 @@
         <v>16</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>0.25702595709999998</v>
       </c>
       <c r="C9" s="8">
-        <v>0</v>
+        <v>0.24998000000000001</v>
       </c>
       <c r="D9" s="8">
         <v>0</v>
       </c>
-      <c r="E9" s="8">
-        <v>0</v>
+      <c r="E9" s="16">
+        <v>97.258659324999996</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -16142,45 +16521,48 @@
         <v>17</v>
       </c>
       <c r="B12" s="8">
-        <v>0</v>
+        <v>0.1379179955</v>
       </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>0.13289400000000001</v>
       </c>
       <c r="D12" s="8">
-        <v>0</v>
+        <v>1.2470000000000001E-3</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>97.261419410499997</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R13" s="5"/>
     </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="D17" s="17"/>
+    </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
@@ -16290,16 +16672,16 @@
       <c r="N23" s="8">
         <v>912.37877988820003</v>
       </c>
-      <c r="O23" s="15" t="s">
+      <c r="O23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P23" s="15" t="s">
+      <c r="P23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q23" s="15" t="s">
+      <c r="Q23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="15" t="s">
+      <c r="R23" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S23" s="6" t="s">
@@ -16355,16 +16737,16 @@
       <c r="N24" s="8">
         <v>913.34052999999994</v>
       </c>
-      <c r="O24" s="15" t="s">
+      <c r="O24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P24" s="15" t="s">
+      <c r="P24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q24" s="15" t="s">
+      <c r="Q24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R24" s="15" t="s">
+      <c r="R24" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S24" s="6" t="s">
@@ -16420,16 +16802,16 @@
       <c r="N25" s="8">
         <v>2.1246999999999999E-2</v>
       </c>
-      <c r="O25" s="15" t="s">
+      <c r="O25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P25" s="15" t="s">
+      <c r="P25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q25" s="15" t="s">
+      <c r="Q25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R25" s="15" t="s">
+      <c r="R25" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S25" s="6" t="s">
@@ -16485,16 +16867,16 @@
       <c r="N26" s="8">
         <v>100.1077400235</v>
       </c>
-      <c r="O26" s="15" t="s">
+      <c r="O26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P26" s="15" t="s">
+      <c r="P26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q26" s="15" t="s">
+      <c r="Q26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R26" s="15" t="s">
+      <c r="R26" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S26" s="6" t="s">
@@ -16511,29 +16893,29 @@
       <c r="P27" s="5"/>
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
@@ -16845,29 +17227,29 @@
     </row>
     <row r="49" spans="1:21" ht="229.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="10"/>
-      <c r="T50" s="10"/>
-      <c r="U50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
@@ -17140,29 +17522,29 @@
     </row>
     <row r="56" spans="1:21" ht="206" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="57" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
-      <c r="Q57" s="14"/>
-      <c r="R57" s="14"/>
-      <c r="S57" s="14"/>
-      <c r="T57" s="14"/>
-      <c r="U57" s="14"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="15"/>
+      <c r="R57" s="15"/>
+      <c r="S57" s="15"/>
+      <c r="T57" s="15"/>
+      <c r="U57" s="15"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
@@ -17491,29 +17873,29 @@
     </row>
     <row r="63" spans="1:21" ht="221" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
-      <c r="P64" s="10"/>
-      <c r="Q64" s="10"/>
-      <c r="R64" s="10"/>
-      <c r="S64" s="10"/>
-      <c r="T64" s="10"/>
-      <c r="U64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
@@ -17842,29 +18224,29 @@
     </row>
     <row r="70" spans="1:21" ht="204.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="71" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
-      <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10"/>
-      <c r="O71" s="10"/>
-      <c r="P71" s="10"/>
-      <c r="Q71" s="10"/>
-      <c r="R71" s="10"/>
-      <c r="S71" s="10"/>
-      <c r="T71" s="10"/>
-      <c r="U71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="11"/>
+      <c r="T71" s="11"/>
+      <c r="U71" s="11"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
@@ -18193,29 +18575,29 @@
     </row>
     <row r="77" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="78" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
-      <c r="H78" s="10"/>
-      <c r="I78" s="10"/>
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="10"/>
-      <c r="N78" s="10"/>
-      <c r="O78" s="10"/>
-      <c r="P78" s="10"/>
-      <c r="Q78" s="10"/>
-      <c r="R78" s="10"/>
-      <c r="S78" s="10"/>
-      <c r="T78" s="10"/>
-      <c r="U78" s="10"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="11"/>
+      <c r="L78" s="11"/>
+      <c r="M78" s="11"/>
+      <c r="N78" s="11"/>
+      <c r="O78" s="11"/>
+      <c r="P78" s="11"/>
+      <c r="Q78" s="11"/>
+      <c r="R78" s="11"/>
+      <c r="S78" s="11"/>
+      <c r="T78" s="11"/>
+      <c r="U78" s="11"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
@@ -18286,127 +18668,287 @@
       <c r="A80" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="6"/>
-      <c r="Q80" s="6"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="1"/>
-      <c r="T80" s="1"/>
-      <c r="U80" s="1"/>
+      <c r="B80" s="8">
+        <v>1.5187259999999999E-4</v>
+      </c>
+      <c r="C80" s="8">
+        <v>3.0302999999999998E-4</v>
+      </c>
+      <c r="D80" s="8">
+        <v>5.3191179999999998E-4</v>
+      </c>
+      <c r="E80" s="8">
+        <v>7.7605250000000001E-4</v>
+      </c>
+      <c r="F80" s="8">
+        <v>1.734972E-3</v>
+      </c>
+      <c r="G80" s="8">
+        <v>2.3238658999999999E-3</v>
+      </c>
+      <c r="H80" s="8">
+        <v>1.29802227E-2</v>
+      </c>
+      <c r="I80" s="8">
+        <v>2.9631853100000001E-2</v>
+      </c>
+      <c r="J80" s="8">
+        <v>5.2245855299999998E-2</v>
+      </c>
+      <c r="K80" s="8">
+        <v>6.7632913599999997E-2</v>
+      </c>
+      <c r="L80" s="8">
+        <v>0.126075983</v>
+      </c>
+      <c r="M80" s="8">
+        <v>0.1911890507</v>
+      </c>
+      <c r="N80" s="8">
+        <v>0.26713109019999998</v>
+      </c>
+      <c r="O80" s="8">
+        <v>0.34028887749999998</v>
+      </c>
+      <c r="P80" s="8">
+        <v>0.42636799809999998</v>
+      </c>
+      <c r="Q80" s="8">
+        <v>0.58567595480000001</v>
+      </c>
+      <c r="R80" s="8">
+        <v>0.61323094369999998</v>
+      </c>
+      <c r="S80" s="8">
+        <v>0.70510792730000005</v>
+      </c>
+      <c r="T80" s="8">
+        <v>1.2633860110999999</v>
+      </c>
+      <c r="U80" s="8">
+        <v>1.8008699417</v>
+      </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
-      <c r="O81" s="1"/>
-      <c r="P81" s="6"/>
-      <c r="Q81" s="6"/>
-      <c r="R81" s="1"/>
-      <c r="S81" s="1"/>
-      <c r="T81" s="1"/>
-      <c r="U81" s="1"/>
+      <c r="B81" s="8">
+        <v>1.5699999999999999E-4</v>
+      </c>
+      <c r="C81" s="8">
+        <v>0</v>
+      </c>
+      <c r="D81" s="8">
+        <v>5.2400000000000005E-4</v>
+      </c>
+      <c r="E81" s="8">
+        <v>7.6199999999999998E-4</v>
+      </c>
+      <c r="F81" s="8">
+        <v>0</v>
+      </c>
+      <c r="G81" s="8">
+        <v>2.2650000000000001E-3</v>
+      </c>
+      <c r="H81" s="8">
+        <v>6.4689999999999999E-3</v>
+      </c>
+      <c r="I81" s="8">
+        <v>2.6924E-2</v>
+      </c>
+      <c r="J81" s="8">
+        <v>5.0789000000000001E-2</v>
+      </c>
+      <c r="K81" s="8">
+        <v>5.5757000000000001E-2</v>
+      </c>
+      <c r="L81" s="8">
+        <v>0.122611</v>
+      </c>
+      <c r="M81" s="8">
+        <v>0.17460100000000001</v>
+      </c>
+      <c r="N81" s="8">
+        <v>0.25854199999999999</v>
+      </c>
+      <c r="O81" s="8">
+        <v>0.32839699999999999</v>
+      </c>
+      <c r="P81" s="8">
+        <v>0.41468899999999997</v>
+      </c>
+      <c r="Q81" s="8">
+        <v>0.56961799999999996</v>
+      </c>
+      <c r="R81" s="8">
+        <v>0.58808700000000003</v>
+      </c>
+      <c r="S81" s="8">
+        <v>0.667022</v>
+      </c>
+      <c r="T81" s="8">
+        <v>1.2138519999999999</v>
+      </c>
+      <c r="U81" s="8">
+        <v>1.7301839999999999</v>
+      </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
-      <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
-      <c r="N82" s="1"/>
-      <c r="O82" s="1"/>
-      <c r="P82" s="6"/>
-      <c r="Q82" s="6"/>
-      <c r="R82" s="1"/>
-      <c r="S82" s="1"/>
-      <c r="T82" s="1"/>
-      <c r="U82" s="1"/>
+      <c r="B82" s="8">
+        <v>0</v>
+      </c>
+      <c r="C82" s="8">
+        <v>3.01E-4</v>
+      </c>
+      <c r="D82" s="8">
+        <v>0</v>
+      </c>
+      <c r="E82" s="8">
+        <v>0</v>
+      </c>
+      <c r="F82" s="8">
+        <v>1.6900000000000001E-3</v>
+      </c>
+      <c r="G82" s="8">
+        <v>0</v>
+      </c>
+      <c r="H82" s="8">
+        <v>6.1619999999999999E-3</v>
+      </c>
+      <c r="I82" s="8">
+        <v>1.895E-3</v>
+      </c>
+      <c r="J82" s="8">
+        <v>0</v>
+      </c>
+      <c r="K82" s="8">
+        <v>1.0022E-2</v>
+      </c>
+      <c r="L82" s="8">
+        <v>0</v>
+      </c>
+      <c r="M82" s="8">
+        <v>1.1348E-2</v>
+      </c>
+      <c r="N82" s="8">
+        <v>1.2669999999999999E-3</v>
+      </c>
+      <c r="O82" s="8">
+        <v>2.5699999999999998E-3</v>
+      </c>
+      <c r="P82" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="8">
+        <v>0</v>
+      </c>
+      <c r="R82" s="8">
+        <v>8.3210000000000003E-3</v>
+      </c>
+      <c r="S82" s="8">
+        <v>1.8761E-2</v>
+      </c>
+      <c r="T82" s="8">
+        <v>1.5075E-2</v>
+      </c>
+      <c r="U82" s="8">
+        <v>2.1578E-2</v>
+      </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
-      <c r="O83" s="1"/>
-      <c r="P83" s="6"/>
-      <c r="Q83" s="6"/>
-      <c r="R83" s="1"/>
-      <c r="S83" s="1"/>
-      <c r="T83" s="1"/>
-      <c r="U83" s="1"/>
+      <c r="B83" s="8">
+        <v>103.3760954474</v>
+      </c>
+      <c r="C83" s="8">
+        <v>99.330094728600002</v>
+      </c>
+      <c r="D83" s="8">
+        <v>98.512563693399997</v>
+      </c>
+      <c r="E83" s="8">
+        <v>98.189236497699994</v>
+      </c>
+      <c r="F83" s="8">
+        <v>97.407912051699995</v>
+      </c>
+      <c r="G83" s="8">
+        <v>97.466898122499998</v>
+      </c>
+      <c r="H83" s="8">
+        <v>97.309578502299999</v>
+      </c>
+      <c r="I83" s="8">
+        <v>97.256826629100004</v>
+      </c>
+      <c r="J83" s="8">
+        <v>97.211538939899995</v>
+      </c>
+      <c r="K83" s="8">
+        <v>97.258858903000004</v>
+      </c>
+      <c r="L83" s="8">
+        <v>97.251670806999996</v>
+      </c>
+      <c r="M83" s="8">
+        <v>97.259230768699993</v>
+      </c>
+      <c r="N83" s="8">
+        <v>97.258989898999999</v>
+      </c>
+      <c r="O83" s="8">
+        <v>97.260598831199999</v>
+      </c>
+      <c r="P83" s="8">
+        <v>97.260817375000002</v>
+      </c>
+      <c r="Q83" s="8">
+        <v>97.258218527400004</v>
+      </c>
+      <c r="R83" s="8">
+        <v>97.256670777400004</v>
+      </c>
+      <c r="S83" s="8">
+        <v>97.259295127200005</v>
+      </c>
+      <c r="T83" s="8">
+        <v>97.272487519999999</v>
+      </c>
+      <c r="U83" s="8">
+        <v>97.273098929900002</v>
+      </c>
     </row>
     <row r="84" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="85" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
-      <c r="I85" s="10"/>
-      <c r="J85" s="10"/>
-      <c r="K85" s="10"/>
-      <c r="L85" s="10"/>
-      <c r="M85" s="10"/>
-      <c r="N85" s="10"/>
-      <c r="O85" s="10"/>
-      <c r="P85" s="10"/>
-      <c r="Q85" s="10"/>
-      <c r="R85" s="10"/>
-      <c r="S85" s="10"/>
-      <c r="T85" s="10"/>
-      <c r="U85" s="10"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="11"/>
+      <c r="L85" s="11"/>
+      <c r="M85" s="11"/>
+      <c r="N85" s="11"/>
+      <c r="O85" s="11"/>
+      <c r="P85" s="11"/>
+      <c r="Q85" s="11"/>
+      <c r="R85" s="11"/>
+      <c r="S85" s="11"/>
+      <c r="T85" s="11"/>
+      <c r="U85" s="11"/>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
@@ -18735,29 +19277,29 @@
     </row>
     <row r="91" spans="1:21" ht="205" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
-      <c r="H92" s="10"/>
-      <c r="I92" s="10"/>
-      <c r="J92" s="10"/>
-      <c r="K92" s="10"/>
-      <c r="L92" s="10"/>
-      <c r="M92" s="10"/>
-      <c r="N92" s="10"/>
-      <c r="O92" s="10"/>
-      <c r="P92" s="10"/>
-      <c r="Q92" s="10"/>
-      <c r="R92" s="10"/>
-      <c r="S92" s="10"/>
-      <c r="T92" s="10"/>
-      <c r="U92" s="10"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="11"/>
+      <c r="L92" s="11"/>
+      <c r="M92" s="11"/>
+      <c r="N92" s="11"/>
+      <c r="O92" s="11"/>
+      <c r="P92" s="11"/>
+      <c r="Q92" s="11"/>
+      <c r="R92" s="11"/>
+      <c r="S92" s="11"/>
+      <c r="T92" s="11"/>
+      <c r="U92" s="11"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
@@ -19086,29 +19628,29 @@
     </row>
     <row r="98" spans="1:21" ht="190.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="99" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B99" s="10"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="10"/>
-      <c r="H99" s="10"/>
-      <c r="I99" s="10"/>
-      <c r="J99" s="10"/>
-      <c r="K99" s="10"/>
-      <c r="L99" s="10"/>
-      <c r="M99" s="10"/>
-      <c r="N99" s="10"/>
-      <c r="O99" s="10"/>
-      <c r="P99" s="10"/>
-      <c r="Q99" s="10"/>
-      <c r="R99" s="10"/>
-      <c r="S99" s="10"/>
-      <c r="T99" s="10"/>
-      <c r="U99" s="10"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="11"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="11"/>
+      <c r="K99" s="11"/>
+      <c r="L99" s="11"/>
+      <c r="M99" s="11"/>
+      <c r="N99" s="11"/>
+      <c r="O99" s="11"/>
+      <c r="P99" s="11"/>
+      <c r="Q99" s="11"/>
+      <c r="R99" s="11"/>
+      <c r="S99" s="11"/>
+      <c r="T99" s="11"/>
+      <c r="U99" s="11"/>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
@@ -19179,101 +19721,261 @@
       <c r="A101" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
-      <c r="P101" s="6"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="1"/>
-      <c r="S101" s="1"/>
-      <c r="T101" s="1"/>
-      <c r="U101" s="1"/>
+      <c r="B101" s="8">
+        <v>1.3399120000000001E-4</v>
+      </c>
+      <c r="C101" s="8">
+        <v>2.920628E-4</v>
+      </c>
+      <c r="D101" s="8">
+        <v>4.880428E-4</v>
+      </c>
+      <c r="E101" s="8">
+        <v>6.8211560000000005E-4</v>
+      </c>
+      <c r="F101" s="8">
+        <v>1.4481544E-3</v>
+      </c>
+      <c r="G101" s="8">
+        <v>2.0570755E-3</v>
+      </c>
+      <c r="H101" s="8">
+        <v>1.0325908700000001E-2</v>
+      </c>
+      <c r="I101" s="8">
+        <v>2.2229909900000001E-2</v>
+      </c>
+      <c r="J101" s="8">
+        <v>3.5598993299999999E-2</v>
+      </c>
+      <c r="K101" s="8">
+        <v>5.4061174400000002E-2</v>
+      </c>
+      <c r="L101" s="8">
+        <v>7.7569961500000006E-2</v>
+      </c>
+      <c r="M101" s="8">
+        <v>0.1030540466</v>
+      </c>
+      <c r="N101" s="8">
+        <v>0.1396610737</v>
+      </c>
+      <c r="O101" s="8">
+        <v>0.17623305319999999</v>
+      </c>
+      <c r="P101" s="8">
+        <v>0.20921897889999999</v>
+      </c>
+      <c r="Q101" s="8">
+        <v>0.24036788940000001</v>
+      </c>
+      <c r="R101" s="8">
+        <v>0.28201198579999998</v>
+      </c>
+      <c r="S101" s="8">
+        <v>0.32031297679999998</v>
+      </c>
+      <c r="T101" s="8">
+        <v>0.47633600230000001</v>
+      </c>
+      <c r="U101" s="8">
+        <v>0.63604521749999998</v>
+      </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="1"/>
-      <c r="P102" s="6"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="1"/>
-      <c r="S102" s="1"/>
-      <c r="T102" s="1"/>
-      <c r="U102" s="1"/>
+      <c r="B102" s="8">
+        <v>1.3799999999999999E-4</v>
+      </c>
+      <c r="C102" s="8">
+        <v>2.9E-4</v>
+      </c>
+      <c r="D102" s="8">
+        <v>4.8200000000000001E-4</v>
+      </c>
+      <c r="E102" s="8">
+        <v>6.69E-4</v>
+      </c>
+      <c r="F102" s="8">
+        <v>1.4170000000000001E-3</v>
+      </c>
+      <c r="G102" s="8">
+        <v>0</v>
+      </c>
+      <c r="H102" s="8">
+        <v>1.0052E-2</v>
+      </c>
+      <c r="I102" s="8">
+        <v>2.1631000000000001E-2</v>
+      </c>
+      <c r="J102" s="8">
+        <v>3.4598999999999998E-2</v>
+      </c>
+      <c r="K102" s="8">
+        <v>5.2590999999999999E-2</v>
+      </c>
+      <c r="L102" s="8">
+        <v>7.5456999999999996E-2</v>
+      </c>
+      <c r="M102" s="8">
+        <v>0.100207</v>
+      </c>
+      <c r="N102" s="8">
+        <v>0.135856</v>
+      </c>
+      <c r="O102" s="8">
+        <v>0.17141999999999999</v>
+      </c>
+      <c r="P102" s="8">
+        <v>0.20350799999999999</v>
+      </c>
+      <c r="Q102" s="8">
+        <v>0.23380699999999999</v>
+      </c>
+      <c r="R102" s="8">
+        <v>0.27412500000000001</v>
+      </c>
+      <c r="S102" s="8">
+        <v>0.31157899999999999</v>
+      </c>
+      <c r="T102" s="8">
+        <v>0.46196599999999999</v>
+      </c>
+      <c r="U102" s="8">
+        <v>0.61857200000000001</v>
+      </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
-      <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
-      <c r="O103" s="1"/>
-      <c r="P103" s="6"/>
-      <c r="Q103" s="6"/>
-      <c r="R103" s="1"/>
-      <c r="S103" s="1"/>
-      <c r="T103" s="1"/>
-      <c r="U103" s="1"/>
+      <c r="B103" s="8">
+        <v>0</v>
+      </c>
+      <c r="C103" s="8">
+        <v>0</v>
+      </c>
+      <c r="D103" s="8">
+        <v>0</v>
+      </c>
+      <c r="E103" s="8">
+        <v>0</v>
+      </c>
+      <c r="F103" s="8">
+        <v>0</v>
+      </c>
+      <c r="G103" s="8">
+        <v>2.0079999999999998E-3</v>
+      </c>
+      <c r="H103" s="8">
+        <v>0</v>
+      </c>
+      <c r="I103" s="8">
+        <v>0</v>
+      </c>
+      <c r="J103" s="8">
+        <v>0</v>
+      </c>
+      <c r="K103" s="8">
+        <v>0</v>
+      </c>
+      <c r="L103" s="8">
+        <v>0</v>
+      </c>
+      <c r="M103" s="8">
+        <v>0</v>
+      </c>
+      <c r="N103" s="8">
+        <v>0</v>
+      </c>
+      <c r="O103" s="8">
+        <v>0</v>
+      </c>
+      <c r="P103" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="8">
+        <v>0</v>
+      </c>
+      <c r="R103" s="8">
+        <v>1.7200000000000001E-4</v>
+      </c>
+      <c r="S103" s="8">
+        <v>0</v>
+      </c>
+      <c r="T103" s="8">
+        <v>1.3849999999999999E-3</v>
+      </c>
+      <c r="U103" s="8">
+        <v>6.5799999999999995E-4</v>
+      </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
-      <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
-      <c r="O104" s="1"/>
-      <c r="P104" s="6"/>
-      <c r="Q104" s="6"/>
-      <c r="R104" s="1"/>
-      <c r="S104" s="1"/>
-      <c r="T104" s="1"/>
-      <c r="U104" s="1"/>
+      <c r="B104" s="8">
+        <v>102.9918064057</v>
+      </c>
+      <c r="C104" s="8">
+        <v>99.293727346899999</v>
+      </c>
+      <c r="D104" s="8">
+        <v>98.761823546700001</v>
+      </c>
+      <c r="E104" s="8">
+        <v>98.077223907700002</v>
+      </c>
+      <c r="F104" s="8">
+        <v>97.848679091199998</v>
+      </c>
+      <c r="G104" s="8">
+        <v>97.614307278599995</v>
+      </c>
+      <c r="H104" s="8">
+        <v>97.347365061199994</v>
+      </c>
+      <c r="I104" s="8">
+        <v>97.305837497200002</v>
+      </c>
+      <c r="J104" s="8">
+        <v>97.190950617799999</v>
+      </c>
+      <c r="K104" s="8">
+        <v>97.280535598399993</v>
+      </c>
+      <c r="L104" s="8">
+        <v>97.276056986900002</v>
+      </c>
+      <c r="M104" s="8">
+        <v>97.237326699999997</v>
+      </c>
+      <c r="N104" s="8">
+        <v>97.275494463599998</v>
+      </c>
+      <c r="O104" s="8">
+        <v>97.2689270714</v>
+      </c>
+      <c r="P104" s="8">
+        <v>97.270334215199995</v>
+      </c>
+      <c r="Q104" s="8">
+        <v>97.270480087600006</v>
+      </c>
+      <c r="R104" s="8">
+        <v>97.264305714700001</v>
+      </c>
+      <c r="S104" s="8">
+        <v>97.273299095300004</v>
+      </c>
+      <c r="T104" s="8">
+        <v>97.273982590900005</v>
+      </c>
+      <c r="U104" s="8">
+        <v>97.356285834600001</v>
+      </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A415" s="5"/>

</xml_diff>